<commit_message>
Successfully impleneted voidy_analysis function, the isolated voidiness calculation.
</commit_message>
<xml_diff>
--- a/cel_obj_table.xlsx
+++ b/cel_obj_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H145"/>
+  <dimension ref="A1:G145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,20 +451,15 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>z</t>
+          <t>cmvd_Mpc</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>cmvd_Mpc</t>
+          <t>RAdeg_gal</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>RAdeg_gal</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>DEdeg_gal</t>
         </is>
@@ -486,15 +481,12 @@
         <v>29.78214263916016</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1000000014901161</v>
+        <v>422.9823619420345</v>
       </c>
       <c r="F2" t="n">
-        <v>422.9823619420345</v>
+        <v>114.4798012587622</v>
       </c>
       <c r="G2" t="n">
-        <v>114.4798012587622</v>
-      </c>
-      <c r="H2" t="n">
         <v>-32.5502715975377</v>
       </c>
     </row>
@@ -514,15 +506,12 @@
         <v>12.65117645263672</v>
       </c>
       <c r="E3" t="n">
-        <v>0.08900000154972076</v>
+        <v>377.3991422199498</v>
       </c>
       <c r="F3" t="n">
-        <v>377.3991422199498</v>
+        <v>117.760924150212</v>
       </c>
       <c r="G3" t="n">
-        <v>117.760924150212</v>
-      </c>
-      <c r="H3" t="n">
         <v>-50.08405705910805</v>
       </c>
     </row>
@@ -542,15 +531,12 @@
         <v>18.2844295501709</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4429999887943268</v>
+        <v>1722.784654514631</v>
       </c>
       <c r="F4" t="n">
-        <v>1722.784654514631</v>
+        <v>128.8249263315673</v>
       </c>
       <c r="G4" t="n">
-        <v>128.8249263315673</v>
-      </c>
-      <c r="H4" t="n">
         <v>-44.38437320754328</v>
       </c>
     </row>
@@ -570,15 +556,12 @@
         <v>22.75535202026367</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2649999856948853</v>
+        <v>1077.800369873403</v>
       </c>
       <c r="F5" t="n">
-        <v>1077.800369873403</v>
+        <v>129.1513327682703</v>
       </c>
       <c r="G5" t="n">
-        <v>129.1513327682703</v>
-      </c>
-      <c r="H5" t="n">
         <v>-39.86636396877911</v>
       </c>
     </row>
@@ -598,15 +581,12 @@
         <v>13.4044361114502</v>
       </c>
       <c r="E6" t="n">
-        <v>0.5830000042915344</v>
+        <v>2186.405655380971</v>
       </c>
       <c r="F6" t="n">
-        <v>2186.405655380971</v>
+        <v>131.6327174089689</v>
       </c>
       <c r="G6" t="n">
-        <v>131.6327174089689</v>
-      </c>
-      <c r="H6" t="n">
         <v>-49.07177578318304</v>
       </c>
     </row>
@@ -626,15 +606,12 @@
         <v>25.32852172851562</v>
       </c>
       <c r="E7" t="n">
-        <v>0.3580000102519989</v>
+        <v>1422.698307198181</v>
       </c>
       <c r="F7" t="n">
-        <v>1422.698307198181</v>
+        <v>129.8529186114632</v>
       </c>
       <c r="G7" t="n">
-        <v>129.8529186114632</v>
-      </c>
-      <c r="H7" t="n">
         <v>-37.21540373185186</v>
       </c>
     </row>
@@ -654,15 +631,12 @@
         <v>5.654636383056641</v>
       </c>
       <c r="E8" t="n">
-        <v>0.300000011920929</v>
+        <v>1209.647842624998</v>
       </c>
       <c r="F8" t="n">
-        <v>1209.647842624998</v>
+        <v>148.8556672614539</v>
       </c>
       <c r="G8" t="n">
-        <v>148.8556672614539</v>
-      </c>
-      <c r="H8" t="n">
         <v>-54.19102061088856</v>
       </c>
     </row>
@@ -682,15 +656,12 @@
         <v>1.785664200782776</v>
       </c>
       <c r="E9" t="n">
-        <v>0.07999999821186066</v>
+        <v>339.927766599597</v>
       </c>
       <c r="F9" t="n">
-        <v>339.927766599597</v>
+        <v>152.3914027711392</v>
       </c>
       <c r="G9" t="n">
-        <v>152.3914027711392</v>
-      </c>
-      <c r="H9" t="n">
         <v>-57.54007559780352</v>
       </c>
     </row>
@@ -710,15 +681,12 @@
         <v>8.389946937561035</v>
       </c>
       <c r="E10" t="n">
-        <v>0.6809999942779541</v>
+        <v>2489.225587653121</v>
       </c>
       <c r="F10" t="n">
-        <v>2489.225587653121</v>
+        <v>148.2359504042424</v>
       </c>
       <c r="G10" t="n">
-        <v>148.2359504042424</v>
-      </c>
-      <c r="H10" t="n">
         <v>-51.38123321650065</v>
       </c>
     </row>
@@ -738,15 +706,12 @@
         <v>2.002652168273926</v>
       </c>
       <c r="E11" t="n">
-        <v>0.4569999873638153</v>
+        <v>1770.843252129352</v>
       </c>
       <c r="F11" t="n">
-        <v>1770.843252129352</v>
+        <v>165.1466930350609</v>
       </c>
       <c r="G11" t="n">
-        <v>165.1466930350609</v>
-      </c>
-      <c r="H11" t="n">
         <v>-52.82668089433401</v>
       </c>
     </row>
@@ -766,15 +731,12 @@
         <v>-0.04313698038458824</v>
       </c>
       <c r="E12" t="n">
-        <v>0.003000000026077032</v>
+        <v>12.96591135664807</v>
       </c>
       <c r="F12" t="n">
-        <v>12.96591135664807</v>
+        <v>172.1438214764061</v>
       </c>
       <c r="G12" t="n">
-        <v>172.1438214764061</v>
-      </c>
-      <c r="H12" t="n">
         <v>-51.95162955648622</v>
       </c>
     </row>
@@ -794,15 +756,12 @@
         <v>3.57359504699707</v>
       </c>
       <c r="E13" t="n">
-        <v>0.4000000059604645</v>
+        <v>1572.767471022466</v>
       </c>
       <c r="F13" t="n">
-        <v>1572.767471022466</v>
+        <v>172.2738268268965</v>
       </c>
       <c r="G13" t="n">
-        <v>172.2738268268965</v>
-      </c>
-      <c r="H13" t="n">
         <v>-46.9728540251021</v>
       </c>
     </row>
@@ -822,15 +781,12 @@
         <v>15.28416442871094</v>
       </c>
       <c r="E14" t="n">
-        <v>0.1790000051259995</v>
+        <v>743.3176422661688</v>
       </c>
       <c r="F14" t="n">
-        <v>743.3176422661688</v>
+        <v>198.9723667223909</v>
       </c>
       <c r="G14" t="n">
-        <v>198.9723667223909</v>
-      </c>
-      <c r="H14" t="n">
         <v>6.322407808255858</v>
       </c>
     </row>
@@ -850,15 +806,12 @@
         <v>33.12022399902344</v>
       </c>
       <c r="E15" t="n">
-        <v>0.1120000034570694</v>
+        <v>472.4384783695589</v>
       </c>
       <c r="F15" t="n">
-        <v>472.4384783695589</v>
+        <v>185.874446883025</v>
       </c>
       <c r="G15" t="n">
-        <v>185.874446883025</v>
-      </c>
-      <c r="H15" t="n">
         <v>22.04667824967751</v>
       </c>
     </row>
@@ -878,15 +831,12 @@
         <v>17.71304893493652</v>
       </c>
       <c r="E16" t="n">
-        <v>0.4239999949932098</v>
+        <v>1656.947604950266</v>
       </c>
       <c r="F16" t="n">
-        <v>1656.947604950266</v>
+        <v>201.8397573898806</v>
       </c>
       <c r="G16" t="n">
-        <v>201.8397573898806</v>
-      </c>
-      <c r="H16" t="n">
         <v>18.07539141955594</v>
       </c>
     </row>
@@ -906,15 +856,12 @@
         <v>53.90745544433594</v>
       </c>
       <c r="E17" t="n">
-        <v>0.2000000029802322</v>
+        <v>826.3707136061979</v>
       </c>
       <c r="F17" t="n">
-        <v>826.3707136061979</v>
+        <v>164.1736930995773</v>
       </c>
       <c r="G17" t="n">
-        <v>164.1736930995773</v>
-      </c>
-      <c r="H17" t="n">
         <v>30.52602863281245</v>
       </c>
     </row>
@@ -934,15 +881,12 @@
         <v>48.38185119628906</v>
       </c>
       <c r="E18" t="n">
-        <v>0.3767099976539612</v>
+        <v>1489.98505775128</v>
       </c>
       <c r="F18" t="n">
-        <v>1489.98505775128</v>
+        <v>170.5698825442753</v>
       </c>
       <c r="G18" t="n">
-        <v>170.5698825442753</v>
-      </c>
-      <c r="H18" t="n">
         <v>30.15412007607718</v>
       </c>
     </row>
@@ -962,15 +906,12 @@
         <v>9.965688705444336</v>
       </c>
       <c r="E19" t="n">
-        <v>0.2660000026226044</v>
+        <v>1081.60187099801</v>
       </c>
       <c r="F19" t="n">
-        <v>1081.60187099801</v>
+        <v>211.2949664982855</v>
       </c>
       <c r="G19" t="n">
-        <v>211.2949664982855</v>
-      </c>
-      <c r="H19" t="n">
         <v>19.07671444842579</v>
       </c>
     </row>
@@ -990,15 +931,12 @@
         <v>34.95800018310547</v>
       </c>
       <c r="E20" t="n">
-        <v>0.08299999684095383</v>
+        <v>352.4357721162331</v>
       </c>
       <c r="F20" t="n">
-        <v>352.4357721162331</v>
+        <v>186.4471419042782</v>
       </c>
       <c r="G20" t="n">
-        <v>186.4471419042782</v>
-      </c>
-      <c r="H20" t="n">
         <v>30.37076642512884</v>
       </c>
     </row>
@@ -1018,15 +956,12 @@
         <v>52.31039428710938</v>
       </c>
       <c r="E21" t="n">
-        <v>0.1379999965429306</v>
+        <v>578.6172947152628</v>
       </c>
       <c r="F21" t="n">
-        <v>578.6172947152628</v>
+        <v>166.2520819406516</v>
       </c>
       <c r="G21" t="n">
-        <v>166.2520819406516</v>
-      </c>
-      <c r="H21" t="n">
         <v>32.91232473625846</v>
       </c>
     </row>
@@ -1046,15 +981,12 @@
         <v>57.66443634033203</v>
       </c>
       <c r="E22" t="n">
-        <v>0.05400000140070915</v>
+        <v>230.7935158149133</v>
       </c>
       <c r="F22" t="n">
-        <v>230.7935158149133</v>
+        <v>159.8473262299431</v>
       </c>
       <c r="G22" t="n">
-        <v>159.8473262299431</v>
-      </c>
-      <c r="H22" t="n">
         <v>33.90405576615215</v>
       </c>
     </row>
@@ -1074,15 +1006,12 @@
         <v>20.84729194641113</v>
       </c>
       <c r="E23" t="n">
-        <v>0.05799999833106995</v>
+        <v>247.6684183724716</v>
       </c>
       <c r="F23" t="n">
-        <v>247.6684183724716</v>
+        <v>202.4247601227709</v>
       </c>
       <c r="G23" t="n">
-        <v>202.4247601227709</v>
-      </c>
-      <c r="H23" t="n">
         <v>27.73866668831735</v>
       </c>
     </row>
@@ -1102,15 +1031,12 @@
         <v>42.37668228149414</v>
       </c>
       <c r="E24" t="n">
-        <v>0.5299999713897705</v>
+        <v>2015.283911619772</v>
       </c>
       <c r="F24" t="n">
-        <v>2015.283911619772</v>
+        <v>178.2303101447942</v>
       </c>
       <c r="G24" t="n">
-        <v>178.2303101447942</v>
-      </c>
-      <c r="H24" t="n">
         <v>33.39832911945414</v>
       </c>
     </row>
@@ -1130,15 +1056,12 @@
         <v>23.89204978942871</v>
       </c>
       <c r="E25" t="n">
-        <v>0.4020000100135803</v>
+        <v>1579.826051622189</v>
       </c>
       <c r="F25" t="n">
-        <v>1579.826051622189</v>
+        <v>199.510479607579</v>
       </c>
       <c r="G25" t="n">
-        <v>199.510479607579</v>
-      </c>
-      <c r="H25" t="n">
         <v>29.63265514420423</v>
       </c>
     </row>
@@ -1158,15 +1081,12 @@
         <v>3.194593906402588</v>
       </c>
       <c r="E26" t="n">
-        <v>0.5059999823570251</v>
+        <v>1936.049867434469</v>
       </c>
       <c r="F26" t="n">
-        <v>1936.049867434469</v>
+        <v>221.1759682227195</v>
       </c>
       <c r="G26" t="n">
-        <v>221.1759682227195</v>
-      </c>
-      <c r="H26" t="n">
         <v>22.39409690992864</v>
       </c>
     </row>
@@ -1186,15 +1106,12 @@
         <v>41.89826965332031</v>
       </c>
       <c r="E27" t="n">
-        <v>0.2259999960660934</v>
+        <v>927.9669661452913</v>
       </c>
       <c r="F27" t="n">
-        <v>927.9669661452913</v>
+        <v>179.0932631579409</v>
       </c>
       <c r="G27" t="n">
-        <v>179.0932631579409</v>
-      </c>
-      <c r="H27" t="n">
         <v>35.19544797408459</v>
       </c>
     </row>
@@ -1214,15 +1131,12 @@
         <v>4.495641231536865</v>
       </c>
       <c r="E28" t="n">
-        <v>0.1739999949932098</v>
+        <v>723.4123895726626</v>
       </c>
       <c r="F28" t="n">
-        <v>723.4123895726626</v>
+        <v>220.6957511158911</v>
       </c>
       <c r="G28" t="n">
-        <v>220.6957511158911</v>
-      </c>
-      <c r="H28" t="n">
         <v>24.338949894984</v>
       </c>
     </row>
@@ -1242,15 +1156,12 @@
         <v>11.56671619415283</v>
       </c>
       <c r="E29" t="n">
-        <v>0.1990000009536743</v>
+        <v>822.4359267571556</v>
       </c>
       <c r="F29" t="n">
-        <v>822.4359267571556</v>
+        <v>215.4547936858709</v>
       </c>
       <c r="G29" t="n">
-        <v>215.4547936858709</v>
-      </c>
-      <c r="H29" t="n">
         <v>30.89410316823072</v>
       </c>
     </row>
@@ -1270,15 +1181,12 @@
         <v>51.141845703125</v>
       </c>
       <c r="E30" t="n">
-        <v>0.5830000042915344</v>
+        <v>2186.405655380971</v>
       </c>
       <c r="F30" t="n">
-        <v>2186.405655380971</v>
+        <v>167.6055794666185</v>
       </c>
       <c r="G30" t="n">
-        <v>167.6055794666185</v>
-      </c>
-      <c r="H30" t="n">
         <v>39.1364989957745</v>
       </c>
     </row>
@@ -1298,15 +1206,12 @@
         <v>34.90697479248047</v>
       </c>
       <c r="E31" t="n">
-        <v>0.1449999958276749</v>
+        <v>606.9745772102617</v>
       </c>
       <c r="F31" t="n">
-        <v>606.9745772102617</v>
+        <v>188.4881336399034</v>
       </c>
       <c r="G31" t="n">
-        <v>188.4881336399034</v>
-      </c>
-      <c r="H31" t="n">
         <v>38.57761892185869</v>
       </c>
     </row>
@@ -1326,15 +1231,12 @@
         <v>20.10042953491211</v>
       </c>
       <c r="E32" t="n">
-        <v>0.3059999942779541</v>
+        <v>1232.001690836247</v>
       </c>
       <c r="F32" t="n">
-        <v>1232.001690836247</v>
+        <v>206.8248045598298</v>
       </c>
       <c r="G32" t="n">
-        <v>206.8248045598298</v>
-      </c>
-      <c r="H32" t="n">
         <v>35.82570420018077</v>
       </c>
     </row>
@@ -1354,15 +1256,12 @@
         <v>23.19077682495117</v>
       </c>
       <c r="E33" t="n">
-        <v>0.2230000048875809</v>
+        <v>916.3139966249578</v>
       </c>
       <c r="F33" t="n">
-        <v>916.3139966249578</v>
+        <v>204.4006996128279</v>
       </c>
       <c r="G33" t="n">
-        <v>204.4006996128279</v>
-      </c>
-      <c r="H33" t="n">
         <v>39.90343163897078</v>
       </c>
     </row>
@@ -1382,15 +1281,12 @@
         <v>33.48870086669922</v>
       </c>
       <c r="E34" t="n">
-        <v>0.3540000021457672</v>
+        <v>1408.222189015081</v>
       </c>
       <c r="F34" t="n">
-        <v>1408.222189015081</v>
+        <v>191.1184013879268</v>
       </c>
       <c r="G34" t="n">
-        <v>191.1184013879268</v>
-      </c>
-      <c r="H34" t="n">
         <v>42.44470192240891</v>
       </c>
     </row>
@@ -1410,15 +1306,12 @@
         <v>15.9302806854248</v>
       </c>
       <c r="E35" t="n">
-        <v>0.2119999974966049</v>
+        <v>873.4307914196993</v>
       </c>
       <c r="F35" t="n">
-        <v>873.4307914196993</v>
+        <v>213.5799215954228</v>
       </c>
       <c r="G35" t="n">
-        <v>213.5799215954228</v>
-      </c>
-      <c r="H35" t="n">
         <v>38.26181930326724</v>
       </c>
     </row>
@@ -1438,15 +1331,12 @@
         <v>49.87545776367188</v>
       </c>
       <c r="E36" t="n">
-        <v>0.1870000064373016</v>
+        <v>775.0615269997014</v>
       </c>
       <c r="F36" t="n">
-        <v>775.0615269997014</v>
+        <v>168.0950099107559</v>
       </c>
       <c r="G36" t="n">
-        <v>168.0950099107559</v>
-      </c>
-      <c r="H36" t="n">
         <v>45.68697248424435</v>
       </c>
     </row>
@@ -1466,15 +1356,12 @@
         <v>61.8179817199707</v>
       </c>
       <c r="E37" t="n">
-        <v>0.210999995470047</v>
+        <v>869.5202016942904</v>
       </c>
       <c r="F37" t="n">
-        <v>869.5202016942904</v>
+        <v>151.5795904696888</v>
       </c>
       <c r="G37" t="n">
-        <v>151.5795904696888</v>
-      </c>
-      <c r="H37" t="n">
         <v>43.2124825532333</v>
       </c>
     </row>
@@ -1494,15 +1381,12 @@
         <v>1.072644710540771</v>
       </c>
       <c r="E38" t="n">
-        <v>0.5770000219345093</v>
+        <v>2167.296925661129</v>
       </c>
       <c r="F38" t="n">
-        <v>2167.296925661129</v>
+        <v>235.3603953607503</v>
       </c>
       <c r="G38" t="n">
-        <v>235.3603953607503</v>
-      </c>
-      <c r="H38" t="n">
         <v>38.56086142877915</v>
       </c>
     </row>
@@ -1522,15 +1406,12 @@
         <v>45.89204025268555</v>
       </c>
       <c r="E39" t="n">
-        <v>0.3989999890327454</v>
+        <v>1569.235152018134</v>
       </c>
       <c r="F39" t="n">
-        <v>1569.235152018134</v>
+        <v>172.8821816193272</v>
       </c>
       <c r="G39" t="n">
-        <v>172.8821816193272</v>
-      </c>
-      <c r="H39" t="n">
         <v>49.75183136937554</v>
       </c>
     </row>
@@ -1550,15 +1431,12 @@
         <v>49.21414566040039</v>
       </c>
       <c r="E40" t="n">
-        <v>0.3799999952316284</v>
+        <v>1501.744593228529</v>
       </c>
       <c r="F40" t="n">
-        <v>1501.744593228529</v>
+        <v>167.6515683277358</v>
       </c>
       <c r="G40" t="n">
-        <v>167.6515683277358</v>
-      </c>
-      <c r="H40" t="n">
         <v>49.58651425014828</v>
       </c>
     </row>
@@ -1578,15 +1456,12 @@
         <v>29.1705379486084</v>
       </c>
       <c r="E41" t="n">
-        <v>0.5580000281333923</v>
+        <v>2106.343909760358</v>
       </c>
       <c r="F41" t="n">
-        <v>2106.343909760358</v>
+        <v>199.5504344044182</v>
       </c>
       <c r="G41" t="n">
-        <v>199.5504344044182</v>
-      </c>
-      <c r="H41" t="n">
         <v>52.63416273614697</v>
       </c>
     </row>
@@ -1606,15 +1481,12 @@
         <v>34.92112350463867</v>
       </c>
       <c r="E42" t="n">
-        <v>0.6119999885559082</v>
+        <v>2277.828672355331</v>
       </c>
       <c r="F42" t="n">
-        <v>2277.828672355331</v>
+        <v>190.0282006580422</v>
       </c>
       <c r="G42" t="n">
-        <v>190.0282006580422</v>
-      </c>
-      <c r="H42" t="n">
         <v>54.17913076411402</v>
       </c>
     </row>
@@ -1634,15 +1506,12 @@
         <v>6.373631954193115</v>
       </c>
       <c r="E43" t="n">
-        <v>0.6499999761581421</v>
+        <v>2395.304963072071</v>
       </c>
       <c r="F43" t="n">
-        <v>2395.304963072071</v>
+        <v>233.50096097581</v>
       </c>
       <c r="G43" t="n">
-        <v>233.50096097581</v>
-      </c>
-      <c r="H43" t="n">
         <v>46.02256622120216</v>
       </c>
     </row>
@@ -1662,15 +1531,12 @@
         <v>42.48298263549805</v>
       </c>
       <c r="E44" t="n">
-        <v>0.3650000095367432</v>
+        <v>1447.954363211065</v>
       </c>
       <c r="F44" t="n">
-        <v>1447.954363211065</v>
+        <v>176.9216254086938</v>
       </c>
       <c r="G44" t="n">
-        <v>176.9216254086938</v>
-      </c>
-      <c r="H44" t="n">
         <v>54.39503658450563</v>
       </c>
     </row>
@@ -1690,15 +1556,12 @@
         <v>49.43538665771484</v>
       </c>
       <c r="E45" t="n">
-        <v>0.2119999974966049</v>
+        <v>873.4307914196993</v>
       </c>
       <c r="F45" t="n">
-        <v>873.4307914196993</v>
+        <v>165.5301745409713</v>
       </c>
       <c r="G45" t="n">
-        <v>165.5301745409713</v>
-      </c>
-      <c r="H45" t="n">
         <v>52.7128041733207</v>
       </c>
     </row>
@@ -1718,15 +1581,12 @@
         <v>6.142007350921631</v>
       </c>
       <c r="E46" t="n">
-        <v>0.4490000009536743</v>
+        <v>1743.428171899722</v>
       </c>
       <c r="F46" t="n">
-        <v>1743.428171899722</v>
+        <v>237.7476753956505</v>
       </c>
       <c r="G46" t="n">
-        <v>237.7476753956505</v>
-      </c>
-      <c r="H46" t="n">
         <v>49.78141165294394</v>
       </c>
     </row>
@@ -1746,15 +1606,12 @@
         <v>63.29279327392578</v>
       </c>
       <c r="E47" t="n">
-        <v>0.5820000171661377</v>
+        <v>2183.225532378438</v>
       </c>
       <c r="F47" t="n">
-        <v>2183.225532378438</v>
+        <v>145.6929541877977</v>
       </c>
       <c r="G47" t="n">
-        <v>145.6929541877977</v>
-      </c>
-      <c r="H47" t="n">
         <v>46.97503063890456</v>
       </c>
     </row>
@@ -1774,15 +1631,12 @@
         <v>50.88592529296875</v>
       </c>
       <c r="E48" t="n">
-        <v>0.3610000014305115</v>
+        <v>1433.534310193219</v>
       </c>
       <c r="F48" t="n">
-        <v>1433.534310193219</v>
+        <v>161.4466616146051</v>
       </c>
       <c r="G48" t="n">
-        <v>161.4466616146051</v>
-      </c>
-      <c r="H48" t="n">
         <v>54.44603636948661</v>
       </c>
     </row>
@@ -1802,15 +1656,12 @@
         <v>37.62113952636719</v>
       </c>
       <c r="E49" t="n">
-        <v>0.5279999971389771</v>
+        <v>2008.723036449022</v>
       </c>
       <c r="F49" t="n">
-        <v>2008.723036449022</v>
+        <v>184.2725657102087</v>
       </c>
       <c r="G49" t="n">
-        <v>184.2725657102087</v>
-      </c>
-      <c r="H49" t="n">
         <v>59.11119534742926</v>
       </c>
     </row>
@@ -1830,15 +1681,12 @@
         <v>39.00973129272461</v>
       </c>
       <c r="E50" t="n">
-        <v>0.2099999934434891</v>
+        <v>865.6075942787213</v>
       </c>
       <c r="F50" t="n">
-        <v>865.6075942787213</v>
+        <v>180.851954975237</v>
       </c>
       <c r="G50" t="n">
-        <v>180.851954975237</v>
-      </c>
-      <c r="H50" t="n">
         <v>60.55262642715537</v>
       </c>
     </row>
@@ -1858,15 +1706,12 @@
         <v>24.15542984008789</v>
       </c>
       <c r="E51" t="n">
-        <v>0.5600000023841858</v>
+        <v>2112.791679272088</v>
       </c>
       <c r="F51" t="n">
-        <v>2112.791679272088</v>
+        <v>211.5515502940325</v>
       </c>
       <c r="G51" t="n">
-        <v>211.5515502940325</v>
-      </c>
-      <c r="H51" t="n">
         <v>61.00195275957411</v>
       </c>
     </row>
@@ -1886,15 +1731,12 @@
         <v>39.70672988891602</v>
       </c>
       <c r="E52" t="n">
-        <v>0.4979999959468842</v>
+        <v>1909.393880329576</v>
       </c>
       <c r="F52" t="n">
-        <v>1909.393880329576</v>
+        <v>178.3920516037439</v>
       </c>
       <c r="G52" t="n">
-        <v>178.3920516037439</v>
-      </c>
-      <c r="H52" t="n">
         <v>62.16010539961907</v>
       </c>
     </row>
@@ -1914,15 +1756,12 @@
         <v>49.50532150268555</v>
       </c>
       <c r="E53" t="n">
-        <v>0.1400000005960464</v>
+        <v>586.7293479424766</v>
       </c>
       <c r="F53" t="n">
-        <v>586.7293479424766</v>
+        <v>160.2472928171692</v>
       </c>
       <c r="G53" t="n">
-        <v>160.2472928171692</v>
-      </c>
-      <c r="H53" t="n">
         <v>58.20941647675482</v>
       </c>
     </row>
@@ -1942,15 +1781,12 @@
         <v>56.46826171875</v>
       </c>
       <c r="E54" t="n">
-        <v>0.1430000066757202</v>
+        <v>598.8824976040644</v>
       </c>
       <c r="F54" t="n">
-        <v>598.8824976040644</v>
+        <v>149.5898498865417</v>
       </c>
       <c r="G54" t="n">
-        <v>149.5898498865417</v>
-      </c>
-      <c r="H54" t="n">
         <v>54.42879075775696</v>
       </c>
     </row>
@@ -1970,15 +1806,12 @@
         <v>40.3358268737793</v>
       </c>
       <c r="E55" t="n">
-        <v>0.2249999940395355</v>
+        <v>924.0846438011745</v>
       </c>
       <c r="F55" t="n">
-        <v>924.0846438011745</v>
+        <v>175.8469476326254</v>
       </c>
       <c r="G55" t="n">
-        <v>175.8469476326254</v>
-      </c>
-      <c r="H55" t="n">
         <v>63.555059895797</v>
       </c>
     </row>
@@ -1998,15 +1831,12 @@
         <v>38.20518112182617</v>
       </c>
       <c r="E56" t="n">
-        <v>0.02999999932944775</v>
+        <v>128.9003855881938</v>
       </c>
       <c r="F56" t="n">
-        <v>128.9003855881938</v>
+        <v>179.8357877680561</v>
       </c>
       <c r="G56" t="n">
-        <v>179.8357877680561</v>
-      </c>
-      <c r="H56" t="n">
         <v>65.03781332953814</v>
       </c>
     </row>
@@ -2026,15 +1856,12 @@
         <v>39.74899673461914</v>
       </c>
       <c r="E57" t="n">
-        <v>0.0989999994635582</v>
+        <v>418.8482280609101</v>
       </c>
       <c r="F57" t="n">
-        <v>418.8482280609101</v>
+        <v>176.2092588270897</v>
       </c>
       <c r="G57" t="n">
-        <v>176.2092588270897</v>
-      </c>
-      <c r="H57" t="n">
         <v>64.74895803570412</v>
       </c>
     </row>
@@ -2054,15 +1881,12 @@
         <v>15.02733516693115</v>
       </c>
       <c r="E58" t="n">
-        <v>0.6000000238418579</v>
+        <v>2240.185974418625</v>
       </c>
       <c r="F58" t="n">
-        <v>2240.185974418625</v>
+        <v>234.34727958246</v>
       </c>
       <c r="G58" t="n">
-        <v>234.34727958246</v>
-      </c>
-      <c r="H58" t="n">
         <v>63.06038848548737</v>
       </c>
     </row>
@@ -2082,15 +1906,12 @@
         <v>37.58807754516602</v>
       </c>
       <c r="E59" t="n">
-        <v>0.3974219858646393</v>
+        <v>1563.657198577747</v>
       </c>
       <c r="F59" t="n">
-        <v>1563.657198577747</v>
+        <v>180.457347654663</v>
       </c>
       <c r="G59" t="n">
-        <v>180.457347654663</v>
-      </c>
-      <c r="H59" t="n">
         <v>66.2143548292574</v>
       </c>
     </row>
@@ -2110,15 +1931,12 @@
         <v>20.23810386657715</v>
       </c>
       <c r="E60" t="n">
-        <v>0.1379999965429306</v>
+        <v>578.6172947152628</v>
       </c>
       <c r="F60" t="n">
-        <v>578.6172947152628</v>
+        <v>225.5716267064807</v>
       </c>
       <c r="G60" t="n">
-        <v>225.5716267064807</v>
-      </c>
-      <c r="H60" t="n">
         <v>67.36670331755562</v>
       </c>
     </row>
@@ -2138,15 +1956,12 @@
         <v>42.20166015625</v>
       </c>
       <c r="E61" t="n">
-        <v>0.1239999979734421</v>
+        <v>521.6104982541038</v>
       </c>
       <c r="F61" t="n">
-        <v>521.6104982541038</v>
+        <v>167.856902782118</v>
       </c>
       <c r="G61" t="n">
-        <v>167.856902782118</v>
-      </c>
-      <c r="H61" t="n">
         <v>66.16418823817627</v>
       </c>
     </row>
@@ -2166,15 +1981,12 @@
         <v>58.16561508178711</v>
       </c>
       <c r="E62" t="n">
-        <v>0.3600000143051147</v>
+        <v>1429.924347323077</v>
       </c>
       <c r="F62" t="n">
-        <v>1429.924347323077</v>
+        <v>141.6893921444634</v>
       </c>
       <c r="G62" t="n">
-        <v>141.6893921444634</v>
-      </c>
-      <c r="H62" t="n">
         <v>55.9604528362288</v>
       </c>
     </row>
@@ -2194,15 +2006,12 @@
         <v>25.8327808380127</v>
       </c>
       <c r="E63" t="n">
-        <v>0.1560000032186508</v>
+        <v>651.3386580792431</v>
       </c>
       <c r="F63" t="n">
-        <v>651.3386580792431</v>
+        <v>213.1465867327724</v>
       </c>
       <c r="G63" t="n">
-        <v>213.1465867327724</v>
-      </c>
-      <c r="H63" t="n">
         <v>73.27986298713279</v>
       </c>
     </row>
@@ -2222,15 +2031,12 @@
         <v>15.48001480102539</v>
       </c>
       <c r="E64" t="n">
-        <v>0.2440000027418137</v>
+        <v>997.5030593997925</v>
       </c>
       <c r="F64" t="n">
-        <v>997.5030593997925</v>
+        <v>244.6038972738466</v>
       </c>
       <c r="G64" t="n">
-        <v>244.6038972738466</v>
-      </c>
-      <c r="H64" t="n">
         <v>69.83077528557813</v>
       </c>
     </row>
@@ -2250,15 +2056,12 @@
         <v>15.77690410614014</v>
       </c>
       <c r="E65" t="n">
-        <v>0.2989999949932098</v>
+        <v>1205.915061750614</v>
       </c>
       <c r="F65" t="n">
-        <v>1205.915061750614</v>
+        <v>244.5908969669972</v>
       </c>
       <c r="G65" t="n">
-        <v>244.5908969669972</v>
-      </c>
-      <c r="H65" t="n">
         <v>70.30592729967964</v>
       </c>
     </row>
@@ -2278,15 +2081,12 @@
         <v>61.35290145874023</v>
       </c>
       <c r="E66" t="n">
-        <v>0.04899999871850014</v>
+        <v>209.6566093130006</v>
       </c>
       <c r="F66" t="n">
-        <v>209.6566093130006</v>
+        <v>136.7459514614812</v>
       </c>
       <c r="G66" t="n">
-        <v>136.7459514614812</v>
-      </c>
-      <c r="H66" t="n">
         <v>53.90689117248857</v>
       </c>
     </row>
@@ -2306,15 +2106,12 @@
         <v>19.5903205871582</v>
       </c>
       <c r="E67" t="n">
-        <v>0.02171799913048744</v>
+        <v>93.48446529540507</v>
       </c>
       <c r="F67" t="n">
-        <v>93.48446529540507</v>
+        <v>235.771105621029</v>
       </c>
       <c r="G67" t="n">
-        <v>235.771105621029</v>
-      </c>
-      <c r="H67" t="n">
         <v>73.02859819966865</v>
       </c>
     </row>
@@ -2334,15 +2131,12 @@
         <v>24.30084228515625</v>
       </c>
       <c r="E68" t="n">
-        <v>0.2000000029802322</v>
+        <v>826.3707136061979</v>
       </c>
       <c r="F68" t="n">
-        <v>826.3707136061979</v>
+        <v>221.1457388558182</v>
       </c>
       <c r="G68" t="n">
-        <v>221.1457388558182</v>
-      </c>
-      <c r="H68" t="n">
         <v>75.96302613210874</v>
       </c>
     </row>
@@ -2362,15 +2156,12 @@
         <v>49.49262237548828</v>
       </c>
       <c r="E69" t="n">
-        <v>0.3339999914169312</v>
+        <v>1335.3602067056</v>
       </c>
       <c r="F69" t="n">
-        <v>1335.3602067056</v>
+        <v>145.6204816776282</v>
       </c>
       <c r="G69" t="n">
-        <v>145.6204816776282</v>
-      </c>
-      <c r="H69" t="n">
         <v>64.99564919843898</v>
       </c>
     </row>
@@ -2390,15 +2181,12 @@
         <v>60.51219177246094</v>
       </c>
       <c r="E70" t="n">
-        <v>0.06499999761581421</v>
+        <v>277.125303444809</v>
       </c>
       <c r="F70" t="n">
-        <v>277.125303444809</v>
+        <v>133.4418834029724</v>
       </c>
       <c r="G70" t="n">
-        <v>133.4418834029724</v>
-      </c>
-      <c r="H70" t="n">
         <v>55.61926798865239</v>
       </c>
     </row>
@@ -2418,15 +2206,12 @@
         <v>61.34061431884766</v>
       </c>
       <c r="E71" t="n">
-        <v>0.2750000059604645</v>
+        <v>1115.723809237682</v>
       </c>
       <c r="F71" t="n">
-        <v>1115.723809237682</v>
+        <v>131.9651880062851</v>
       </c>
       <c r="G71" t="n">
-        <v>131.9651880062851</v>
-      </c>
-      <c r="H71" t="n">
         <v>55.02232038849426</v>
       </c>
     </row>
@@ -2446,15 +2231,12 @@
         <v>-2.713768005371094</v>
       </c>
       <c r="E72" t="n">
-        <v>0.3589999973773956</v>
+        <v>1426.312274688342</v>
       </c>
       <c r="F72" t="n">
-        <v>1426.312274688342</v>
+        <v>285.6103354390478</v>
       </c>
       <c r="G72" t="n">
-        <v>285.6103354390478</v>
-      </c>
-      <c r="H72" t="n">
         <v>58.96364214349016</v>
       </c>
     </row>
@@ -2474,15 +2256,12 @@
         <v>30.11482238769531</v>
       </c>
       <c r="E73" t="n">
-        <v>0.1299999952316284</v>
+        <v>546.0896141426656</v>
       </c>
       <c r="F73" t="n">
-        <v>546.0896141426656</v>
+        <v>188.8666537572836</v>
       </c>
       <c r="G73" t="n">
-        <v>188.8666537572836</v>
-      </c>
-      <c r="H73" t="n">
         <v>82.06187773446577</v>
       </c>
     </row>
@@ -2502,15 +2281,12 @@
         <v>-0.4782386422157288</v>
       </c>
       <c r="E74" t="n">
-        <v>0.4189999997615814</v>
+        <v>1639.503972536957</v>
       </c>
       <c r="F74" t="n">
-        <v>1639.503972536957</v>
+        <v>285.3804349262129</v>
       </c>
       <c r="G74" t="n">
-        <v>285.3804349262129</v>
-      </c>
-      <c r="H74" t="n">
         <v>61.25154181229235</v>
       </c>
     </row>
@@ -2530,15 +2306,12 @@
         <v>-3.212921857833862</v>
       </c>
       <c r="E75" t="n">
-        <v>0.2989999949932098</v>
+        <v>1205.915061750614</v>
       </c>
       <c r="F75" t="n">
-        <v>1205.915061750614</v>
+        <v>287.5483319154165</v>
       </c>
       <c r="G75" t="n">
-        <v>287.5483319154165</v>
-      </c>
-      <c r="H75" t="n">
         <v>58.70790553974744</v>
       </c>
     </row>
@@ -2558,15 +2331,12 @@
         <v>30.16693115234375</v>
       </c>
       <c r="E76" t="n">
-        <v>0.1840000003576279</v>
+        <v>763.1726232934241</v>
       </c>
       <c r="F76" t="n">
-        <v>763.1726232934241</v>
+        <v>186.4431504600458</v>
       </c>
       <c r="G76" t="n">
-        <v>186.4431504600458</v>
-      </c>
-      <c r="H76" t="n">
         <v>82.7350715996196</v>
       </c>
     </row>
@@ -2586,15 +2356,12 @@
         <v>28.23212242126465</v>
       </c>
       <c r="E77" t="n">
-        <v>0.1019999980926514</v>
+        <v>431.2447065513599</v>
       </c>
       <c r="F77" t="n">
-        <v>431.2447065513599</v>
+        <v>201.7391806851846</v>
       </c>
       <c r="G77" t="n">
-        <v>201.7391806851846</v>
-      </c>
-      <c r="H77" t="n">
         <v>83.29053790221776</v>
       </c>
     </row>
@@ -2614,15 +2381,12 @@
         <v>24.6070442199707</v>
       </c>
       <c r="E78" t="n">
-        <v>0.2189999967813492</v>
+        <v>900.7483492023172</v>
       </c>
       <c r="F78" t="n">
-        <v>900.7483492023172</v>
+        <v>233.9729892145359</v>
       </c>
       <c r="G78" t="n">
-        <v>233.9729892145359</v>
-      </c>
-      <c r="H78" t="n">
         <v>83.42441521408441</v>
       </c>
     </row>
@@ -2642,15 +2406,12 @@
         <v>21.38190269470215</v>
       </c>
       <c r="E79" t="n">
-        <v>0.4339999854564667</v>
+        <v>1691.687106632469</v>
       </c>
       <c r="F79" t="n">
-        <v>1691.687106632469</v>
+        <v>255.0624608818417</v>
       </c>
       <c r="G79" t="n">
-        <v>255.0624608818417</v>
-      </c>
-      <c r="H79" t="n">
         <v>81.66152573596764</v>
       </c>
     </row>
@@ -2670,15 +2431,12 @@
         <v>2.024992942810059</v>
       </c>
       <c r="E80" t="n">
-        <v>0.1580000072717667</v>
+        <v>659.3789000935117</v>
       </c>
       <c r="F80" t="n">
-        <v>659.3789000935117</v>
+        <v>290.0221226405291</v>
       </c>
       <c r="G80" t="n">
-        <v>290.0221226405291</v>
-      </c>
-      <c r="H80" t="n">
         <v>64.33829691205085</v>
       </c>
     </row>
@@ -2698,15 +2456,12 @@
         <v>25.29787635803223</v>
       </c>
       <c r="E81" t="n">
-        <v>0.135000005364418</v>
+        <v>566.434356575713</v>
       </c>
       <c r="F81" t="n">
-        <v>566.434356575713</v>
+        <v>232.8530732554522</v>
       </c>
       <c r="G81" t="n">
-        <v>232.8530732554522</v>
-      </c>
-      <c r="H81" t="n">
         <v>84.91711617677194</v>
       </c>
     </row>
@@ -2726,15 +2481,12 @@
         <v>12.38887977600098</v>
       </c>
       <c r="E82" t="n">
-        <v>0.004282999783754349</v>
+        <v>18.50588103089174</v>
       </c>
       <c r="F82" t="n">
-        <v>18.50588103089174</v>
+        <v>283.7712082555389</v>
       </c>
       <c r="G82" t="n">
-        <v>283.7712082555389</v>
-      </c>
-      <c r="H82" t="n">
         <v>74.48825666506053</v>
       </c>
     </row>
@@ -2754,15 +2506,12 @@
         <v>14.3680305480957</v>
       </c>
       <c r="E83" t="n">
-        <v>0.2560000121593475</v>
+        <v>1043.496525858729</v>
       </c>
       <c r="F83" t="n">
-        <v>1043.496525858729</v>
+        <v>281.8921172763349</v>
       </c>
       <c r="G83" t="n">
-        <v>281.8921172763349</v>
-      </c>
-      <c r="H83" t="n">
         <v>76.41707829778731</v>
       </c>
     </row>
@@ -2782,15 +2531,12 @@
         <v>64.26630401611328</v>
       </c>
       <c r="E84" t="n">
-        <v>0.1630000025033951</v>
+        <v>679.4444413307867</v>
       </c>
       <c r="F84" t="n">
-        <v>679.4444413307867</v>
+        <v>126.4813572877882</v>
       </c>
       <c r="G84" t="n">
-        <v>126.4813572877882</v>
-      </c>
-      <c r="H84" t="n">
         <v>52.72516890602747</v>
       </c>
     </row>
@@ -2810,15 +2556,12 @@
         <v>28.79290008544922</v>
       </c>
       <c r="E85" t="n">
-        <v>0.2364509999752045</v>
+        <v>968.4201348245213</v>
       </c>
       <c r="F85" t="n">
-        <v>968.4201348245213</v>
+        <v>190.8352813272477</v>
       </c>
       <c r="G85" t="n">
-        <v>190.8352813272477</v>
-      </c>
-      <c r="H85" t="n">
         <v>85.34586086634012</v>
       </c>
     </row>
@@ -2838,15 +2581,12 @@
         <v>44.35237503051758</v>
       </c>
       <c r="E86" t="n">
-        <v>0.6000000238418579</v>
+        <v>2240.185974418625</v>
       </c>
       <c r="F86" t="n">
-        <v>2240.185974418625</v>
+        <v>125.6027117904971</v>
       </c>
       <c r="G86" t="n">
-        <v>125.6027117904971</v>
-      </c>
-      <c r="H86" t="n">
         <v>72.75290303465637</v>
       </c>
     </row>
@@ -2866,15 +2606,12 @@
         <v>3.473009824752808</v>
       </c>
       <c r="E87" t="n">
-        <v>0.06599999964237213</v>
+        <v>281.3257125002922</v>
       </c>
       <c r="F87" t="n">
-        <v>281.3257125002922</v>
+        <v>304.3938914960014</v>
       </c>
       <c r="G87" t="n">
-        <v>304.3938914960014</v>
-      </c>
-      <c r="H87" t="n">
         <v>66.33808457924333</v>
       </c>
     </row>
@@ -2894,15 +2631,12 @@
         <v>22.18258476257324</v>
       </c>
       <c r="E88" t="n">
-        <v>0.5090000033378601</v>
+        <v>1946.014319805091</v>
       </c>
       <c r="F88" t="n">
-        <v>1946.014319805091</v>
+        <v>310.9003864000454</v>
       </c>
       <c r="G88" t="n">
-        <v>310.9003864000454</v>
-      </c>
-      <c r="H88" t="n">
         <v>85.00807392479871</v>
       </c>
     </row>
@@ -2922,15 +2656,12 @@
         <v>-5.79459285736084</v>
       </c>
       <c r="E89" t="n">
-        <v>0.5360000133514404</v>
+        <v>2034.921432753547</v>
       </c>
       <c r="F89" t="n">
-        <v>2034.921432753547</v>
+        <v>305.0998846118308</v>
       </c>
       <c r="G89" t="n">
-        <v>305.0998846118308</v>
-      </c>
-      <c r="H89" t="n">
         <v>57.05720524664127</v>
       </c>
     </row>
@@ -2950,15 +2681,12 @@
         <v>61.36655807495117</v>
       </c>
       <c r="E90" t="n">
-        <v>0.2240000069141388</v>
+        <v>920.2003591656152</v>
       </c>
       <c r="F90" t="n">
-        <v>920.2003591656152</v>
+        <v>121.4659798152458</v>
       </c>
       <c r="G90" t="n">
-        <v>121.4659798152458</v>
-      </c>
-      <c r="H90" t="n">
         <v>55.7420815224022</v>
       </c>
     </row>
@@ -2978,15 +2706,12 @@
         <v>48.47776031494141</v>
       </c>
       <c r="E91" t="n">
-        <v>0.5009999871253967</v>
+        <v>1919.40425528274</v>
       </c>
       <c r="F91" t="n">
-        <v>1919.40425528274</v>
+        <v>113.4210086615013</v>
       </c>
       <c r="G91" t="n">
-        <v>113.4210086615013</v>
-      </c>
-      <c r="H91" t="n">
         <v>68.25727662537837</v>
       </c>
     </row>
@@ -3006,15 +2731,12 @@
         <v>14.07064819335938</v>
       </c>
       <c r="E92" t="n">
-        <v>0.5730000138282776</v>
+        <v>2154.520586195584</v>
       </c>
       <c r="F92" t="n">
-        <v>2154.520586195584</v>
+        <v>331.0264520499293</v>
       </c>
       <c r="G92" t="n">
-        <v>331.0264520499293</v>
-      </c>
-      <c r="H92" t="n">
         <v>75.38452389248357</v>
       </c>
     </row>
@@ -3034,15 +2756,12 @@
         <v>44.18074798583984</v>
       </c>
       <c r="E93" t="n">
-        <v>0.5460000038146973</v>
+        <v>2067.499118066273</v>
       </c>
       <c r="F93" t="n">
-        <v>2067.499118066273</v>
+        <v>96.05410900986132</v>
       </c>
       <c r="G93" t="n">
-        <v>96.05410900986132</v>
-      </c>
-      <c r="H93" t="n">
         <v>70.29735077732514</v>
       </c>
     </row>
@@ -3062,15 +2781,12 @@
         <v>39.98970031738281</v>
       </c>
       <c r="E94" t="n">
-        <v>0.1720000058412552</v>
+        <v>715.4362988699944</v>
       </c>
       <c r="F94" t="n">
-        <v>715.4362988699944</v>
+        <v>87.33566812682206</v>
       </c>
       <c r="G94" t="n">
-        <v>87.33566812682206</v>
-      </c>
-      <c r="H94" t="n">
         <v>73.50951317099407</v>
       </c>
     </row>
@@ -3090,15 +2806,12 @@
         <v>15.98397254943848</v>
       </c>
       <c r="E95" t="n">
-        <v>0.2440000027418137</v>
+        <v>997.5030593997925</v>
       </c>
       <c r="F95" t="n">
-        <v>997.5030593997925</v>
+        <v>2.539795875341265</v>
       </c>
       <c r="G95" t="n">
-        <v>2.539795875341265</v>
-      </c>
-      <c r="H95" t="n">
         <v>70.08723433248876</v>
       </c>
     </row>
@@ -3118,15 +2831,12 @@
         <v>4.028957843780518</v>
       </c>
       <c r="E96" t="n">
-        <v>0.3440000116825104</v>
+        <v>1371.891644524125</v>
       </c>
       <c r="F96" t="n">
-        <v>1371.891644524125</v>
+        <v>343.356454326494</v>
       </c>
       <c r="G96" t="n">
-        <v>343.356454326494</v>
-      </c>
-      <c r="H96" t="n">
         <v>60.99387507635056</v>
       </c>
     </row>
@@ -3146,15 +2856,12 @@
         <v>52.82292938232422</v>
       </c>
       <c r="E97" t="n">
-        <v>0.07648999989032745</v>
+        <v>325.2711537377689</v>
       </c>
       <c r="F97" t="n">
-        <v>325.2711537377689</v>
+        <v>98.17146981808737</v>
       </c>
       <c r="G97" t="n">
-        <v>98.17146981808737</v>
-      </c>
-      <c r="H97" t="n">
         <v>60.26679845594848</v>
       </c>
     </row>
@@ -3174,15 +2881,12 @@
         <v>48.51522445678711</v>
       </c>
       <c r="E98" t="n">
-        <v>0.4959999918937683</v>
+        <v>1902.710656439457</v>
       </c>
       <c r="F98" t="n">
-        <v>1902.710656439457</v>
+        <v>91.19850370499088</v>
       </c>
       <c r="G98" t="n">
-        <v>91.19850370499088</v>
-      </c>
-      <c r="H98" t="n">
         <v>63.09742003770977</v>
       </c>
     </row>
@@ -3202,15 +2906,12 @@
         <v>25.7291259765625</v>
       </c>
       <c r="E99" t="n">
-        <v>0.2370000034570694</v>
+        <v>970.5390841006508</v>
       </c>
       <c r="F99" t="n">
-        <v>970.5390841006508</v>
+        <v>33.71460610300097</v>
       </c>
       <c r="G99" t="n">
-        <v>33.71460610300097</v>
-      </c>
-      <c r="H99" t="n">
         <v>70.59372559903728</v>
       </c>
     </row>
@@ -3230,15 +2931,12 @@
         <v>4.745282173156738</v>
       </c>
       <c r="E100" t="n">
-        <v>0.1430000066757202</v>
+        <v>598.8824976040644</v>
       </c>
       <c r="F100" t="n">
-        <v>598.8824976040644</v>
+        <v>349.978509379617</v>
       </c>
       <c r="G100" t="n">
-        <v>349.978509379617</v>
-      </c>
-      <c r="H100" t="n">
         <v>59.3198698029064</v>
       </c>
     </row>
@@ -3258,15 +2956,12 @@
         <v>54.39066696166992</v>
       </c>
       <c r="E101" t="n">
-        <v>0.1529999971389771</v>
+        <v>639.2633050973789</v>
       </c>
       <c r="F101" t="n">
-        <v>639.2633050973789</v>
+        <v>98.30243691724219</v>
       </c>
       <c r="G101" t="n">
-        <v>98.30243691724219</v>
-      </c>
-      <c r="H101" t="n">
         <v>58.30848489225325</v>
       </c>
     </row>
@@ -3286,15 +2981,12 @@
         <v>58.01887893676758</v>
       </c>
       <c r="E102" t="n">
-        <v>0.6349999904632568</v>
+        <v>2349.244257634401</v>
       </c>
       <c r="F102" t="n">
-        <v>2349.244257634401</v>
+        <v>101.8492086867801</v>
       </c>
       <c r="G102" t="n">
-        <v>101.8492086867801</v>
-      </c>
-      <c r="H102" t="n">
         <v>55.21857129706387</v>
       </c>
     </row>
@@ -3314,15 +3006,12 @@
         <v>42.67203521728516</v>
       </c>
       <c r="E103" t="n">
-        <v>0.1289999932050705</v>
+        <v>542.0147093189177</v>
       </c>
       <c r="F103" t="n">
-        <v>542.0147093189177</v>
+        <v>77.48566790521888</v>
       </c>
       <c r="G103" t="n">
-        <v>77.48566790521888</v>
-      </c>
-      <c r="H103" t="n">
         <v>64.8988126310412</v>
       </c>
     </row>
@@ -3342,15 +3031,12 @@
         <v>56.66003799438477</v>
       </c>
       <c r="E104" t="n">
-        <v>0.1500000059604645</v>
+        <v>627.1700359849448</v>
       </c>
       <c r="F104" t="n">
-        <v>627.1700359849448</v>
+        <v>97.72870692965985</v>
       </c>
       <c r="G104" t="n">
-        <v>97.72870692965985</v>
-      </c>
-      <c r="H104" t="n">
         <v>54.99658828453175</v>
       </c>
     </row>
@@ -3370,15 +3056,12 @@
         <v>39.52298355102539</v>
       </c>
       <c r="E105" t="n">
-        <v>0.3440000116825104</v>
+        <v>1371.891644524125</v>
       </c>
       <c r="F105" t="n">
-        <v>1371.891644524125</v>
+        <v>68.79583747417368</v>
       </c>
       <c r="G105" t="n">
-        <v>68.79583747417368</v>
-      </c>
-      <c r="H105" t="n">
         <v>64.42668452711504</v>
       </c>
     </row>
@@ -3398,15 +3081,12 @@
         <v>6.175134658813477</v>
       </c>
       <c r="E106" t="n">
-        <v>0.3959999978542328</v>
+        <v>1558.62649529763</v>
       </c>
       <c r="F106" t="n">
-        <v>1558.62649529763</v>
+        <v>359.0613035363558</v>
       </c>
       <c r="G106" t="n">
-        <v>359.0613035363558</v>
-      </c>
-      <c r="H106" t="n">
         <v>56.59426497141165</v>
       </c>
     </row>
@@ -3426,15 +3106,12 @@
         <v>12.00308227539062</v>
       </c>
       <c r="E107" t="n">
-        <v>0.1630000025033951</v>
+        <v>679.4444413307867</v>
       </c>
       <c r="F107" t="n">
-        <v>679.4444413307867</v>
+        <v>8.326391244799357</v>
       </c>
       <c r="G107" t="n">
-        <v>8.326391244799357</v>
-      </c>
-      <c r="H107" t="n">
         <v>59.82810578059493</v>
       </c>
     </row>
@@ -3454,15 +3131,12 @@
         <v>25.26393508911133</v>
       </c>
       <c r="E108" t="n">
-        <v>0.5290219783782959</v>
+        <v>2012.076573556624</v>
       </c>
       <c r="F108" t="n">
-        <v>2012.076573556624</v>
+        <v>35.06898725925156</v>
       </c>
       <c r="G108" t="n">
-        <v>35.06898725925156</v>
-      </c>
-      <c r="H108" t="n">
         <v>64.8249872712824</v>
       </c>
     </row>
@@ -3482,15 +3156,12 @@
         <v>27.75633811950684</v>
       </c>
       <c r="E109" t="n">
-        <v>0.2269999980926514</v>
+        <v>931.8472681578297</v>
       </c>
       <c r="F109" t="n">
-        <v>931.8472681578297</v>
+        <v>41.19890036398075</v>
       </c>
       <c r="G109" t="n">
-        <v>41.19890036398075</v>
-      </c>
-      <c r="H109" t="n">
         <v>63.8522071735304</v>
       </c>
     </row>
@@ -3510,15 +3181,12 @@
         <v>37.36803436279297</v>
       </c>
       <c r="E110" t="n">
-        <v>0.3330000042915344</v>
+        <v>1331.696061964219</v>
       </c>
       <c r="F110" t="n">
-        <v>1331.696061964219</v>
+        <v>61.92235747685517</v>
       </c>
       <c r="G110" t="n">
-        <v>61.92235747685517</v>
-      </c>
-      <c r="H110" t="n">
         <v>61.36237350674613</v>
       </c>
     </row>
@@ -3538,15 +3206,12 @@
         <v>22.64022445678711</v>
       </c>
       <c r="E111" t="n">
-        <v>0.2349999994039536</v>
+        <v>962.8168789726126</v>
       </c>
       <c r="F111" t="n">
-        <v>962.8168789726126</v>
+        <v>31.45102290888001</v>
       </c>
       <c r="G111" t="n">
-        <v>31.45102290888001</v>
-      </c>
-      <c r="H111" t="n">
         <v>60.35999634319712</v>
       </c>
     </row>
@@ -3566,15 +3231,12 @@
         <v>47.97346878051758</v>
       </c>
       <c r="E112" t="n">
-        <v>0.3440000116825104</v>
+        <v>1371.891644524125</v>
       </c>
       <c r="F112" t="n">
-        <v>1371.891644524125</v>
+        <v>80.9535755751856</v>
       </c>
       <c r="G112" t="n">
-        <v>80.9535755751856</v>
-      </c>
-      <c r="H112" t="n">
         <v>56.98629153475792</v>
       </c>
     </row>
@@ -3594,15 +3256,12 @@
         <v>37.54251480102539</v>
       </c>
       <c r="E113" t="n">
-        <v>0.6729999780654907</v>
+        <v>2465.150914639177</v>
       </c>
       <c r="F113" t="n">
-        <v>2465.150914639177</v>
+        <v>61.70862488595789</v>
       </c>
       <c r="G113" t="n">
-        <v>61.70862488595789</v>
-      </c>
-      <c r="H113" t="n">
         <v>59.90456332383156</v>
       </c>
     </row>
@@ -3622,15 +3281,12 @@
         <v>8.218801498413086</v>
       </c>
       <c r="E114" t="n">
-        <v>0.3759999871253967</v>
+        <v>1487.444413390686</v>
       </c>
       <c r="F114" t="n">
-        <v>1487.444413390686</v>
+        <v>8.730330769087979</v>
       </c>
       <c r="G114" t="n">
-        <v>8.730330769087979</v>
-      </c>
-      <c r="H114" t="n">
         <v>52.83404159105811</v>
       </c>
     </row>
@@ -3650,15 +3306,12 @@
         <v>17.36773490905762</v>
       </c>
       <c r="E115" t="n">
-        <v>0.565280020236969</v>
+        <v>2129.778114886851</v>
       </c>
       <c r="F115" t="n">
-        <v>2129.778114886851</v>
+        <v>22.80134452177674</v>
       </c>
       <c r="G115" t="n">
-        <v>22.80134452177674</v>
-      </c>
-      <c r="H115" t="n">
         <v>57.20281900749549</v>
       </c>
     </row>
@@ -3678,15 +3331,12 @@
         <v>27.14417457580566</v>
       </c>
       <c r="E116" t="n">
-        <v>0.2700000107288361</v>
+        <v>1096.787424633644</v>
       </c>
       <c r="F116" t="n">
-        <v>1096.787424633644</v>
+        <v>40.97986187978024</v>
       </c>
       <c r="G116" t="n">
-        <v>40.97986187978024</v>
-      </c>
-      <c r="H116" t="n">
         <v>59.54763194954369</v>
       </c>
     </row>
@@ -3706,15 +3356,12 @@
         <v>2.060366868972778</v>
       </c>
       <c r="E117" t="n">
-        <v>0.2199999988079071</v>
+        <v>904.6427903224928</v>
       </c>
       <c r="F117" t="n">
-        <v>904.6427903224928</v>
+        <v>2.367075362555521</v>
       </c>
       <c r="G117" t="n">
-        <v>2.367075362555521</v>
-      </c>
-      <c r="H117" t="n">
         <v>47.99279308444518</v>
       </c>
     </row>
@@ -3734,15 +3381,12 @@
         <v>40.73994827270508</v>
       </c>
       <c r="E118" t="n">
-        <v>0.06499999761581421</v>
+        <v>277.125303444809</v>
       </c>
       <c r="F118" t="n">
-        <v>277.125303444809</v>
+        <v>66.76651396705567</v>
       </c>
       <c r="G118" t="n">
-        <v>66.76651396705567</v>
-      </c>
-      <c r="H118" t="n">
         <v>56.89182212745664</v>
       </c>
     </row>
@@ -3762,15 +3406,12 @@
         <v>30.27317047119141</v>
       </c>
       <c r="E119" t="n">
-        <v>0.06499999761581421</v>
+        <v>277.125303444809</v>
       </c>
       <c r="F119" t="n">
-        <v>277.125303444809</v>
+        <v>47.77962265205297</v>
       </c>
       <c r="G119" t="n">
-        <v>47.77962265205297</v>
-      </c>
-      <c r="H119" t="n">
         <v>54.84301768980958</v>
       </c>
     </row>
@@ -3790,15 +3431,12 @@
         <v>18.93068313598633</v>
       </c>
       <c r="E120" t="n">
-        <v>0.3070000112056732</v>
+        <v>1235.720342438146</v>
       </c>
       <c r="F120" t="n">
-        <v>1235.720342438146</v>
+        <v>29.25278554792897</v>
       </c>
       <c r="G120" t="n">
-        <v>29.25278554792897</v>
-      </c>
-      <c r="H120" t="n">
         <v>52.0464613686915</v>
       </c>
     </row>
@@ -3818,15 +3456,12 @@
         <v>14.81568145751953</v>
       </c>
       <c r="E121" t="n">
-        <v>0.6050000190734863</v>
+        <v>2255.902501594245</v>
       </c>
       <c r="F121" t="n">
-        <v>2255.902501594245</v>
+        <v>24.34762000956751</v>
       </c>
       <c r="G121" t="n">
-        <v>24.34762000956751</v>
-      </c>
-      <c r="H121" t="n">
         <v>48.81774577195303</v>
       </c>
     </row>
@@ -3846,15 +3481,12 @@
         <v>4.879972457885742</v>
       </c>
       <c r="E122" t="n">
-        <v>0.03996099904179573</v>
+        <v>171.3237639398314</v>
       </c>
       <c r="F122" t="n">
-        <v>171.3237639398314</v>
+        <v>12.27756886738662</v>
       </c>
       <c r="G122" t="n">
-        <v>12.27756886738662</v>
-      </c>
-      <c r="H122" t="n">
         <v>43.38510723073886</v>
       </c>
     </row>
@@ -3874,15 +3506,12 @@
         <v>20.17705154418945</v>
       </c>
       <c r="E123" t="n">
-        <v>0.2220000028610229</v>
+        <v>912.4256141983458</v>
       </c>
       <c r="F123" t="n">
-        <v>912.4256141983458</v>
+        <v>33.62416920162958</v>
       </c>
       <c r="G123" t="n">
-        <v>33.62416920162958</v>
-      </c>
-      <c r="H123" t="n">
         <v>47.78168755695976</v>
       </c>
     </row>
@@ -3902,15 +3531,12 @@
         <v>56.44340133666992</v>
       </c>
       <c r="E124" t="n">
-        <v>0.300000011920929</v>
+        <v>1209.647842624998</v>
       </c>
       <c r="F124" t="n">
-        <v>1209.647842624998</v>
+        <v>87.61477950088891</v>
       </c>
       <c r="G124" t="n">
-        <v>87.61477950088891</v>
-      </c>
-      <c r="H124" t="n">
         <v>45.75468964677962</v>
       </c>
     </row>
@@ -3930,15 +3556,12 @@
         <v>11.0573263168335</v>
       </c>
       <c r="E125" t="n">
-        <v>0.1430000066757202</v>
+        <v>598.8824976040644</v>
       </c>
       <c r="F125" t="n">
-        <v>598.8824976040644</v>
+        <v>22.97464182629868</v>
       </c>
       <c r="G125" t="n">
-        <v>22.97464182629868</v>
-      </c>
-      <c r="H125" t="n">
         <v>42.13516682302727</v>
       </c>
     </row>
@@ -3958,15 +3581,12 @@
         <v>50.16685104370117</v>
       </c>
       <c r="E126" t="n">
-        <v>0.6209999918937683</v>
+        <v>2305.888248308498</v>
       </c>
       <c r="F126" t="n">
-        <v>2305.888248308498</v>
+        <v>78.62070005851318</v>
       </c>
       <c r="G126" t="n">
-        <v>78.62070005851318</v>
-      </c>
-      <c r="H126" t="n">
         <v>46.96057254045356</v>
       </c>
     </row>
@@ -3986,15 +3606,12 @@
         <v>56.4957389831543</v>
       </c>
       <c r="E127" t="n">
-        <v>0.449999988079071</v>
+        <v>1746.861857496495</v>
       </c>
       <c r="F127" t="n">
-        <v>1746.861857496495</v>
+        <v>87.17804013571619</v>
       </c>
       <c r="G127" t="n">
-        <v>87.17804013571619</v>
-      </c>
-      <c r="H127" t="n">
         <v>44.78413662138935</v>
       </c>
     </row>
@@ -4014,15 +3631,12 @@
         <v>15.83572101593018</v>
       </c>
       <c r="E128" t="n">
-        <v>0.4959999918937683</v>
+        <v>1902.710656439457</v>
       </c>
       <c r="F128" t="n">
-        <v>1902.710656439457</v>
+        <v>29.33763480478526</v>
       </c>
       <c r="G128" t="n">
-        <v>29.33763480478526</v>
-      </c>
-      <c r="H128" t="n">
         <v>43.41828545322375</v>
       </c>
     </row>
@@ -4042,15 +3656,12 @@
         <v>47.19518280029297</v>
       </c>
       <c r="E129" t="n">
-        <v>0.1986300051212311</v>
+        <v>820.9795643094412</v>
       </c>
       <c r="F129" t="n">
-        <v>820.9795643094412</v>
+        <v>73.86428573709217</v>
       </c>
       <c r="G129" t="n">
-        <v>73.86428573709217</v>
-      </c>
-      <c r="H129" t="n">
         <v>45.64854529020995</v>
       </c>
     </row>
@@ -4070,15 +3681,12 @@
         <v>35.26229095458984</v>
       </c>
       <c r="E130" t="n">
-        <v>0.4973799884319305</v>
+        <v>1907.322882417562</v>
       </c>
       <c r="F130" t="n">
-        <v>1907.322882417562</v>
+        <v>56.96303155478957</v>
       </c>
       <c r="G130" t="n">
-        <v>56.96303155478957</v>
-      </c>
-      <c r="H130" t="n">
         <v>43.8921473549683</v>
       </c>
     </row>
@@ -4098,15 +3706,12 @@
         <v>39.81490707397461</v>
       </c>
       <c r="E131" t="n">
-        <v>0.5929999947547913</v>
+        <v>2218.105585899384</v>
       </c>
       <c r="F131" t="n">
-        <v>2218.105585899384</v>
+        <v>63.46049227208619</v>
       </c>
       <c r="G131" t="n">
-        <v>63.46049227208619</v>
-      </c>
-      <c r="H131" t="n">
         <v>40.95690199972307</v>
       </c>
     </row>
@@ -4126,15 +3731,12 @@
         <v>49.84615325927734</v>
       </c>
       <c r="E132" t="n">
-        <v>0.04699999839067459</v>
+        <v>201.1884205905175</v>
       </c>
       <c r="F132" t="n">
-        <v>201.1884205905175</v>
+        <v>76.66087340567729</v>
       </c>
       <c r="G132" t="n">
-        <v>76.66087340567729</v>
-      </c>
-      <c r="H132" t="n">
         <v>40.07035923704507</v>
       </c>
     </row>
@@ -4154,15 +3756,12 @@
         <v>40.40338897705078</v>
       </c>
       <c r="E133" t="n">
-        <v>0.239999994635582</v>
+        <v>982.1071720326452</v>
       </c>
       <c r="F133" t="n">
-        <v>982.1071720326452</v>
+        <v>64.40155662759337</v>
       </c>
       <c r="G133" t="n">
-        <v>64.40155662759337</v>
-      </c>
-      <c r="H133" t="n">
         <v>39.12261782369705</v>
       </c>
     </row>
@@ -4182,15 +3781,12 @@
         <v>39.75818634033203</v>
       </c>
       <c r="E134" t="n">
-        <v>0.03299999982118607</v>
+        <v>141.697084695296</v>
       </c>
       <c r="F134" t="n">
-        <v>141.697084695296</v>
+        <v>63.59781706285712</v>
       </c>
       <c r="G134" t="n">
-        <v>63.59781706285712</v>
-      </c>
-      <c r="H134" t="n">
         <v>38.85626839795113</v>
       </c>
     </row>
@@ -4210,15 +3806,12 @@
         <v>7.314035415649414</v>
       </c>
       <c r="E135" t="n">
-        <v>0.2370000034570694</v>
+        <v>970.5390841006508</v>
       </c>
       <c r="F135" t="n">
-        <v>970.5390841006508</v>
+        <v>63.55150843812832</v>
       </c>
       <c r="G135" t="n">
-        <v>63.55150843812832</v>
-      </c>
-      <c r="H135" t="n">
         <v>-33.41099096884161</v>
       </c>
     </row>
@@ -4238,15 +3831,12 @@
         <v>-0.686768651008606</v>
       </c>
       <c r="E136" t="n">
-        <v>0.3409999907016754</v>
+        <v>1360.953256212888</v>
       </c>
       <c r="F136" t="n">
-        <v>1360.953256212888</v>
+        <v>57.05081428995042</v>
       </c>
       <c r="G136" t="n">
-        <v>57.05081428995042</v>
-      </c>
-      <c r="H136" t="n">
         <v>-39.75220781580951</v>
       </c>
     </row>
@@ -4266,15 +3856,12 @@
         <v>-0.6149818301200867</v>
       </c>
       <c r="E137" t="n">
-        <v>0.4950000047683716</v>
+        <v>1899.366209855216</v>
       </c>
       <c r="F137" t="n">
-        <v>1899.366209855216</v>
+        <v>57.75266804044341</v>
       </c>
       <c r="G137" t="n">
-        <v>57.75266804044341</v>
-      </c>
-      <c r="H137" t="n">
         <v>-40.3719759791578</v>
       </c>
     </row>
@@ -4294,15 +3881,12 @@
         <v>-0.06335502862930298</v>
       </c>
       <c r="E138" t="n">
-        <v>0.3619999885559082</v>
+        <v>1437.142271361721</v>
       </c>
       <c r="F138" t="n">
-        <v>1437.142271361721</v>
+        <v>61.31126713700598</v>
       </c>
       <c r="G138" t="n">
-        <v>61.31126713700598</v>
-      </c>
-      <c r="H138" t="n">
         <v>-42.95404180444078</v>
       </c>
     </row>
@@ -4322,15 +3906,12 @@
         <v>24.3468189239502</v>
       </c>
       <c r="E139" t="n">
-        <v>0.5049999952316284</v>
+        <v>1932.724619037558</v>
       </c>
       <c r="F139" t="n">
-        <v>1932.724619037558</v>
+        <v>83.49402123884857</v>
       </c>
       <c r="G139" t="n">
-        <v>83.49402123884857</v>
-      </c>
-      <c r="H139" t="n">
         <v>-26.45310175546729</v>
       </c>
     </row>
@@ -4350,15 +3931,12 @@
         <v>14.86622333526611</v>
       </c>
       <c r="E140" t="n">
-        <v>0.503000020980835</v>
+        <v>1926.068372333629</v>
       </c>
       <c r="F140" t="n">
-        <v>1926.068372333629</v>
+        <v>88.84708373928603</v>
       </c>
       <c r="G140" t="n">
-        <v>88.84708373928603</v>
-      </c>
-      <c r="H140" t="n">
         <v>-41.04000458576156</v>
       </c>
     </row>
@@ -4378,15 +3956,12 @@
         <v>14.75438690185547</v>
       </c>
       <c r="E141" t="n">
-        <v>0.164000004529953</v>
+        <v>683.4515571949081</v>
       </c>
       <c r="F141" t="n">
-        <v>683.4515571949081</v>
+        <v>90.52923262707655</v>
       </c>
       <c r="G141" t="n">
-        <v>90.52923262707655</v>
-      </c>
-      <c r="H141" t="n">
         <v>-41.90635784661719</v>
       </c>
     </row>
@@ -4406,15 +3981,12 @@
         <v>34.60570907592773</v>
       </c>
       <c r="E142" t="n">
-        <v>0.09799999743700027</v>
+        <v>414.7121310817099</v>
       </c>
       <c r="F142" t="n">
-        <v>414.7121310817099</v>
+        <v>102.902685252486</v>
       </c>
       <c r="G142" t="n">
-        <v>102.902685252486</v>
-      </c>
-      <c r="H142" t="n">
         <v>-24.78935319679015</v>
       </c>
     </row>
@@ -4434,15 +4006,12 @@
         <v>21.39655303955078</v>
       </c>
       <c r="E143" t="n">
-        <v>0.2910000085830688</v>
+        <v>1175.980668839187</v>
       </c>
       <c r="F143" t="n">
-        <v>1175.980668839187</v>
+        <v>101.2521659165168</v>
       </c>
       <c r="G143" t="n">
-        <v>101.2521659165168</v>
-      </c>
-      <c r="H143" t="n">
         <v>-38.40568155886272</v>
       </c>
     </row>
@@ -4462,15 +4031,12 @@
         <v>34.65128707885742</v>
       </c>
       <c r="E144" t="n">
-        <v>0.3659999966621399</v>
+        <v>1451.554321387228</v>
       </c>
       <c r="F144" t="n">
-        <v>1451.554321387228</v>
+        <v>107.4255305496436</v>
       </c>
       <c r="G144" t="n">
-        <v>107.4255305496436</v>
-      </c>
-      <c r="H144" t="n">
         <v>-26.16964491264739</v>
       </c>
     </row>
@@ -4490,15 +4056,12 @@
         <v>7.084443092346191</v>
       </c>
       <c r="E145" t="n">
-        <v>0.1720000058412552</v>
+        <v>715.4362988699944</v>
       </c>
       <c r="F145" t="n">
-        <v>715.4362988699944</v>
+        <v>95.99098400006483</v>
       </c>
       <c r="G145" t="n">
-        <v>95.99098400006483</v>
-      </c>
-      <c r="H145" t="n">
         <v>-52.36756608842526</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Filtered out sources that were in the Segue Footprint
</commit_message>
<xml_diff>
--- a/cel_obj_table.xlsx
+++ b/cel_obj_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G145"/>
+  <dimension ref="A1:G122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,3602 +467,3027 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>3</v>
+        <v>88</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>b'3FHL J0018.6+2946 '</t>
+          <t>b'3FHL J0648.7+1517 '</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>4.652533054351807</v>
+        <v>102.1869277954102</v>
       </c>
       <c r="D2" t="n">
-        <v>29.78214263916016</v>
+        <v>15.28416442871094</v>
       </c>
       <c r="E2" t="n">
-        <v>422.9823619420345</v>
+        <v>743.3176422661688</v>
       </c>
       <c r="F2" t="n">
-        <v>114.4798012587622</v>
+        <v>198.9723667223909</v>
       </c>
       <c r="G2" t="n">
-        <v>-32.5502715975377</v>
+        <v>6.322407808255858</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>5</v>
+        <v>96</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>b'3FHL J0037.8+1239 '</t>
+          <t>b'3FHL J0730.4+3307 '</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>9.461506843566895</v>
+        <v>112.6081008911133</v>
       </c>
       <c r="D3" t="n">
-        <v>12.65117645263672</v>
+        <v>33.12022399902344</v>
       </c>
       <c r="E3" t="n">
-        <v>377.3991422199498</v>
+        <v>472.4384783695589</v>
       </c>
       <c r="F3" t="n">
-        <v>117.760924150212</v>
+        <v>185.874446883025</v>
       </c>
       <c r="G3" t="n">
-        <v>-50.08405705910805</v>
+        <v>22.04667824967751</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>12</v>
+        <v>97</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>b'3FHL J0109.1+1817 '</t>
+          <t>b'3FHL J0738.1+1742 '</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17.29154396057129</v>
+        <v>114.5327682495117</v>
       </c>
       <c r="D4" t="n">
-        <v>18.2844295501709</v>
+        <v>17.71304893493652</v>
       </c>
       <c r="E4" t="n">
-        <v>1722.784654514631</v>
+        <v>1656.947604950266</v>
       </c>
       <c r="F4" t="n">
-        <v>128.8249263315673</v>
+        <v>201.8397573898806</v>
       </c>
       <c r="G4" t="n">
-        <v>-44.38437320754328</v>
+        <v>18.07539141955594</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>b'3FHL J0112.1+2245 '</t>
+          <t>b'3FHL J0753.1+5354 '</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>18.03292655944824</v>
+        <v>118.2864151000977</v>
       </c>
       <c r="D5" t="n">
-        <v>22.75535202026367</v>
+        <v>53.90745544433594</v>
       </c>
       <c r="E5" t="n">
-        <v>1077.800369873403</v>
+        <v>826.3707136061979</v>
       </c>
       <c r="F5" t="n">
-        <v>129.1513327682703</v>
+        <v>164.1736930995773</v>
       </c>
       <c r="G5" t="n">
-        <v>-39.86636396877911</v>
+        <v>30.52602863281245</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>17</v>
+        <v>101</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>b'3FHL J0114.8+1324 '</t>
+          <t>b'3FHL J0754.8+4822 '</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>18.70676612854004</v>
+        <v>118.7094268798828</v>
       </c>
       <c r="D6" t="n">
-        <v>13.4044361114502</v>
+        <v>48.38185119628906</v>
       </c>
       <c r="E6" t="n">
-        <v>2186.405655380971</v>
+        <v>1489.98505775128</v>
       </c>
       <c r="F6" t="n">
-        <v>131.6327174089689</v>
+        <v>170.5698825442753</v>
       </c>
       <c r="G6" t="n">
-        <v>-49.07177578318304</v>
+        <v>30.15412007607718</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>18</v>
+        <v>102</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>b'3FHL J0115.8+2519 '</t>
+          <t>b'3FHL J0757.1+0957 '</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>18.95399475097656</v>
+        <v>119.2889862060547</v>
       </c>
       <c r="D7" t="n">
-        <v>25.32852172851562</v>
+        <v>9.965688705444336</v>
       </c>
       <c r="E7" t="n">
-        <v>1422.698307198181</v>
+        <v>1081.60187099801</v>
       </c>
       <c r="F7" t="n">
-        <v>129.8529186114632</v>
+        <v>211.2949664982855</v>
       </c>
       <c r="G7" t="n">
-        <v>-37.21540373185186</v>
+        <v>19.07671444842579</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>25</v>
+        <v>105</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>b'3FHL J0151.0+0539 '</t>
+          <t>b'3FHL J0809.7+3457 '</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>27.75368118286133</v>
+        <v>122.4298248291016</v>
       </c>
       <c r="D8" t="n">
-        <v>5.654636383056641</v>
+        <v>34.95800018310547</v>
       </c>
       <c r="E8" t="n">
-        <v>1209.647842624998</v>
+        <v>352.4357721162331</v>
       </c>
       <c r="F8" t="n">
-        <v>148.8556672614539</v>
+        <v>186.4471419042782</v>
       </c>
       <c r="G8" t="n">
-        <v>-54.19102061088856</v>
+        <v>30.37076642512884</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>26</v>
+        <v>106</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>b'3FHL J0152.6+0147 '</t>
+          <t>b'3FHL J0809.8+5218 '</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>28.17214775085449</v>
+        <v>122.4586029052734</v>
       </c>
       <c r="D9" t="n">
-        <v>1.785664200782776</v>
+        <v>52.31039428710938</v>
       </c>
       <c r="E9" t="n">
-        <v>339.927766599597</v>
+        <v>578.6172947152628</v>
       </c>
       <c r="F9" t="n">
-        <v>152.3914027711392</v>
+        <v>166.2520819406516</v>
       </c>
       <c r="G9" t="n">
-        <v>-57.54007559780352</v>
+        <v>32.91232473625846</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>28</v>
+        <v>109</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>b'3FHL J0154.0+0823 '</t>
+          <t>b'3FHL J0816.4+5739 '</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>28.50320816040039</v>
+        <v>124.1090469360352</v>
       </c>
       <c r="D10" t="n">
-        <v>8.389946937561035</v>
+        <v>57.66443634033203</v>
       </c>
       <c r="E10" t="n">
-        <v>2489.225587653121</v>
+        <v>230.7935158149133</v>
       </c>
       <c r="F10" t="n">
-        <v>148.2359504042424</v>
+        <v>159.8473262299431</v>
       </c>
       <c r="G10" t="n">
-        <v>-51.38123321650065</v>
+        <v>33.90405576615215</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>38</v>
+        <v>110</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>b'3FHL J0227.3+0200 '</t>
+          <t>b'3FHL J0816.9+2050 '</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>36.82808685302734</v>
+        <v>124.2364349365234</v>
       </c>
       <c r="D11" t="n">
-        <v>2.002652168273926</v>
+        <v>20.84729194641113</v>
       </c>
       <c r="E11" t="n">
-        <v>1770.843252129352</v>
+        <v>247.6684183724716</v>
       </c>
       <c r="F11" t="n">
-        <v>165.1466930350609</v>
+        <v>202.4247601227709</v>
       </c>
       <c r="G11" t="n">
-        <v>-52.82668089433401</v>
+        <v>27.73866668831735</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>43</v>
+        <v>111</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>b'3FHL J0242.7-0002 '</t>
+          <t>b'3FHL J0818.2+4222 '</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>40.67588806152344</v>
+        <v>124.5621643066406</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.04313698038458824</v>
+        <v>42.37668228149414</v>
       </c>
       <c r="E12" t="n">
-        <v>12.96591135664807</v>
+        <v>2015.283911619772</v>
       </c>
       <c r="F12" t="n">
-        <v>172.1438214764061</v>
+        <v>178.2303101447942</v>
       </c>
       <c r="G12" t="n">
-        <v>-51.95162955648622</v>
+        <v>33.39832911945414</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>46</v>
+        <v>112</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>b'3FHL J0256.4+0334 '</t>
+          <t>b'3FHL J0820.9+2353 '</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>44.10073852539062</v>
+        <v>125.2343978881836</v>
       </c>
       <c r="D13" t="n">
-        <v>3.57359504699707</v>
+        <v>23.89204978942871</v>
       </c>
       <c r="E13" t="n">
-        <v>1572.767471022466</v>
+        <v>1579.826051622189</v>
       </c>
       <c r="F13" t="n">
-        <v>172.2738268268965</v>
+        <v>199.510479607579</v>
       </c>
       <c r="G13" t="n">
-        <v>-46.9728540251021</v>
+        <v>29.63265514420423</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>b'3FHL J0648.7+1517 '</t>
+          <t>b'3FHL J0825.7+0311 '</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>102.1869277954102</v>
+        <v>126.4462661743164</v>
       </c>
       <c r="D14" t="n">
-        <v>15.28416442871094</v>
+        <v>3.194593906402588</v>
       </c>
       <c r="E14" t="n">
-        <v>743.3176422661688</v>
+        <v>1936.049867434469</v>
       </c>
       <c r="F14" t="n">
-        <v>198.9723667223909</v>
+        <v>221.1759682227195</v>
       </c>
       <c r="G14" t="n">
-        <v>6.322407808255858</v>
+        <v>22.39409690992864</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>b'3FHL J0730.4+3307 '</t>
+          <t>b'3FHL J0828.3+4153 '</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>112.6081008911133</v>
+        <v>127.0883941650391</v>
       </c>
       <c r="D15" t="n">
-        <v>33.12022399902344</v>
+        <v>41.89826965332031</v>
       </c>
       <c r="E15" t="n">
-        <v>472.4384783695589</v>
+        <v>927.9669661452913</v>
       </c>
       <c r="F15" t="n">
-        <v>185.874446883025</v>
+        <v>179.0932631579409</v>
       </c>
       <c r="G15" t="n">
-        <v>22.04667824967751</v>
+        <v>35.19544797408459</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>b'3FHL J0738.1+1742 '</t>
+          <t>b'3FHL J0831.8+0429 '</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>114.5327682495117</v>
+        <v>127.9610137939453</v>
       </c>
       <c r="D16" t="n">
-        <v>17.71304893493652</v>
+        <v>4.495641231536865</v>
       </c>
       <c r="E16" t="n">
-        <v>1656.947604950266</v>
+        <v>723.4123895726626</v>
       </c>
       <c r="F16" t="n">
-        <v>201.8397573898806</v>
+        <v>220.6957511158911</v>
       </c>
       <c r="G16" t="n">
-        <v>18.07539141955594</v>
+        <v>24.338949894984</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>b'3FHL J0753.1+5354 '</t>
+          <t>b'3FHL J0847.2+1134 '</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>118.2864151000977</v>
+        <v>131.8077850341797</v>
       </c>
       <c r="D17" t="n">
-        <v>53.90745544433594</v>
+        <v>11.56671619415283</v>
       </c>
       <c r="E17" t="n">
-        <v>826.3707136061979</v>
+        <v>822.4359267571556</v>
       </c>
       <c r="F17" t="n">
-        <v>164.1736930995773</v>
+        <v>215.4547936858709</v>
       </c>
       <c r="G17" t="n">
-        <v>30.52602863281245</v>
+        <v>30.89410316823072</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>b'3FHL J0754.8+4822 '</t>
+          <t>b'3FHL J0849.9+5108 '</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>118.7094268798828</v>
+        <v>132.4937896728516</v>
       </c>
       <c r="D18" t="n">
-        <v>48.38185119628906</v>
+        <v>51.141845703125</v>
       </c>
       <c r="E18" t="n">
-        <v>1489.98505775128</v>
+        <v>2186.405655380971</v>
       </c>
       <c r="F18" t="n">
-        <v>170.5698825442753</v>
+        <v>167.6055794666185</v>
       </c>
       <c r="G18" t="n">
-        <v>30.15412007607718</v>
+        <v>39.1364989957745</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>b'3FHL J0757.1+0957 '</t>
+          <t>b'3FHL J0850.6+3454 '</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>119.2889862060547</v>
+        <v>132.6519165039062</v>
       </c>
       <c r="D19" t="n">
-        <v>9.965688705444336</v>
+        <v>34.90697479248047</v>
       </c>
       <c r="E19" t="n">
-        <v>1081.60187099801</v>
+        <v>606.9745772102617</v>
       </c>
       <c r="F19" t="n">
-        <v>211.2949664982855</v>
+        <v>188.4881336399034</v>
       </c>
       <c r="G19" t="n">
-        <v>19.07671444842579</v>
+        <v>38.57761892185869</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>b'3FHL J0809.7+3457 '</t>
+          <t>b'3FHL J0854.8+2006 '</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>122.4298248291016</v>
+        <v>133.7121429443359</v>
       </c>
       <c r="D20" t="n">
-        <v>34.95800018310547</v>
+        <v>20.10042953491211</v>
       </c>
       <c r="E20" t="n">
-        <v>352.4357721162331</v>
+        <v>1232.001690836247</v>
       </c>
       <c r="F20" t="n">
-        <v>186.4471419042782</v>
+        <v>206.8248045598298</v>
       </c>
       <c r="G20" t="n">
-        <v>30.37076642512884</v>
+        <v>35.82570420018077</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>b'3FHL J0809.8+5218 '</t>
+          <t>b'3FHL J0908.9+2311 '</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>122.4586029052734</v>
+        <v>137.2379302978516</v>
       </c>
       <c r="D21" t="n">
-        <v>52.31039428710938</v>
+        <v>23.19077682495117</v>
       </c>
       <c r="E21" t="n">
-        <v>578.6172947152628</v>
+        <v>916.3139966249578</v>
       </c>
       <c r="F21" t="n">
-        <v>166.2520819406516</v>
+        <v>204.4006996128279</v>
       </c>
       <c r="G21" t="n">
-        <v>32.91232473625846</v>
+        <v>39.90343163897078</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>b'3FHL J0816.4+5739 '</t>
+          <t>b'3FHL J0910.5+3329 '</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>124.1090469360352</v>
+        <v>137.62841796875</v>
       </c>
       <c r="D22" t="n">
-        <v>57.66443634033203</v>
+        <v>33.48870086669922</v>
       </c>
       <c r="E22" t="n">
-        <v>230.7935158149133</v>
+        <v>1408.222189015081</v>
       </c>
       <c r="F22" t="n">
-        <v>159.8473262299431</v>
+        <v>191.1184013879268</v>
       </c>
       <c r="G22" t="n">
-        <v>33.90405576615215</v>
+        <v>42.44470192240891</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>b'3FHL J0816.9+2050 '</t>
+          <t>b'3FHL J0912.4+1555 '</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>124.2364349365234</v>
+        <v>138.1239929199219</v>
       </c>
       <c r="D23" t="n">
-        <v>20.84729194641113</v>
+        <v>15.9302806854248</v>
       </c>
       <c r="E23" t="n">
-        <v>247.6684183724716</v>
+        <v>873.4307914196993</v>
       </c>
       <c r="F23" t="n">
-        <v>202.4247601227709</v>
+        <v>213.5799215954228</v>
       </c>
       <c r="G23" t="n">
-        <v>27.73866668831735</v>
+        <v>38.26181930326724</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>b'3FHL J0818.2+4222 '</t>
+          <t>b'3FHL J0930.4+4952 '</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>124.5621643066406</v>
+        <v>142.6244659423828</v>
       </c>
       <c r="D24" t="n">
-        <v>42.37668228149414</v>
+        <v>49.87545776367188</v>
       </c>
       <c r="E24" t="n">
-        <v>2015.283911619772</v>
+        <v>775.0615269997014</v>
       </c>
       <c r="F24" t="n">
-        <v>178.2303101447942</v>
+        <v>168.0950099107559</v>
       </c>
       <c r="G24" t="n">
-        <v>33.39832911945414</v>
+        <v>45.68697248424435</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>b'3FHL J0820.9+2353 '</t>
+          <t>b'3FHL J0940.5+6149 '</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>125.2343978881836</v>
+        <v>145.1408081054688</v>
       </c>
       <c r="D25" t="n">
-        <v>23.89204978942871</v>
+        <v>61.8179817199707</v>
       </c>
       <c r="E25" t="n">
-        <v>1579.826051622189</v>
+        <v>869.5202016942904</v>
       </c>
       <c r="F25" t="n">
-        <v>199.510479607579</v>
+        <v>151.5795904696888</v>
       </c>
       <c r="G25" t="n">
-        <v>29.63265514420423</v>
+        <v>43.2124825532333</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>113</v>
+        <v>130</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>b'3FHL J0825.7+0311 '</t>
+          <t>b'3FHL J0946.2+0104 '</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>126.4462661743164</v>
+        <v>146.5630645751953</v>
       </c>
       <c r="D26" t="n">
-        <v>3.194593906402588</v>
+        <v>1.072644710540771</v>
       </c>
       <c r="E26" t="n">
-        <v>1936.049867434469</v>
+        <v>2167.296925661129</v>
       </c>
       <c r="F26" t="n">
-        <v>221.1759682227195</v>
+        <v>235.3603953607503</v>
       </c>
       <c r="G26" t="n">
-        <v>22.39409690992864</v>
+        <v>38.56086142877915</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>114</v>
+        <v>131</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>b'3FHL J0828.3+4153 '</t>
+          <t>b'3FHL J0950.3+4553 '</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>127.0883941650391</v>
+        <v>147.5764617919922</v>
       </c>
       <c r="D27" t="n">
-        <v>41.89826965332031</v>
+        <v>45.89204025268555</v>
       </c>
       <c r="E27" t="n">
-        <v>927.9669661452913</v>
+        <v>1569.235152018134</v>
       </c>
       <c r="F27" t="n">
-        <v>179.0932631579409</v>
+        <v>172.8821816193272</v>
       </c>
       <c r="G27" t="n">
-        <v>35.19544797408459</v>
+        <v>49.75183136937554</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>b'3FHL J0831.8+0429 '</t>
+          <t>b'3FHL J0954.2+4912 '</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>127.9610137939453</v>
+        <v>148.5668640136719</v>
       </c>
       <c r="D28" t="n">
-        <v>4.495641231536865</v>
+        <v>49.21414566040039</v>
       </c>
       <c r="E28" t="n">
-        <v>723.4123895726626</v>
+        <v>1501.744593228529</v>
       </c>
       <c r="F28" t="n">
-        <v>220.6957511158911</v>
+        <v>167.6515683277358</v>
       </c>
       <c r="G28" t="n">
-        <v>24.338949894984</v>
+        <v>49.58651425014828</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>b'3FHL J0847.2+1134 '</t>
+          <t>b'3FHL J1001.2+2910 '</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>131.8077850341797</v>
+        <v>150.3133544921875</v>
       </c>
       <c r="D29" t="n">
-        <v>11.56671619415283</v>
+        <v>29.1705379486084</v>
       </c>
       <c r="E29" t="n">
-        <v>822.4359267571556</v>
+        <v>2106.343909760358</v>
       </c>
       <c r="F29" t="n">
-        <v>215.4547936858709</v>
+        <v>199.5504344044182</v>
       </c>
       <c r="G29" t="n">
-        <v>30.89410316823072</v>
+        <v>52.63416273614697</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>118</v>
+        <v>137</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>b'3FHL J0849.9+5108 '</t>
+          <t>b'3FHL J1006.9+3455 '</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>132.4937896728516</v>
+        <v>151.7499389648438</v>
       </c>
       <c r="D30" t="n">
-        <v>51.141845703125</v>
+        <v>34.92112350463867</v>
       </c>
       <c r="E30" t="n">
-        <v>2186.405655380971</v>
+        <v>2277.828672355331</v>
       </c>
       <c r="F30" t="n">
-        <v>167.6055794666185</v>
+        <v>190.0282006580422</v>
       </c>
       <c r="G30" t="n">
-        <v>39.1364989957745</v>
+        <v>54.17913076411402</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>b'3FHL J0850.6+3454 '</t>
+          <t>b'3FHL J1008.0+0622 '</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>132.6519165039062</v>
+        <v>152.0041351318359</v>
       </c>
       <c r="D31" t="n">
-        <v>34.90697479248047</v>
+        <v>6.373631954193115</v>
       </c>
       <c r="E31" t="n">
-        <v>606.9745772102617</v>
+        <v>2395.304963072071</v>
       </c>
       <c r="F31" t="n">
-        <v>188.4881336399034</v>
+        <v>233.50096097581</v>
       </c>
       <c r="G31" t="n">
-        <v>38.57761892185869</v>
+        <v>46.02256622120216</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>b'3FHL J0854.8+2006 '</t>
+          <t>b'3FHL J1012.6+4228 '</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>133.7121429443359</v>
+        <v>153.1730499267578</v>
       </c>
       <c r="D32" t="n">
-        <v>20.10042953491211</v>
+        <v>42.48298263549805</v>
       </c>
       <c r="E32" t="n">
-        <v>1232.001690836247</v>
+        <v>1447.954363211065</v>
       </c>
       <c r="F32" t="n">
-        <v>206.8248045598298</v>
+        <v>176.9216254086938</v>
       </c>
       <c r="G32" t="n">
-        <v>35.82570420018077</v>
+        <v>54.39503658450563</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>122</v>
+        <v>141</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>b'3FHL J0908.9+2311 '</t>
+          <t>b'3FHL J1015.0+4926 '</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>137.2379302978516</v>
+        <v>153.7693176269531</v>
       </c>
       <c r="D33" t="n">
-        <v>23.19077682495117</v>
+        <v>49.43538665771484</v>
       </c>
       <c r="E33" t="n">
-        <v>916.3139966249578</v>
+        <v>873.4307914196993</v>
       </c>
       <c r="F33" t="n">
-        <v>204.4006996128279</v>
+        <v>165.5301745409713</v>
       </c>
       <c r="G33" t="n">
-        <v>39.90343163897078</v>
+        <v>52.7128041733207</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>123</v>
+        <v>142</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>b'3FHL J0910.5+3329 '</t>
+          <t>b'3FHL J1026.9+0608 '</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>137.62841796875</v>
+        <v>156.7403564453125</v>
       </c>
       <c r="D34" t="n">
-        <v>33.48870086669922</v>
+        <v>6.142007350921631</v>
       </c>
       <c r="E34" t="n">
-        <v>1408.222189015081</v>
+        <v>1743.428171899722</v>
       </c>
       <c r="F34" t="n">
-        <v>191.1184013879268</v>
+        <v>237.7476753956505</v>
       </c>
       <c r="G34" t="n">
-        <v>42.44470192240891</v>
+        <v>49.78141165294394</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>b'3FHL J0912.4+1555 '</t>
+          <t>b'3FHL J1027.5+6317 '</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>138.1239929199219</v>
+        <v>156.8891754150391</v>
       </c>
       <c r="D35" t="n">
-        <v>15.9302806854248</v>
+        <v>63.29279327392578</v>
       </c>
       <c r="E35" t="n">
-        <v>873.4307914196993</v>
+        <v>2183.225532378438</v>
       </c>
       <c r="F35" t="n">
-        <v>213.5799215954228</v>
+        <v>145.6929541877977</v>
       </c>
       <c r="G35" t="n">
-        <v>38.26181930326724</v>
+        <v>46.97503063890456</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>b'3FHL J0930.4+4952 '</t>
+          <t>b'3FHL J1031.3+5053 '</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>142.6244659423828</v>
+        <v>157.8328399658203</v>
       </c>
       <c r="D36" t="n">
-        <v>49.87545776367188</v>
+        <v>50.88592529296875</v>
       </c>
       <c r="E36" t="n">
-        <v>775.0615269997014</v>
+        <v>1433.534310193219</v>
       </c>
       <c r="F36" t="n">
-        <v>168.0950099107559</v>
+        <v>161.4466616146051</v>
       </c>
       <c r="G36" t="n">
-        <v>45.68697248424435</v>
+        <v>54.44603636948661</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>b'3FHL J0940.5+6149 '</t>
+          <t>b'3FHL J1032.7+3737 '</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>145.1408081054688</v>
+        <v>158.1970977783203</v>
       </c>
       <c r="D37" t="n">
-        <v>61.8179817199707</v>
+        <v>37.62113952636719</v>
       </c>
       <c r="E37" t="n">
-        <v>869.5202016942904</v>
+        <v>2008.723036449022</v>
       </c>
       <c r="F37" t="n">
-        <v>151.5795904696888</v>
+        <v>184.2725657102087</v>
       </c>
       <c r="G37" t="n">
-        <v>43.2124825532333</v>
+        <v>59.11119534742926</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>130</v>
+        <v>148</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>b'3FHL J0946.2+0104 '</t>
+          <t>b'3FHL J1041.7+3900 '</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>146.5630645751953</v>
+        <v>160.4421539306641</v>
       </c>
       <c r="D38" t="n">
-        <v>1.072644710540771</v>
+        <v>39.00973129272461</v>
       </c>
       <c r="E38" t="n">
-        <v>2167.296925661129</v>
+        <v>865.6075942787213</v>
       </c>
       <c r="F38" t="n">
-        <v>235.3603953607503</v>
+        <v>180.851954975237</v>
       </c>
       <c r="G38" t="n">
-        <v>38.56086142877915</v>
+        <v>60.55262642715537</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>b'3FHL J0950.3+4553 '</t>
+          <t>b'3FHL J1043.1+2409 '</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>147.5764617919922</v>
+        <v>160.7764892578125</v>
       </c>
       <c r="D39" t="n">
-        <v>45.89204025268555</v>
+        <v>24.15542984008789</v>
       </c>
       <c r="E39" t="n">
-        <v>1569.235152018134</v>
+        <v>2112.791679272088</v>
       </c>
       <c r="F39" t="n">
-        <v>172.8821816193272</v>
+        <v>211.5515502940325</v>
       </c>
       <c r="G39" t="n">
-        <v>49.75183136937554</v>
+        <v>61.00195275957411</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>133</v>
+        <v>150</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>b'3FHL J0954.2+4912 '</t>
+          <t>b'3FHL J1051.4+3942 '</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>148.5668640136719</v>
+        <v>162.8575439453125</v>
       </c>
       <c r="D40" t="n">
-        <v>49.21414566040039</v>
+        <v>39.70672988891602</v>
       </c>
       <c r="E40" t="n">
-        <v>1501.744593228529</v>
+        <v>1909.393880329576</v>
       </c>
       <c r="F40" t="n">
-        <v>167.6515683277358</v>
+        <v>178.3920516037439</v>
       </c>
       <c r="G40" t="n">
-        <v>49.58651425014828</v>
+        <v>62.16010539961907</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>135</v>
+        <v>151</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>b'3FHL J1001.2+2910 '</t>
+          <t>b'3FHL J1053.6+4930 '</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>150.3133544921875</v>
+        <v>163.4012298583984</v>
       </c>
       <c r="D41" t="n">
-        <v>29.1705379486084</v>
+        <v>49.50532150268555</v>
       </c>
       <c r="E41" t="n">
-        <v>2106.343909760358</v>
+        <v>586.7293479424766</v>
       </c>
       <c r="F41" t="n">
-        <v>199.5504344044182</v>
+        <v>160.2472928171692</v>
       </c>
       <c r="G41" t="n">
-        <v>52.63416273614697</v>
+        <v>58.20941647675482</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>b'3FHL J1006.9+3455 '</t>
+          <t>b'3FHL J1058.6+5628 '</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>151.7499389648438</v>
+        <v>164.6645202636719</v>
       </c>
       <c r="D42" t="n">
-        <v>34.92112350463867</v>
+        <v>56.46826171875</v>
       </c>
       <c r="E42" t="n">
-        <v>2277.828672355331</v>
+        <v>598.8824976040644</v>
       </c>
       <c r="F42" t="n">
-        <v>190.0282006580422</v>
+        <v>149.5898498865417</v>
       </c>
       <c r="G42" t="n">
-        <v>54.17913076411402</v>
+        <v>54.42879075775696</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>138</v>
+        <v>155</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>b'3FHL J1008.0+0622 '</t>
+          <t>b'3FHL J1100.3+4020 '</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>152.0041351318359</v>
+        <v>165.0803070068359</v>
       </c>
       <c r="D43" t="n">
-        <v>6.373631954193115</v>
+        <v>40.3358268737793</v>
       </c>
       <c r="E43" t="n">
-        <v>2395.304963072071</v>
+        <v>924.0846438011745</v>
       </c>
       <c r="F43" t="n">
-        <v>233.50096097581</v>
+        <v>175.8469476326254</v>
       </c>
       <c r="G43" t="n">
-        <v>46.02256622120216</v>
+        <v>63.555059895797</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>140</v>
+        <v>157</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>b'3FHL J1012.6+4228 '</t>
+          <t>b'3FHL J1104.4+3812 '</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>153.1730499267578</v>
+        <v>166.1207580566406</v>
       </c>
       <c r="D44" t="n">
-        <v>42.48298263549805</v>
+        <v>38.20518112182617</v>
       </c>
       <c r="E44" t="n">
-        <v>1447.954363211065</v>
+        <v>128.9003855881938</v>
       </c>
       <c r="F44" t="n">
-        <v>176.9216254086938</v>
+        <v>179.8357877680561</v>
       </c>
       <c r="G44" t="n">
-        <v>54.39503658450563</v>
+        <v>65.03781332953814</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>141</v>
+        <v>158</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>b'3FHL J1015.0+4926 '</t>
+          <t>b'3FHL J1105.8+3944 '</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>153.7693176269531</v>
+        <v>166.4540252685547</v>
       </c>
       <c r="D45" t="n">
-        <v>49.43538665771484</v>
+        <v>39.74899673461914</v>
       </c>
       <c r="E45" t="n">
-        <v>873.4307914196993</v>
+        <v>418.8482280609101</v>
       </c>
       <c r="F45" t="n">
-        <v>165.5301745409713</v>
+        <v>176.2092588270897</v>
       </c>
       <c r="G45" t="n">
-        <v>52.7128041733207</v>
+        <v>64.74895803570412</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>142</v>
+        <v>159</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>b'3FHL J1026.9+0608 '</t>
+          <t>b'3FHL J1107.8+1501 '</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>156.7403564453125</v>
+        <v>166.9655914306641</v>
       </c>
       <c r="D46" t="n">
-        <v>6.142007350921631</v>
+        <v>15.02733516693115</v>
       </c>
       <c r="E46" t="n">
-        <v>1743.428171899722</v>
+        <v>2240.185974418625</v>
       </c>
       <c r="F46" t="n">
-        <v>237.7476753956505</v>
+        <v>234.34727958246</v>
       </c>
       <c r="G46" t="n">
-        <v>49.78141165294394</v>
+        <v>63.06038848548737</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>144</v>
+        <v>160</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>b'3FHL J1027.5+6317 '</t>
+          <t>b'3FHL J1109.7+3735 '</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>156.8891754150391</v>
+        <v>167.4311370849609</v>
       </c>
       <c r="D47" t="n">
-        <v>63.29279327392578</v>
+        <v>37.58807754516602</v>
       </c>
       <c r="E47" t="n">
-        <v>2183.225532378438</v>
+        <v>1563.657198577747</v>
       </c>
       <c r="F47" t="n">
-        <v>145.6929541877977</v>
+        <v>180.457347654663</v>
       </c>
       <c r="G47" t="n">
-        <v>46.97503063890456</v>
+        <v>66.2143548292574</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>146</v>
+        <v>161</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>b'3FHL J1031.3+5053 '</t>
+          <t>b'3FHL J1117.0+2014 '</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>157.8328399658203</v>
+        <v>169.2679595947266</v>
       </c>
       <c r="D48" t="n">
-        <v>50.88592529296875</v>
+        <v>20.23810386657715</v>
       </c>
       <c r="E48" t="n">
-        <v>1433.534310193219</v>
+        <v>578.6172947152628</v>
       </c>
       <c r="F48" t="n">
-        <v>161.4466616146051</v>
+        <v>225.5716267064807</v>
       </c>
       <c r="G48" t="n">
-        <v>54.44603636948661</v>
+        <v>67.36670331755562</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>147</v>
+        <v>163</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>b'3FHL J1032.7+3737 '</t>
+          <t>b'3FHL J1120.8+4212 '</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>158.1970977783203</v>
+        <v>170.2008819580078</v>
       </c>
       <c r="D49" t="n">
-        <v>37.62113952636719</v>
+        <v>42.20166015625</v>
       </c>
       <c r="E49" t="n">
-        <v>2008.723036449022</v>
+        <v>521.6104982541038</v>
       </c>
       <c r="F49" t="n">
-        <v>184.2725657102087</v>
+        <v>167.856902782118</v>
       </c>
       <c r="G49" t="n">
-        <v>59.11119534742926</v>
+        <v>66.16418823817627</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>148</v>
+        <v>166</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>b'3FHL J1041.7+3900 '</t>
+          <t>b'3FHL J1131.6+5809 '</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>160.4421539306641</v>
+        <v>172.9062042236328</v>
       </c>
       <c r="D50" t="n">
-        <v>39.00973129272461</v>
+        <v>58.16561508178711</v>
       </c>
       <c r="E50" t="n">
-        <v>865.6075942787213</v>
+        <v>1429.924347323077</v>
       </c>
       <c r="F50" t="n">
-        <v>180.851954975237</v>
+        <v>141.6893921444634</v>
       </c>
       <c r="G50" t="n">
-        <v>60.55262642715537</v>
+        <v>55.9604528362288</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>b'3FHL J1043.1+2409 '</t>
+          <t>b'3FHL J1136.8+2549 '</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>160.7764892578125</v>
+        <v>174.2185363769531</v>
       </c>
       <c r="D51" t="n">
-        <v>24.15542984008789</v>
+        <v>25.8327808380127</v>
       </c>
       <c r="E51" t="n">
-        <v>2112.791679272088</v>
+        <v>651.3386580792431</v>
       </c>
       <c r="F51" t="n">
-        <v>211.5515502940325</v>
+        <v>213.1465867327724</v>
       </c>
       <c r="G51" t="n">
-        <v>61.00195275957411</v>
+        <v>73.27986298713279</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>150</v>
+        <v>171</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>b'3FHL J1051.4+3942 '</t>
+          <t>b'3FHL J1140.5+1528 '</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>162.8575439453125</v>
+        <v>175.1320648193359</v>
       </c>
       <c r="D52" t="n">
-        <v>39.70672988891602</v>
+        <v>15.48001480102539</v>
       </c>
       <c r="E52" t="n">
-        <v>1909.393880329576</v>
+        <v>997.5030593997925</v>
       </c>
       <c r="F52" t="n">
-        <v>178.3920516037439</v>
+        <v>244.6038972738466</v>
       </c>
       <c r="G52" t="n">
-        <v>62.16010539961907</v>
+        <v>69.83077528557813</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>b'3FHL J1053.6+4930 '</t>
+          <t>b'3FHL J1142.0+1546 '</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>163.4012298583984</v>
+        <v>175.5173187255859</v>
       </c>
       <c r="D53" t="n">
-        <v>49.50532150268555</v>
+        <v>15.77690410614014</v>
       </c>
       <c r="E53" t="n">
-        <v>586.7293479424766</v>
+        <v>1205.915061750614</v>
       </c>
       <c r="F53" t="n">
-        <v>160.2472928171692</v>
+        <v>244.5908969669972</v>
       </c>
       <c r="G53" t="n">
-        <v>58.20941647675482</v>
+        <v>70.30592729967964</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>154</v>
+        <v>173</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>b'3FHL J1058.6+5628 '</t>
+          <t>b'3FHL J1143.1+6121 '</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>164.6645202636719</v>
+        <v>175.7978515625</v>
       </c>
       <c r="D54" t="n">
-        <v>56.46826171875</v>
+        <v>61.35290145874023</v>
       </c>
       <c r="E54" t="n">
-        <v>598.8824976040644</v>
+        <v>209.6566093130006</v>
       </c>
       <c r="F54" t="n">
-        <v>149.5898498865417</v>
+        <v>136.7459514614812</v>
       </c>
       <c r="G54" t="n">
-        <v>54.42879075775696</v>
+        <v>53.90689117248857</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>155</v>
+        <v>174</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>b'3FHL J1100.3+4020 '</t>
+          <t>b'3FHL J1145.0+1935 '</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>165.0803070068359</v>
+        <v>176.2684783935547</v>
       </c>
       <c r="D55" t="n">
-        <v>40.3358268737793</v>
+        <v>19.5903205871582</v>
       </c>
       <c r="E55" t="n">
-        <v>924.0846438011745</v>
+        <v>93.48446529540507</v>
       </c>
       <c r="F55" t="n">
-        <v>175.8469476326254</v>
+        <v>235.771105621029</v>
       </c>
       <c r="G55" t="n">
-        <v>63.555059895797</v>
+        <v>73.02859819966865</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>157</v>
+        <v>175</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>b'3FHL J1104.4+3812 '</t>
+          <t>b'3FHL J1150.3+2418 '</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>166.1207580566406</v>
+        <v>177.5877227783203</v>
       </c>
       <c r="D56" t="n">
-        <v>38.20518112182617</v>
+        <v>24.30084228515625</v>
       </c>
       <c r="E56" t="n">
-        <v>128.9003855881938</v>
+        <v>826.3707136061979</v>
       </c>
       <c r="F56" t="n">
-        <v>179.8357877680561</v>
+        <v>221.1457388558182</v>
       </c>
       <c r="G56" t="n">
-        <v>65.03781332953814</v>
+        <v>75.96302613210874</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>158</v>
+        <v>176</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>b'3FHL J1105.8+3944 '</t>
+          <t>b'3FHL J1153.2+4929 '</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>166.4540252685547</v>
+        <v>178.3224639892578</v>
       </c>
       <c r="D57" t="n">
-        <v>39.74899673461914</v>
+        <v>49.49262237548828</v>
       </c>
       <c r="E57" t="n">
-        <v>418.8482280609101</v>
+        <v>1335.3602067056</v>
       </c>
       <c r="F57" t="n">
-        <v>176.2092588270897</v>
+        <v>145.6204816776282</v>
       </c>
       <c r="G57" t="n">
-        <v>64.74895803570412</v>
+        <v>64.99564919843898</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>b'3FHL J1107.8+1501 '</t>
+          <t>b'3FHL J1203.1+6030 '</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>166.9655914306641</v>
+        <v>180.7808227539062</v>
       </c>
       <c r="D58" t="n">
-        <v>15.02733516693115</v>
+        <v>60.51219177246094</v>
       </c>
       <c r="E58" t="n">
-        <v>2240.185974418625</v>
+        <v>277.125303444809</v>
       </c>
       <c r="F58" t="n">
-        <v>234.34727958246</v>
+        <v>133.4418834029724</v>
       </c>
       <c r="G58" t="n">
-        <v>63.06038848548737</v>
+        <v>55.61926798865239</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>160</v>
+        <v>182</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>b'3FHL J1109.7+3735 '</t>
+          <t>b'3FHL J1208.1+6120 '</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>167.4311370849609</v>
+        <v>182.0427551269531</v>
       </c>
       <c r="D59" t="n">
-        <v>37.58807754516602</v>
+        <v>61.34061431884766</v>
       </c>
       <c r="E59" t="n">
-        <v>1563.657198577747</v>
+        <v>1115.723809237682</v>
       </c>
       <c r="F59" t="n">
-        <v>180.457347654663</v>
+        <v>131.9651880062851</v>
       </c>
       <c r="G59" t="n">
-        <v>66.2143548292574</v>
+        <v>55.02232038849426</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>161</v>
+        <v>184</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>b'3FHL J1117.0+2014 '</t>
+          <t>b'3FHL J1216.0-0242 '</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>169.2679595947266</v>
+        <v>184.0193023681641</v>
       </c>
       <c r="D60" t="n">
-        <v>20.23810386657715</v>
+        <v>-2.713768005371094</v>
       </c>
       <c r="E60" t="n">
-        <v>578.6172947152628</v>
+        <v>1426.312274688342</v>
       </c>
       <c r="F60" t="n">
-        <v>225.5716267064807</v>
+        <v>285.6103354390478</v>
       </c>
       <c r="G60" t="n">
-        <v>67.36670331755562</v>
+        <v>58.96364214349016</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>163</v>
+        <v>185</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>b'3FHL J1120.8+4212 '</t>
+          <t>b'3FHL J1217.9+3006 '</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>170.2008819580078</v>
+        <v>184.4772338867188</v>
       </c>
       <c r="D61" t="n">
-        <v>42.20166015625</v>
+        <v>30.11482238769531</v>
       </c>
       <c r="E61" t="n">
-        <v>521.6104982541038</v>
+        <v>546.0896141426656</v>
       </c>
       <c r="F61" t="n">
-        <v>167.856902782118</v>
+        <v>188.8666537572836</v>
       </c>
       <c r="G61" t="n">
-        <v>66.16418823817627</v>
+        <v>82.06187773446577</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>166</v>
+        <v>186</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>b'3FHL J1131.6+5809 '</t>
+          <t>b'3FHL J1218.0-0028 '</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>172.9062042236328</v>
+        <v>184.51953125</v>
       </c>
       <c r="D62" t="n">
-        <v>58.16561508178711</v>
+        <v>-0.4782386422157288</v>
       </c>
       <c r="E62" t="n">
-        <v>1429.924347323077</v>
+        <v>1639.503972536957</v>
       </c>
       <c r="F62" t="n">
-        <v>141.6893921444634</v>
+        <v>285.3804349262129</v>
       </c>
       <c r="G62" t="n">
-        <v>55.9604528362288</v>
+        <v>61.25154181229235</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>169</v>
+        <v>187</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>b'3FHL J1136.8+2549 '</t>
+          <t>b'3FHL J1219.7-0312 '</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>174.2185363769531</v>
+        <v>184.9271392822266</v>
       </c>
       <c r="D63" t="n">
-        <v>25.8327808380127</v>
+        <v>-3.212921857833862</v>
       </c>
       <c r="E63" t="n">
-        <v>651.3386580792431</v>
+        <v>1205.915061750614</v>
       </c>
       <c r="F63" t="n">
-        <v>213.1465867327724</v>
+        <v>287.5483319154165</v>
       </c>
       <c r="G63" t="n">
-        <v>73.27986298713279</v>
+        <v>58.70790553974744</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>171</v>
+        <v>189</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>b'3FHL J1140.5+1528 '</t>
+          <t>b'3FHL J1221.3+3010 '</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>175.1320648193359</v>
+        <v>185.3371734619141</v>
       </c>
       <c r="D64" t="n">
-        <v>15.48001480102539</v>
+        <v>30.16693115234375</v>
       </c>
       <c r="E64" t="n">
-        <v>997.5030593997925</v>
+        <v>763.1726232934241</v>
       </c>
       <c r="F64" t="n">
-        <v>244.6038972738466</v>
+        <v>186.4431504600458</v>
       </c>
       <c r="G64" t="n">
-        <v>69.83077528557813</v>
+        <v>82.7350715996196</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>172</v>
+        <v>190</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>b'3FHL J1142.0+1546 '</t>
+          <t>b'3FHL J1221.5+2813 '</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>175.5173187255859</v>
+        <v>185.3848114013672</v>
       </c>
       <c r="D65" t="n">
-        <v>15.77690410614014</v>
+        <v>28.23212242126465</v>
       </c>
       <c r="E65" t="n">
-        <v>1205.915061750614</v>
+        <v>431.2447065513599</v>
       </c>
       <c r="F65" t="n">
-        <v>244.5908969669972</v>
+        <v>201.7391806851846</v>
       </c>
       <c r="G65" t="n">
-        <v>70.30592729967964</v>
+        <v>83.29053790221776</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>173</v>
+        <v>191</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>b'3FHL J1143.1+6121 '</t>
+          <t>b'3FHL J1224.4+2436 '</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>175.7978515625</v>
+        <v>186.1085205078125</v>
       </c>
       <c r="D66" t="n">
-        <v>61.35290145874023</v>
+        <v>24.6070442199707</v>
       </c>
       <c r="E66" t="n">
-        <v>209.6566093130006</v>
+        <v>900.7483492023172</v>
       </c>
       <c r="F66" t="n">
-        <v>136.7459514614812</v>
+        <v>233.9729892145359</v>
       </c>
       <c r="G66" t="n">
-        <v>53.90689117248857</v>
+        <v>83.42441521408441</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>b'3FHL J1145.0+1935 '</t>
+          <t>b'3FHL J1224.9+2122 '</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>176.2684783935547</v>
+        <v>186.2270355224609</v>
       </c>
       <c r="D67" t="n">
-        <v>19.5903205871582</v>
+        <v>21.38190269470215</v>
       </c>
       <c r="E67" t="n">
-        <v>93.48446529540507</v>
+        <v>1691.687106632469</v>
       </c>
       <c r="F67" t="n">
-        <v>235.771105621029</v>
+        <v>255.0624608818417</v>
       </c>
       <c r="G67" t="n">
-        <v>73.02859819966865</v>
+        <v>81.66152573596764</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>175</v>
+        <v>195</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>b'3FHL J1150.3+2418 '</t>
+          <t>b'3FHL J1229.2+0201 '</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>177.5877227783203</v>
+        <v>187.3038330078125</v>
       </c>
       <c r="D68" t="n">
-        <v>24.30084228515625</v>
+        <v>2.024992942810059</v>
       </c>
       <c r="E68" t="n">
-        <v>826.3707136061979</v>
+        <v>659.3789000935117</v>
       </c>
       <c r="F68" t="n">
-        <v>221.1457388558182</v>
+        <v>290.0221226405291</v>
       </c>
       <c r="G68" t="n">
-        <v>75.96302613210874</v>
+        <v>64.33829691205085</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>176</v>
+        <v>196</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>b'3FHL J1153.2+4929 '</t>
+          <t>b'3FHL J1230.2+2517 '</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>178.3224639892578</v>
+        <v>187.5732727050781</v>
       </c>
       <c r="D69" t="n">
-        <v>49.49262237548828</v>
+        <v>25.29787635803223</v>
       </c>
       <c r="E69" t="n">
-        <v>1335.3602067056</v>
+        <v>566.434356575713</v>
       </c>
       <c r="F69" t="n">
-        <v>145.6204816776282</v>
+        <v>232.8530732554522</v>
       </c>
       <c r="G69" t="n">
-        <v>64.99564919843898</v>
+        <v>84.91711617677194</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>179</v>
+        <v>197</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>b'3FHL J1203.1+6030 '</t>
+          <t>b'3FHL J1230.8+1223 '</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>180.7808227539062</v>
+        <v>187.7033386230469</v>
       </c>
       <c r="D70" t="n">
-        <v>60.51219177246094</v>
+        <v>12.38887977600098</v>
       </c>
       <c r="E70" t="n">
-        <v>277.125303444809</v>
+        <v>18.50588103089174</v>
       </c>
       <c r="F70" t="n">
-        <v>133.4418834029724</v>
+        <v>283.7712082555389</v>
       </c>
       <c r="G70" t="n">
-        <v>55.61926798865239</v>
+        <v>74.48825666506053</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>182</v>
+        <v>198</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>b'3FHL J1208.1+6120 '</t>
+          <t>b'3FHL J1231.4+1422 '</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>182.0427551269531</v>
+        <v>187.8662414550781</v>
       </c>
       <c r="D71" t="n">
-        <v>61.34061431884766</v>
+        <v>14.3680305480957</v>
       </c>
       <c r="E71" t="n">
-        <v>1115.723809237682</v>
+        <v>1043.496525858729</v>
       </c>
       <c r="F71" t="n">
-        <v>131.9651880062851</v>
+        <v>281.8921172763349</v>
       </c>
       <c r="G71" t="n">
-        <v>55.02232038849426</v>
+        <v>76.41707829778731</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>184</v>
+        <v>199</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>b'3FHL J1216.0-0242 '</t>
+          <t>b'3FHL J1231.6+6415 '</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>184.0193023681641</v>
+        <v>187.9054565429688</v>
       </c>
       <c r="D72" t="n">
-        <v>-2.713768005371094</v>
+        <v>64.26630401611328</v>
       </c>
       <c r="E72" t="n">
-        <v>1426.312274688342</v>
+        <v>679.4444413307867</v>
       </c>
       <c r="F72" t="n">
-        <v>285.6103354390478</v>
+        <v>126.4813572877882</v>
       </c>
       <c r="G72" t="n">
-        <v>58.96364214349016</v>
+        <v>52.72516890602747</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>b'3FHL J1217.9+3006 '</t>
+          <t>b'3FHL J1231.7+2847 '</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>184.4772338867188</v>
+        <v>187.9381866455078</v>
       </c>
       <c r="D73" t="n">
-        <v>30.11482238769531</v>
+        <v>28.79290008544922</v>
       </c>
       <c r="E73" t="n">
-        <v>546.0896141426656</v>
+        <v>968.4201348245213</v>
       </c>
       <c r="F73" t="n">
-        <v>188.8666537572836</v>
+        <v>190.8352813272477</v>
       </c>
       <c r="G73" t="n">
-        <v>82.06187773446577</v>
+        <v>85.34586086634012</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>186</v>
+        <v>204</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>b'3FHL J1218.0-0028 '</t>
+          <t>b'3FHL J1247.0+4421 '</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>184.51953125</v>
+        <v>191.7523803710938</v>
       </c>
       <c r="D74" t="n">
-        <v>-0.4782386422157288</v>
+        <v>44.35237503051758</v>
       </c>
       <c r="E74" t="n">
-        <v>1639.503972536957</v>
+        <v>2240.185974418625</v>
       </c>
       <c r="F74" t="n">
-        <v>285.3804349262129</v>
+        <v>125.6027117904971</v>
       </c>
       <c r="G74" t="n">
-        <v>61.25154181229235</v>
+        <v>72.75290303465637</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>187</v>
+        <v>206</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>b'3FHL J1219.7-0312 '</t>
+          <t>b'3FHL J1253.7+0328 '</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>184.9271392822266</v>
+        <v>193.4472503662109</v>
       </c>
       <c r="D75" t="n">
-        <v>-3.212921857833862</v>
+        <v>3.473009824752808</v>
       </c>
       <c r="E75" t="n">
-        <v>1205.915061750614</v>
+        <v>281.3257125002922</v>
       </c>
       <c r="F75" t="n">
-        <v>287.5483319154165</v>
+        <v>304.3938914960014</v>
       </c>
       <c r="G75" t="n">
-        <v>58.70790553974744</v>
+        <v>66.33808457924333</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>189</v>
+        <v>207</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>b'3FHL J1221.3+3010 '</t>
+          <t>b'3FHL J1254.4+2210 '</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>185.3371734619141</v>
+        <v>193.6058959960938</v>
       </c>
       <c r="D76" t="n">
-        <v>30.16693115234375</v>
+        <v>22.18258476257324</v>
       </c>
       <c r="E76" t="n">
-        <v>763.1726232934241</v>
+        <v>1946.014319805091</v>
       </c>
       <c r="F76" t="n">
-        <v>186.4431504600458</v>
+        <v>310.9003864000454</v>
       </c>
       <c r="G76" t="n">
-        <v>82.7350715996196</v>
+        <v>85.00807392479871</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>b'3FHL J1221.5+2813 '</t>
+          <t>b'3FHL J1256.1-0547 '</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>185.3848114013672</v>
+        <v>194.0442810058594</v>
       </c>
       <c r="D77" t="n">
-        <v>28.23212242126465</v>
+        <v>-5.79459285736084</v>
       </c>
       <c r="E77" t="n">
-        <v>431.2447065513599</v>
+        <v>2034.921432753547</v>
       </c>
       <c r="F77" t="n">
-        <v>201.7391806851846</v>
+        <v>305.0998846118308</v>
       </c>
       <c r="G77" t="n">
-        <v>83.29053790221776</v>
+        <v>57.05720524664127</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>191</v>
+        <v>210</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>b'3FHL J1224.4+2436 '</t>
+          <t>b'3FHL J1258.3+6121 '</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>186.1085205078125</v>
+        <v>194.5815887451172</v>
       </c>
       <c r="D78" t="n">
-        <v>24.6070442199707</v>
+        <v>61.36655807495117</v>
       </c>
       <c r="E78" t="n">
-        <v>900.7483492023172</v>
+        <v>920.2003591656152</v>
       </c>
       <c r="F78" t="n">
-        <v>233.9729892145359</v>
+        <v>121.4659798152458</v>
       </c>
       <c r="G78" t="n">
-        <v>83.42441521408441</v>
+        <v>55.7420815224022</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>192</v>
+        <v>213</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>b'3FHL J1224.9+2122 '</t>
+          <t>b'3FHL J1312.6+4828 '</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>186.2270355224609</v>
+        <v>198.1574249267578</v>
       </c>
       <c r="D79" t="n">
-        <v>21.38190269470215</v>
+        <v>48.47776031494141</v>
       </c>
       <c r="E79" t="n">
-        <v>1691.687106632469</v>
+        <v>1919.40425528274</v>
       </c>
       <c r="F79" t="n">
-        <v>255.0624608818417</v>
+        <v>113.4210086615013</v>
       </c>
       <c r="G79" t="n">
-        <v>81.66152573596764</v>
+        <v>68.25727662537837</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>195</v>
+        <v>216</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>b'3FHL J1229.2+0201 '</t>
+          <t>b'3FHL J1319.5+1404 '</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>187.3038330078125</v>
+        <v>199.8961791992188</v>
       </c>
       <c r="D80" t="n">
-        <v>2.024992942810059</v>
+        <v>14.07064819335938</v>
       </c>
       <c r="E80" t="n">
-        <v>659.3789000935117</v>
+        <v>2154.520586195584</v>
       </c>
       <c r="F80" t="n">
-        <v>290.0221226405291</v>
+        <v>331.0264520499293</v>
       </c>
       <c r="G80" t="n">
-        <v>64.33829691205085</v>
+        <v>75.38452389248357</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>196</v>
+        <v>220</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>b'3FHL J1230.2+2517 '</t>
+          <t>b'3FHL J1340.5+4410 '</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>187.5732727050781</v>
+        <v>205.1303100585938</v>
       </c>
       <c r="D81" t="n">
-        <v>25.29787635803223</v>
+        <v>44.18074798583984</v>
       </c>
       <c r="E81" t="n">
-        <v>566.434356575713</v>
+        <v>2067.499118066273</v>
       </c>
       <c r="F81" t="n">
-        <v>232.8530732554522</v>
+        <v>96.05410900986132</v>
       </c>
       <c r="G81" t="n">
-        <v>84.91711617677194</v>
+        <v>70.29735077732514</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>197</v>
+        <v>221</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>b'3FHL J1230.8+1223 '</t>
+          <t>b'3FHL J1341.2+3959 '</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>187.7033386230469</v>
+        <v>205.3132781982422</v>
       </c>
       <c r="D82" t="n">
-        <v>12.38887977600098</v>
+        <v>39.98970031738281</v>
       </c>
       <c r="E82" t="n">
-        <v>18.50588103089174</v>
+        <v>715.4362988699944</v>
       </c>
       <c r="F82" t="n">
-        <v>283.7712082555389</v>
+        <v>87.33566812682206</v>
       </c>
       <c r="G82" t="n">
-        <v>74.48825666506053</v>
+        <v>73.50951317099407</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>198</v>
+        <v>223</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>b'3FHL J1231.4+1422 '</t>
+          <t>b'3FHL J1402.6+1559 '</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>187.8662414550781</v>
+        <v>210.6538238525391</v>
       </c>
       <c r="D83" t="n">
-        <v>14.3680305480957</v>
+        <v>15.98397254943848</v>
       </c>
       <c r="E83" t="n">
-        <v>1043.496525858729</v>
+        <v>997.5030593997925</v>
       </c>
       <c r="F83" t="n">
-        <v>281.8921172763349</v>
+        <v>2.539795875341265</v>
       </c>
       <c r="G83" t="n">
-        <v>76.41707829778731</v>
+        <v>70.08723433248876</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>199</v>
+        <v>225</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>b'3FHL J1231.6+6415 '</t>
+          <t>b'3FHL J1404.9+0401 '</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>187.9054565429688</v>
+        <v>211.2331237792969</v>
       </c>
       <c r="D84" t="n">
-        <v>64.26630401611328</v>
+        <v>4.028957843780518</v>
       </c>
       <c r="E84" t="n">
-        <v>679.4444413307867</v>
+        <v>1371.891644524125</v>
       </c>
       <c r="F84" t="n">
-        <v>126.4813572877882</v>
+        <v>343.356454326494</v>
       </c>
       <c r="G84" t="n">
-        <v>52.72516890602747</v>
+        <v>60.99387507635056</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>200</v>
+        <v>226</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>b'3FHL J1231.7+2847 '</t>
+          <t>b'3FHL J1411.8+5249 '</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>187.9381866455078</v>
+        <v>212.9649963378906</v>
       </c>
       <c r="D85" t="n">
-        <v>28.79290008544922</v>
+        <v>52.82292938232422</v>
       </c>
       <c r="E85" t="n">
-        <v>968.4201348245213</v>
+        <v>325.2711537377689</v>
       </c>
       <c r="F85" t="n">
-        <v>190.8352813272477</v>
+        <v>98.17146981808737</v>
       </c>
       <c r="G85" t="n">
-        <v>85.34586086634012</v>
+        <v>60.26679845594848</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>204</v>
+        <v>227</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>b'3FHL J1247.0+4421 '</t>
+          <t>b'3FHL J1415.6+4830 '</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>191.7523803710938</v>
+        <v>213.9147796630859</v>
       </c>
       <c r="D86" t="n">
-        <v>44.35237503051758</v>
+        <v>48.51522445678711</v>
       </c>
       <c r="E86" t="n">
-        <v>2240.185974418625</v>
+        <v>1902.710656439457</v>
       </c>
       <c r="F86" t="n">
-        <v>125.6027117904971</v>
+        <v>91.19850370499088</v>
       </c>
       <c r="G86" t="n">
-        <v>72.75290303465637</v>
+        <v>63.09742003770977</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>206</v>
+        <v>229</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>b'3FHL J1253.7+0328 '</t>
+          <t>b'3FHL J1418.0+2543 '</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>193.4472503662109</v>
+        <v>214.5009460449219</v>
       </c>
       <c r="D87" t="n">
-        <v>3.473009824752808</v>
+        <v>25.7291259765625</v>
       </c>
       <c r="E87" t="n">
-        <v>281.3257125002922</v>
+        <v>970.5390841006508</v>
       </c>
       <c r="F87" t="n">
-        <v>304.3938914960014</v>
+        <v>33.71460610300097</v>
       </c>
       <c r="G87" t="n">
-        <v>66.33808457924333</v>
+        <v>70.59372559903728</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>207</v>
+        <v>230</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>b'3FHL J1254.4+2210 '</t>
+          <t>b'3FHL J1419.4+0444 '</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>193.6058959960938</v>
+        <v>214.8675231933594</v>
       </c>
       <c r="D88" t="n">
-        <v>22.18258476257324</v>
+        <v>4.745282173156738</v>
       </c>
       <c r="E88" t="n">
-        <v>1946.014319805091</v>
+        <v>598.8824976040644</v>
       </c>
       <c r="F88" t="n">
-        <v>310.9003864000454</v>
+        <v>349.978509379617</v>
       </c>
       <c r="G88" t="n">
-        <v>85.00807392479871</v>
+        <v>59.3198698029064</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>208</v>
+        <v>231</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>b'3FHL J1256.1-0547 '</t>
+          <t>b'3FHL J1419.7+5423 '</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>194.0442810058594</v>
+        <v>214.9465789794922</v>
       </c>
       <c r="D89" t="n">
-        <v>-5.79459285736084</v>
+        <v>54.39066696166992</v>
       </c>
       <c r="E89" t="n">
-        <v>2034.921432753547</v>
+        <v>639.2633050973789</v>
       </c>
       <c r="F89" t="n">
-        <v>305.0998846118308</v>
+        <v>98.30243691724219</v>
       </c>
       <c r="G89" t="n">
-        <v>57.05720524664127</v>
+        <v>58.30848489225325</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>210</v>
+        <v>232</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>b'3FHL J1258.3+6121 '</t>
+          <t>b'3FHL J1422.6+5801 '</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>194.5815887451172</v>
+        <v>215.6541900634766</v>
       </c>
       <c r="D90" t="n">
-        <v>61.36655807495117</v>
+        <v>58.01887893676758</v>
       </c>
       <c r="E90" t="n">
-        <v>920.2003591656152</v>
+        <v>2349.244257634401</v>
       </c>
       <c r="F90" t="n">
-        <v>121.4659798152458</v>
+        <v>101.8492086867801</v>
       </c>
       <c r="G90" t="n">
-        <v>55.7420815224022</v>
+        <v>55.21857129706387</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>213</v>
+        <v>233</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>b'3FHL J1312.6+4828 '</t>
+          <t>b'3FHL J1428.5+4240 '</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>198.1574249267578</v>
+        <v>217.1364593505859</v>
       </c>
       <c r="D91" t="n">
-        <v>48.47776031494141</v>
+        <v>42.67203521728516</v>
       </c>
       <c r="E91" t="n">
-        <v>1919.40425528274</v>
+        <v>542.0147093189177</v>
       </c>
       <c r="F91" t="n">
-        <v>113.4210086615013</v>
+        <v>77.48566790521888</v>
       </c>
       <c r="G91" t="n">
-        <v>68.25727662537837</v>
+        <v>64.8988126310412</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>216</v>
+        <v>234</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>b'3FHL J1319.5+1404 '</t>
+          <t>b'3FHL J1436.9+5639 '</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>199.8961791992188</v>
+        <v>219.2470092773438</v>
       </c>
       <c r="D92" t="n">
-        <v>14.07064819335938</v>
+        <v>56.66003799438477</v>
       </c>
       <c r="E92" t="n">
-        <v>2154.520586195584</v>
+        <v>627.1700359849448</v>
       </c>
       <c r="F92" t="n">
-        <v>331.0264520499293</v>
+        <v>97.72870692965985</v>
       </c>
       <c r="G92" t="n">
-        <v>75.38452389248357</v>
+        <v>54.99658828453175</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>b'3FHL J1340.5+4410 '</t>
+          <t>b'3FHL J1439.3+3931 '</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>205.1303100585938</v>
+        <v>219.8288269042969</v>
       </c>
       <c r="D93" t="n">
-        <v>44.18074798583984</v>
+        <v>39.52298355102539</v>
       </c>
       <c r="E93" t="n">
-        <v>2067.499118066273</v>
+        <v>1371.891644524125</v>
       </c>
       <c r="F93" t="n">
-        <v>96.05410900986132</v>
+        <v>68.79583747417368</v>
       </c>
       <c r="G93" t="n">
-        <v>70.29735077732514</v>
+        <v>64.42668452711504</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>221</v>
+        <v>236</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>b'3FHL J1341.2+3959 '</t>
+          <t>b'3FHL J1440.9+0610 '</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>205.3132781982422</v>
+        <v>220.2337188720703</v>
       </c>
       <c r="D94" t="n">
-        <v>39.98970031738281</v>
+        <v>6.175134658813477</v>
       </c>
       <c r="E94" t="n">
-        <v>715.4362988699944</v>
+        <v>1558.62649529763</v>
       </c>
       <c r="F94" t="n">
-        <v>87.33566812682206</v>
+        <v>359.0613035363558</v>
       </c>
       <c r="G94" t="n">
-        <v>73.50951317099407</v>
+        <v>56.59426497141165</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>223</v>
+        <v>237</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>b'3FHL J1402.6+1559 '</t>
+          <t>b'3FHL J1442.8+1200 '</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>210.6538238525391</v>
+        <v>220.7103729248047</v>
       </c>
       <c r="D95" t="n">
-        <v>15.98397254943848</v>
+        <v>12.00308227539062</v>
       </c>
       <c r="E95" t="n">
-        <v>997.5030593997925</v>
+        <v>679.4444413307867</v>
       </c>
       <c r="F95" t="n">
-        <v>2.539795875341265</v>
+        <v>8.326391244799357</v>
       </c>
       <c r="G95" t="n">
-        <v>70.08723433248876</v>
+        <v>59.82810578059493</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>225</v>
+        <v>238</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>b'3FHL J1404.9+0401 '</t>
+          <t>b'3FHL J1443.5+2515 '</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>211.2331237792969</v>
+        <v>220.8969116210938</v>
       </c>
       <c r="D96" t="n">
-        <v>4.028957843780518</v>
+        <v>25.26393508911133</v>
       </c>
       <c r="E96" t="n">
-        <v>1371.891644524125</v>
+        <v>2012.076573556624</v>
       </c>
       <c r="F96" t="n">
-        <v>343.356454326494</v>
+        <v>35.06898725925156</v>
       </c>
       <c r="G96" t="n">
-        <v>60.99387507635056</v>
+        <v>64.8249872712824</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>226</v>
+        <v>240</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>b'3FHL J1411.8+5249 '</t>
+          <t>b'3FHL J1449.5+2745 '</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>212.9649963378906</v>
+        <v>222.3851776123047</v>
       </c>
       <c r="D97" t="n">
-        <v>52.82292938232422</v>
+        <v>27.75633811950684</v>
       </c>
       <c r="E97" t="n">
-        <v>325.2711537377689</v>
+        <v>931.8472681578297</v>
       </c>
       <c r="F97" t="n">
-        <v>98.17146981808737</v>
+        <v>41.19890036398075</v>
       </c>
       <c r="G97" t="n">
-        <v>60.26679845594848</v>
+        <v>63.8522071735304</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>227</v>
+        <v>242</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>b'3FHL J1415.6+4830 '</t>
+          <t>b'3FHL J1458.7+3722 '</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>213.9147796630859</v>
+        <v>224.6948089599609</v>
       </c>
       <c r="D98" t="n">
-        <v>48.51522445678711</v>
+        <v>37.36803436279297</v>
       </c>
       <c r="E98" t="n">
-        <v>1902.710656439457</v>
+        <v>1331.696061964219</v>
       </c>
       <c r="F98" t="n">
-        <v>91.19850370499088</v>
+        <v>61.92235747685517</v>
       </c>
       <c r="G98" t="n">
-        <v>63.09742003770977</v>
+        <v>61.36237350674613</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>229</v>
+        <v>243</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>b'3FHL J1418.0+2543 '</t>
+          <t>b'3FHL J1500.9+2238 '</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>214.5009460449219</v>
+        <v>225.2482757568359</v>
       </c>
       <c r="D99" t="n">
-        <v>25.7291259765625</v>
+        <v>22.64022445678711</v>
       </c>
       <c r="E99" t="n">
-        <v>970.5390841006508</v>
+        <v>962.8168789726126</v>
       </c>
       <c r="F99" t="n">
-        <v>33.71460610300097</v>
+        <v>31.45102290888001</v>
       </c>
       <c r="G99" t="n">
-        <v>70.59372559903728</v>
+        <v>60.35999634319712</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>230</v>
+        <v>244</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>b'3FHL J1419.4+0444 '</t>
+          <t>b'3FHL J1503.3+4758 '</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>214.8675231933594</v>
+        <v>225.8384399414062</v>
       </c>
       <c r="D100" t="n">
-        <v>4.745282173156738</v>
+        <v>47.97346878051758</v>
       </c>
       <c r="E100" t="n">
-        <v>598.8824976040644</v>
+        <v>1371.891644524125</v>
       </c>
       <c r="F100" t="n">
-        <v>349.978509379617</v>
+        <v>80.9535755751856</v>
       </c>
       <c r="G100" t="n">
-        <v>59.3198698029064</v>
+        <v>56.98629153475792</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>231</v>
+        <v>245</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>b'3FHL J1419.7+5423 '</t>
+          <t>b'3FHL J1506.0+3732 '</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>214.9465789794922</v>
+        <v>226.5228424072266</v>
       </c>
       <c r="D101" t="n">
-        <v>54.39066696166992</v>
+        <v>37.54251480102539</v>
       </c>
       <c r="E101" t="n">
-        <v>639.2633050973789</v>
+        <v>2465.150914639177</v>
       </c>
       <c r="F101" t="n">
-        <v>98.30243691724219</v>
+        <v>61.70862488595789</v>
       </c>
       <c r="G101" t="n">
-        <v>58.30848489225325</v>
+        <v>59.90456332383156</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
-        <v>232</v>
+        <v>246</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>b'3FHL J1422.6+5801 '</t>
+          <t>b'3FHL J1506.7+0813 '</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>215.6541900634766</v>
+        <v>226.6905822753906</v>
       </c>
       <c r="D102" t="n">
-        <v>58.01887893676758</v>
+        <v>8.218801498413086</v>
       </c>
       <c r="E102" t="n">
-        <v>2349.244257634401</v>
+        <v>1487.444413390686</v>
       </c>
       <c r="F102" t="n">
-        <v>101.8492086867801</v>
+        <v>8.730330769087979</v>
       </c>
       <c r="G102" t="n">
-        <v>55.21857129706387</v>
+        <v>52.83404159105811</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
-        <v>233</v>
+        <v>247</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>b'3FHL J1428.5+4240 '</t>
+          <t>b'3FHL J1507.2+1722 '</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>217.1364593505859</v>
+        <v>226.8249816894531</v>
       </c>
       <c r="D103" t="n">
-        <v>42.67203521728516</v>
+        <v>17.36773490905762</v>
       </c>
       <c r="E103" t="n">
-        <v>542.0147093189177</v>
+        <v>2129.778114886851</v>
       </c>
       <c r="F103" t="n">
-        <v>77.48566790521888</v>
+        <v>22.80134452177674</v>
       </c>
       <c r="G103" t="n">
-        <v>64.8988126310412</v>
+        <v>57.20281900749549</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
-        <v>234</v>
+        <v>248</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>b'3FHL J1436.9+5639 '</t>
+          <t>b'3FHL J1508.7+2708 '</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>219.2470092773438</v>
+        <v>227.1883544921875</v>
       </c>
       <c r="D104" t="n">
-        <v>56.66003799438477</v>
+        <v>27.14417457580566</v>
       </c>
       <c r="E104" t="n">
-        <v>627.1700359849448</v>
+        <v>1096.787424633644</v>
       </c>
       <c r="F104" t="n">
-        <v>97.72870692965985</v>
+        <v>40.97986187978024</v>
       </c>
       <c r="G104" t="n">
-        <v>54.99658828453175</v>
+        <v>59.54763194954369</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
-        <v>235</v>
+        <v>250</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>b'3FHL J1439.3+3931 '</t>
+          <t>b'3FHL J1512.2+0203 '</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>219.8288269042969</v>
+        <v>228.0720062255859</v>
       </c>
       <c r="D105" t="n">
-        <v>39.52298355102539</v>
+        <v>2.060366868972778</v>
       </c>
       <c r="E105" t="n">
-        <v>1371.891644524125</v>
+        <v>904.6427903224928</v>
       </c>
       <c r="F105" t="n">
-        <v>68.79583747417368</v>
+        <v>2.367075362555521</v>
       </c>
       <c r="G105" t="n">
-        <v>64.42668452711504</v>
+        <v>47.99279308444518</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
-        <v>236</v>
+        <v>253</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>b'3FHL J1440.9+0610 '</t>
+          <t>b'3FHL J1518.5+4044 '</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>220.2337188720703</v>
+        <v>229.6453247070312</v>
       </c>
       <c r="D106" t="n">
-        <v>6.175134658813477</v>
+        <v>40.73994827270508</v>
       </c>
       <c r="E106" t="n">
-        <v>1558.62649529763</v>
+        <v>277.125303444809</v>
       </c>
       <c r="F106" t="n">
-        <v>359.0613035363558</v>
+        <v>66.76651396705567</v>
       </c>
       <c r="G106" t="n">
-        <v>56.59426497141165</v>
+        <v>56.89182212745664</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
-        <v>237</v>
+        <v>254</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>b'3FHL J1442.8+1200 '</t>
+          <t>b'3FHL J1531.9+3016 '</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>220.7103729248047</v>
+        <v>232.9860992431641</v>
       </c>
       <c r="D107" t="n">
-        <v>12.00308227539062</v>
+        <v>30.27317047119141</v>
       </c>
       <c r="E107" t="n">
-        <v>679.4444413307867</v>
+        <v>277.125303444809</v>
       </c>
       <c r="F107" t="n">
-        <v>8.326391244799357</v>
+        <v>47.77962265205297</v>
       </c>
       <c r="G107" t="n">
-        <v>59.82810578059493</v>
+        <v>54.84301768980958</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
-        <v>238</v>
+        <v>255</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>b'3FHL J1443.5+2515 '</t>
+          <t>b'3FHL J1533.2+1855 '</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>220.8969116210938</v>
+        <v>233.3144226074219</v>
       </c>
       <c r="D108" t="n">
-        <v>25.26393508911133</v>
+        <v>18.93068313598633</v>
       </c>
       <c r="E108" t="n">
-        <v>2012.076573556624</v>
+        <v>1235.720342438146</v>
       </c>
       <c r="F108" t="n">
-        <v>35.06898725925156</v>
+        <v>29.25278554792897</v>
       </c>
       <c r="G108" t="n">
-        <v>64.8249872712824</v>
+        <v>52.0464613686915</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
-        <v>240</v>
+        <v>256</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>b'3FHL J1449.5+2745 '</t>
+          <t>b'3FHL J1540.7+1448 '</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>222.3851776123047</v>
+        <v>235.1949615478516</v>
       </c>
       <c r="D109" t="n">
-        <v>27.75633811950684</v>
+        <v>14.81568145751953</v>
       </c>
       <c r="E109" t="n">
-        <v>931.8472681578297</v>
+        <v>2255.902501594245</v>
       </c>
       <c r="F109" t="n">
-        <v>41.19890036398075</v>
+        <v>24.34762000956751</v>
       </c>
       <c r="G109" t="n">
-        <v>63.8522071735304</v>
+        <v>48.81774577195303</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
-        <v>242</v>
+        <v>258</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>b'3FHL J1458.7+3722 '</t>
+          <t>b'3FHL J1543.6+0452 '</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>224.6948089599609</v>
+        <v>235.9000091552734</v>
       </c>
       <c r="D110" t="n">
-        <v>37.36803436279297</v>
+        <v>4.879972457885742</v>
       </c>
       <c r="E110" t="n">
-        <v>1331.696061964219</v>
+        <v>171.3237639398314</v>
       </c>
       <c r="F110" t="n">
-        <v>61.92235747685517</v>
+        <v>12.27756886738662</v>
       </c>
       <c r="G110" t="n">
-        <v>61.36237350674613</v>
+        <v>43.38510723073886</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
-        <v>243</v>
+        <v>260</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>b'3FHL J1500.9+2238 '</t>
+          <t>b'3FHL J1554.2+2010 '</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>225.2482757568359</v>
+        <v>238.5714263916016</v>
       </c>
       <c r="D111" t="n">
-        <v>22.64022445678711</v>
+        <v>20.17705154418945</v>
       </c>
       <c r="E111" t="n">
-        <v>962.8168789726126</v>
+        <v>912.4256141983458</v>
       </c>
       <c r="F111" t="n">
-        <v>31.45102290888001</v>
+        <v>33.62416920162958</v>
       </c>
       <c r="G111" t="n">
-        <v>60.35999634319712</v>
+        <v>47.78168755695976</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
-        <v>244</v>
+        <v>261</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>b'3FHL J1503.3+4758 '</t>
+          <t>b'3FHL J1558.8+5626 '</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>225.8384399414062</v>
+        <v>239.7223358154297</v>
       </c>
       <c r="D112" t="n">
-        <v>47.97346878051758</v>
+        <v>56.44340133666992</v>
       </c>
       <c r="E112" t="n">
-        <v>1371.891644524125</v>
+        <v>1209.647842624998</v>
       </c>
       <c r="F112" t="n">
-        <v>80.9535755751856</v>
+        <v>87.61477950088891</v>
       </c>
       <c r="G112" t="n">
-        <v>56.98629153475792</v>
+        <v>45.75468964677962</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
-        <v>245</v>
+        <v>263</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>b'3FHL J1506.0+3732 '</t>
+          <t>b'3FHL J1603.8+1103 '</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>226.5228424072266</v>
+        <v>240.9507446289062</v>
       </c>
       <c r="D113" t="n">
-        <v>37.54251480102539</v>
+        <v>11.0573263168335</v>
       </c>
       <c r="E113" t="n">
-        <v>2465.150914639177</v>
+        <v>598.8824976040644</v>
       </c>
       <c r="F113" t="n">
-        <v>61.70862488595789</v>
+        <v>22.97464182629868</v>
       </c>
       <c r="G113" t="n">
-        <v>59.90456332383156</v>
+        <v>42.13516682302727</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
-        <v>246</v>
+        <v>264</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>b'3FHL J1506.7+0813 '</t>
+          <t>b'3FHL J1603.8+5010 '</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>226.6905822753906</v>
+        <v>240.9585723876953</v>
       </c>
       <c r="D114" t="n">
-        <v>8.218801498413086</v>
+        <v>50.16685104370117</v>
       </c>
       <c r="E114" t="n">
-        <v>1487.444413390686</v>
+        <v>2305.888248308498</v>
       </c>
       <c r="F114" t="n">
-        <v>8.730330769087979</v>
+        <v>78.62070005851318</v>
       </c>
       <c r="G114" t="n">
-        <v>52.83404159105811</v>
+        <v>46.96057254045356</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
-        <v>247</v>
+        <v>265</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>b'3FHL J1507.2+1722 '</t>
+          <t>b'3FHL J1606.2+5629 '</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>226.8249816894531</v>
+        <v>241.56298828125</v>
       </c>
       <c r="D115" t="n">
-        <v>17.36773490905762</v>
+        <v>56.4957389831543</v>
       </c>
       <c r="E115" t="n">
-        <v>2129.778114886851</v>
+        <v>1746.861857496495</v>
       </c>
       <c r="F115" t="n">
-        <v>22.80134452177674</v>
+        <v>87.17804013571619</v>
       </c>
       <c r="G115" t="n">
-        <v>57.20281900749549</v>
+        <v>44.78413662138935</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
-        <v>248</v>
+        <v>266</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>b'3FHL J1508.7+2708 '</t>
+          <t>b'3FHL J1607.0+1550 '</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>227.1883544921875</v>
+        <v>241.7560882568359</v>
       </c>
       <c r="D116" t="n">
-        <v>27.14417457580566</v>
+        <v>15.83572101593018</v>
       </c>
       <c r="E116" t="n">
-        <v>1096.787424633644</v>
+        <v>1902.710656439457</v>
       </c>
       <c r="F116" t="n">
-        <v>40.97986187978024</v>
+        <v>29.33763480478526</v>
       </c>
       <c r="G116" t="n">
-        <v>59.54763194954369</v>
+        <v>43.41828545322375</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
-        <v>250</v>
+        <v>267</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>b'3FHL J1512.2+0203 '</t>
+          <t>b'3FHL J1615.4+4711 '</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>228.0720062255859</v>
+        <v>243.8666687011719</v>
       </c>
       <c r="D117" t="n">
-        <v>2.060366868972778</v>
+        <v>47.19518280029297</v>
       </c>
       <c r="E117" t="n">
-        <v>904.6427903224928</v>
+        <v>820.9795643094412</v>
       </c>
       <c r="F117" t="n">
-        <v>2.367075362555521</v>
+        <v>73.86428573709217</v>
       </c>
       <c r="G117" t="n">
-        <v>47.99279308444518</v>
+        <v>45.64854529020995</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
-        <v>253</v>
+        <v>268</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>b'3FHL J1518.5+4044 '</t>
+          <t>b'3FHL J1626.2+3515 '</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>229.6453247070312</v>
+        <v>246.5747680664062</v>
       </c>
       <c r="D118" t="n">
-        <v>40.73994827270508</v>
+        <v>35.26229095458984</v>
       </c>
       <c r="E118" t="n">
-        <v>277.125303444809</v>
+        <v>1907.322882417562</v>
       </c>
       <c r="F118" t="n">
-        <v>66.76651396705567</v>
+        <v>56.96303155478957</v>
       </c>
       <c r="G118" t="n">
-        <v>56.89182212745664</v>
+        <v>43.8921473549683</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
-        <v>254</v>
+        <v>271</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>b'3FHL J1531.9+3016 '</t>
+          <t>b'3FHL J1642.9+3948 '</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>232.9860992431641</v>
+        <v>250.7349090576172</v>
       </c>
       <c r="D119" t="n">
-        <v>30.27317047119141</v>
+        <v>39.81490707397461</v>
       </c>
       <c r="E119" t="n">
-        <v>277.125303444809</v>
+        <v>2218.105585899384</v>
       </c>
       <c r="F119" t="n">
-        <v>47.77962265205297</v>
+        <v>63.46049227208619</v>
       </c>
       <c r="G119" t="n">
-        <v>54.84301768980958</v>
+        <v>40.95690199972307</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
-        <v>255</v>
+        <v>273</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>b'3FHL J1533.2+1855 '</t>
+          <t>b'3FHL J1647.6+4950 '</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>233.3144226074219</v>
+        <v>251.9024505615234</v>
       </c>
       <c r="D120" t="n">
-        <v>18.93068313598633</v>
+        <v>49.84615325927734</v>
       </c>
       <c r="E120" t="n">
-        <v>1235.720342438146</v>
+        <v>201.1884205905175</v>
       </c>
       <c r="F120" t="n">
-        <v>29.25278554792897</v>
+        <v>76.66087340567729</v>
       </c>
       <c r="G120" t="n">
-        <v>52.0464613686915</v>
+        <v>40.07035923704507</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
-        <v>256</v>
+        <v>274</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>b'3FHL J1540.7+1448 '</t>
+          <t>b'3FHL J1652.7+4024 '</t>
         </is>
       </c>
       <c r="C121" t="n">
-        <v>235.1949615478516</v>
+        <v>253.1941070556641</v>
       </c>
       <c r="D121" t="n">
-        <v>14.81568145751953</v>
+        <v>40.40338897705078</v>
       </c>
       <c r="E121" t="n">
-        <v>2255.902501594245</v>
+        <v>982.1071720326452</v>
       </c>
       <c r="F121" t="n">
-        <v>24.34762000956751</v>
+        <v>64.40155662759337</v>
       </c>
       <c r="G121" t="n">
-        <v>48.81774577195303</v>
+        <v>39.12261782369705</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
-        <v>258</v>
+        <v>275</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>b'3FHL J1543.6+0452 '</t>
+          <t>b'3FHL J1653.8+3945 '</t>
         </is>
       </c>
       <c r="C122" t="n">
-        <v>235.9000091552734</v>
+        <v>253.4710998535156</v>
       </c>
       <c r="D122" t="n">
-        <v>4.879972457885742</v>
+        <v>39.75818634033203</v>
       </c>
       <c r="E122" t="n">
-        <v>171.3237639398314</v>
+        <v>141.697084695296</v>
       </c>
       <c r="F122" t="n">
-        <v>12.27756886738662</v>
+        <v>63.59781706285712</v>
       </c>
       <c r="G122" t="n">
-        <v>43.38510723073886</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" s="1" t="n">
-        <v>260</v>
-      </c>
-      <c r="B123" t="inlineStr">
-        <is>
-          <t>b'3FHL J1554.2+2010 '</t>
-        </is>
-      </c>
-      <c r="C123" t="n">
-        <v>238.5714263916016</v>
-      </c>
-      <c r="D123" t="n">
-        <v>20.17705154418945</v>
-      </c>
-      <c r="E123" t="n">
-        <v>912.4256141983458</v>
-      </c>
-      <c r="F123" t="n">
-        <v>33.62416920162958</v>
-      </c>
-      <c r="G123" t="n">
-        <v>47.78168755695976</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" s="1" t="n">
-        <v>261</v>
-      </c>
-      <c r="B124" t="inlineStr">
-        <is>
-          <t>b'3FHL J1558.8+5626 '</t>
-        </is>
-      </c>
-      <c r="C124" t="n">
-        <v>239.7223358154297</v>
-      </c>
-      <c r="D124" t="n">
-        <v>56.44340133666992</v>
-      </c>
-      <c r="E124" t="n">
-        <v>1209.647842624998</v>
-      </c>
-      <c r="F124" t="n">
-        <v>87.61477950088891</v>
-      </c>
-      <c r="G124" t="n">
-        <v>45.75468964677962</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" s="1" t="n">
-        <v>263</v>
-      </c>
-      <c r="B125" t="inlineStr">
-        <is>
-          <t>b'3FHL J1603.8+1103 '</t>
-        </is>
-      </c>
-      <c r="C125" t="n">
-        <v>240.9507446289062</v>
-      </c>
-      <c r="D125" t="n">
-        <v>11.0573263168335</v>
-      </c>
-      <c r="E125" t="n">
-        <v>598.8824976040644</v>
-      </c>
-      <c r="F125" t="n">
-        <v>22.97464182629868</v>
-      </c>
-      <c r="G125" t="n">
-        <v>42.13516682302727</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" s="1" t="n">
-        <v>264</v>
-      </c>
-      <c r="B126" t="inlineStr">
-        <is>
-          <t>b'3FHL J1603.8+5010 '</t>
-        </is>
-      </c>
-      <c r="C126" t="n">
-        <v>240.9585723876953</v>
-      </c>
-      <c r="D126" t="n">
-        <v>50.16685104370117</v>
-      </c>
-      <c r="E126" t="n">
-        <v>2305.888248308498</v>
-      </c>
-      <c r="F126" t="n">
-        <v>78.62070005851318</v>
-      </c>
-      <c r="G126" t="n">
-        <v>46.96057254045356</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" s="1" t="n">
-        <v>265</v>
-      </c>
-      <c r="B127" t="inlineStr">
-        <is>
-          <t>b'3FHL J1606.2+5629 '</t>
-        </is>
-      </c>
-      <c r="C127" t="n">
-        <v>241.56298828125</v>
-      </c>
-      <c r="D127" t="n">
-        <v>56.4957389831543</v>
-      </c>
-      <c r="E127" t="n">
-        <v>1746.861857496495</v>
-      </c>
-      <c r="F127" t="n">
-        <v>87.17804013571619</v>
-      </c>
-      <c r="G127" t="n">
-        <v>44.78413662138935</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" s="1" t="n">
-        <v>266</v>
-      </c>
-      <c r="B128" t="inlineStr">
-        <is>
-          <t>b'3FHL J1607.0+1550 '</t>
-        </is>
-      </c>
-      <c r="C128" t="n">
-        <v>241.7560882568359</v>
-      </c>
-      <c r="D128" t="n">
-        <v>15.83572101593018</v>
-      </c>
-      <c r="E128" t="n">
-        <v>1902.710656439457</v>
-      </c>
-      <c r="F128" t="n">
-        <v>29.33763480478526</v>
-      </c>
-      <c r="G128" t="n">
-        <v>43.41828545322375</v>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" s="1" t="n">
-        <v>267</v>
-      </c>
-      <c r="B129" t="inlineStr">
-        <is>
-          <t>b'3FHL J1615.4+4711 '</t>
-        </is>
-      </c>
-      <c r="C129" t="n">
-        <v>243.8666687011719</v>
-      </c>
-      <c r="D129" t="n">
-        <v>47.19518280029297</v>
-      </c>
-      <c r="E129" t="n">
-        <v>820.9795643094412</v>
-      </c>
-      <c r="F129" t="n">
-        <v>73.86428573709217</v>
-      </c>
-      <c r="G129" t="n">
-        <v>45.64854529020995</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" s="1" t="n">
-        <v>268</v>
-      </c>
-      <c r="B130" t="inlineStr">
-        <is>
-          <t>b'3FHL J1626.2+3515 '</t>
-        </is>
-      </c>
-      <c r="C130" t="n">
-        <v>246.5747680664062</v>
-      </c>
-      <c r="D130" t="n">
-        <v>35.26229095458984</v>
-      </c>
-      <c r="E130" t="n">
-        <v>1907.322882417562</v>
-      </c>
-      <c r="F130" t="n">
-        <v>56.96303155478957</v>
-      </c>
-      <c r="G130" t="n">
-        <v>43.8921473549683</v>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" s="1" t="n">
-        <v>271</v>
-      </c>
-      <c r="B131" t="inlineStr">
-        <is>
-          <t>b'3FHL J1642.9+3948 '</t>
-        </is>
-      </c>
-      <c r="C131" t="n">
-        <v>250.7349090576172</v>
-      </c>
-      <c r="D131" t="n">
-        <v>39.81490707397461</v>
-      </c>
-      <c r="E131" t="n">
-        <v>2218.105585899384</v>
-      </c>
-      <c r="F131" t="n">
-        <v>63.46049227208619</v>
-      </c>
-      <c r="G131" t="n">
-        <v>40.95690199972307</v>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" s="1" t="n">
-        <v>273</v>
-      </c>
-      <c r="B132" t="inlineStr">
-        <is>
-          <t>b'3FHL J1647.6+4950 '</t>
-        </is>
-      </c>
-      <c r="C132" t="n">
-        <v>251.9024505615234</v>
-      </c>
-      <c r="D132" t="n">
-        <v>49.84615325927734</v>
-      </c>
-      <c r="E132" t="n">
-        <v>201.1884205905175</v>
-      </c>
-      <c r="F132" t="n">
-        <v>76.66087340567729</v>
-      </c>
-      <c r="G132" t="n">
-        <v>40.07035923704507</v>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" s="1" t="n">
-        <v>274</v>
-      </c>
-      <c r="B133" t="inlineStr">
-        <is>
-          <t>b'3FHL J1652.7+4024 '</t>
-        </is>
-      </c>
-      <c r="C133" t="n">
-        <v>253.1941070556641</v>
-      </c>
-      <c r="D133" t="n">
-        <v>40.40338897705078</v>
-      </c>
-      <c r="E133" t="n">
-        <v>982.1071720326452</v>
-      </c>
-      <c r="F133" t="n">
-        <v>64.40155662759337</v>
-      </c>
-      <c r="G133" t="n">
-        <v>39.12261782369705</v>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" s="1" t="n">
-        <v>275</v>
-      </c>
-      <c r="B134" t="inlineStr">
-        <is>
-          <t>b'3FHL J1653.8+3945 '</t>
-        </is>
-      </c>
-      <c r="C134" t="n">
-        <v>253.4710998535156</v>
-      </c>
-      <c r="D134" t="n">
-        <v>39.75818634033203</v>
-      </c>
-      <c r="E134" t="n">
-        <v>141.697084695296</v>
-      </c>
-      <c r="F134" t="n">
-        <v>63.59781706285712</v>
-      </c>
-      <c r="G134" t="n">
         <v>38.85626839795113</v>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" s="1" t="n">
-        <v>326</v>
-      </c>
-      <c r="B135" t="inlineStr">
-        <is>
-          <t>b'3FHL J2145.8+0718 '</t>
-        </is>
-      </c>
-      <c r="C135" t="n">
-        <v>326.453369140625</v>
-      </c>
-      <c r="D135" t="n">
-        <v>7.314035415649414</v>
-      </c>
-      <c r="E135" t="n">
-        <v>970.5390841006508</v>
-      </c>
-      <c r="F135" t="n">
-        <v>63.55150843812832</v>
-      </c>
-      <c r="G135" t="n">
-        <v>-33.41099096884161</v>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" s="1" t="n">
-        <v>328</v>
-      </c>
-      <c r="B136" t="inlineStr">
-        <is>
-          <t>b'3FHL J2153.1-0041 '</t>
-        </is>
-      </c>
-      <c r="C136" t="n">
-        <v>328.2919616699219</v>
-      </c>
-      <c r="D136" t="n">
-        <v>-0.686768651008606</v>
-      </c>
-      <c r="E136" t="n">
-        <v>1360.953256212888</v>
-      </c>
-      <c r="F136" t="n">
-        <v>57.05081428995042</v>
-      </c>
-      <c r="G136" t="n">
-        <v>-39.75220781580951</v>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" s="1" t="n">
-        <v>329</v>
-      </c>
-      <c r="B137" t="inlineStr">
-        <is>
-          <t>b'3FHL J2156.4-0036 '</t>
-        </is>
-      </c>
-      <c r="C137" t="n">
-        <v>329.1090087890625</v>
-      </c>
-      <c r="D137" t="n">
-        <v>-0.6149818301200867</v>
-      </c>
-      <c r="E137" t="n">
-        <v>1899.366209855216</v>
-      </c>
-      <c r="F137" t="n">
-        <v>57.75266804044341</v>
-      </c>
-      <c r="G137" t="n">
-        <v>-40.3719759791578</v>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" s="1" t="n">
-        <v>334</v>
-      </c>
-      <c r="B138" t="inlineStr">
-        <is>
-          <t>b'3FHL J2211.0-0003 '</t>
-        </is>
-      </c>
-      <c r="C138" t="n">
-        <v>332.7731628417969</v>
-      </c>
-      <c r="D138" t="n">
-        <v>-0.06335502862930298</v>
-      </c>
-      <c r="E138" t="n">
-        <v>1437.142271361721</v>
-      </c>
-      <c r="F138" t="n">
-        <v>61.31126713700598</v>
-      </c>
-      <c r="G138" t="n">
-        <v>-42.95404180444078</v>
-      </c>
-    </row>
-    <row r="139">
-      <c r="A139" s="1" t="n">
-        <v>335</v>
-      </c>
-      <c r="B139" t="inlineStr">
-        <is>
-          <t>b'3FHL J2216.9+2420 '</t>
-        </is>
-      </c>
-      <c r="C139" t="n">
-        <v>334.2324829101562</v>
-      </c>
-      <c r="D139" t="n">
-        <v>24.3468189239502</v>
-      </c>
-      <c r="E139" t="n">
-        <v>1932.724619037558</v>
-      </c>
-      <c r="F139" t="n">
-        <v>83.49402123884857</v>
-      </c>
-      <c r="G139" t="n">
-        <v>-26.45310175546729</v>
-      </c>
-    </row>
-    <row r="140">
-      <c r="A140" s="1" t="n">
-        <v>346</v>
-      </c>
-      <c r="B140" t="inlineStr">
-        <is>
-          <t>b'3FHL J2307.7+1451 '</t>
-        </is>
-      </c>
-      <c r="C140" t="n">
-        <v>346.9254455566406</v>
-      </c>
-      <c r="D140" t="n">
-        <v>14.86622333526611</v>
-      </c>
-      <c r="E140" t="n">
-        <v>1926.068372333629</v>
-      </c>
-      <c r="F140" t="n">
-        <v>88.84708373928603</v>
-      </c>
-      <c r="G140" t="n">
-        <v>-41.04000458576156</v>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" s="1" t="n">
-        <v>347</v>
-      </c>
-      <c r="B141" t="inlineStr">
-        <is>
-          <t>b'3FHL J2314.0+1445 '</t>
-        </is>
-      </c>
-      <c r="C141" t="n">
-        <v>348.5031433105469</v>
-      </c>
-      <c r="D141" t="n">
-        <v>14.75438690185547</v>
-      </c>
-      <c r="E141" t="n">
-        <v>683.4515571949081</v>
-      </c>
-      <c r="F141" t="n">
-        <v>90.52923262707655</v>
-      </c>
-      <c r="G141" t="n">
-        <v>-41.90635784661719</v>
-      </c>
-    </row>
-    <row r="142">
-      <c r="A142" s="1" t="n">
-        <v>349</v>
-      </c>
-      <c r="B142" t="inlineStr">
-        <is>
-          <t>b'3FHL J2322.6+3436 '</t>
-        </is>
-      </c>
-      <c r="C142" t="n">
-        <v>350.6634826660156</v>
-      </c>
-      <c r="D142" t="n">
-        <v>34.60570907592773</v>
-      </c>
-      <c r="E142" t="n">
-        <v>414.7121310817099</v>
-      </c>
-      <c r="F142" t="n">
-        <v>102.902685252486</v>
-      </c>
-      <c r="G142" t="n">
-        <v>-24.78935319679015</v>
-      </c>
-    </row>
-    <row r="143">
-      <c r="A143" s="1" t="n">
-        <v>356</v>
-      </c>
-      <c r="B143" t="inlineStr">
-        <is>
-          <t>b'3FHL J2338.9+2123 '</t>
-        </is>
-      </c>
-      <c r="C143" t="n">
-        <v>354.7449645996094</v>
-      </c>
-      <c r="D143" t="n">
-        <v>21.39655303955078</v>
-      </c>
-      <c r="E143" t="n">
-        <v>1175.980668839187</v>
-      </c>
-      <c r="F143" t="n">
-        <v>101.2521659165168</v>
-      </c>
-      <c r="G143" t="n">
-        <v>-38.40568155886272</v>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144" s="1" t="n">
-        <v>358</v>
-      </c>
-      <c r="B144" t="inlineStr">
-        <is>
-          <t>b'3FHL J2343.6+3439 '</t>
-        </is>
-      </c>
-      <c r="C144" t="n">
-        <v>355.9011535644531</v>
-      </c>
-      <c r="D144" t="n">
-        <v>34.65128707885742</v>
-      </c>
-      <c r="E144" t="n">
-        <v>1451.554321387228</v>
-      </c>
-      <c r="F144" t="n">
-        <v>107.4255305496436</v>
-      </c>
-      <c r="G144" t="n">
-        <v>-26.16964491264739</v>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" s="1" t="n">
-        <v>360</v>
-      </c>
-      <c r="B145" t="inlineStr">
-        <is>
-          <t>b'3FHL J2346.6+0705 '</t>
-        </is>
-      </c>
-      <c r="C145" t="n">
-        <v>356.672607421875</v>
-      </c>
-      <c r="D145" t="n">
-        <v>7.084443092346191</v>
-      </c>
-      <c r="E145" t="n">
-        <v>715.4362988699944</v>
-      </c>
-      <c r="F145" t="n">
-        <v>95.99098400006483</v>
-      </c>
-      <c r="G145" t="n">
-        <v>-52.36756608842526</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Significant Change. Plotting GRS directly from work_vhe instead of copy on voids and GRS plot.
</commit_message>
<xml_diff>
--- a/cel_obj_table.xlsx
+++ b/cel_obj_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G122"/>
+  <dimension ref="A1:G121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,3026 +467,3001 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>b'3FHL J0648.7+1517 '</t>
+          <t>b'3FHL J0730.4+3307 '</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>102.1869277954102</v>
+        <v>112.6081008911133</v>
       </c>
       <c r="D2" t="n">
-        <v>15.28416442871094</v>
+        <v>33.12022399902344</v>
       </c>
       <c r="E2" t="n">
-        <v>743.3176422661688</v>
+        <v>472.4384783695589</v>
       </c>
       <c r="F2" t="n">
-        <v>198.9723667223909</v>
+        <v>185.874446883025</v>
       </c>
       <c r="G2" t="n">
-        <v>6.322407808255858</v>
+        <v>22.04667824967751</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>b'3FHL J0730.4+3307 '</t>
+          <t>b'3FHL J0738.1+1742 '</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>112.6081008911133</v>
+        <v>114.5327682495117</v>
       </c>
       <c r="D3" t="n">
-        <v>33.12022399902344</v>
+        <v>17.71304893493652</v>
       </c>
       <c r="E3" t="n">
-        <v>472.4384783695589</v>
+        <v>1656.947604950266</v>
       </c>
       <c r="F3" t="n">
-        <v>185.874446883025</v>
+        <v>201.8397573898806</v>
       </c>
       <c r="G3" t="n">
-        <v>22.04667824967751</v>
+        <v>18.07539141955594</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>b'3FHL J0738.1+1742 '</t>
+          <t>b'3FHL J0753.1+5354 '</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>114.5327682495117</v>
+        <v>118.2864151000977</v>
       </c>
       <c r="D4" t="n">
-        <v>17.71304893493652</v>
+        <v>53.90745544433594</v>
       </c>
       <c r="E4" t="n">
-        <v>1656.947604950266</v>
+        <v>826.3707136061979</v>
       </c>
       <c r="F4" t="n">
-        <v>201.8397573898806</v>
+        <v>164.1736930995773</v>
       </c>
       <c r="G4" t="n">
-        <v>18.07539141955594</v>
+        <v>30.52602863281245</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>b'3FHL J0753.1+5354 '</t>
+          <t>b'3FHL J0754.8+4822 '</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>118.2864151000977</v>
+        <v>118.7094268798828</v>
       </c>
       <c r="D5" t="n">
-        <v>53.90745544433594</v>
+        <v>48.38185119628906</v>
       </c>
       <c r="E5" t="n">
-        <v>826.3707136061979</v>
+        <v>1489.98505775128</v>
       </c>
       <c r="F5" t="n">
-        <v>164.1736930995773</v>
+        <v>170.5698825442753</v>
       </c>
       <c r="G5" t="n">
-        <v>30.52602863281245</v>
+        <v>30.15412007607718</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>b'3FHL J0754.8+4822 '</t>
+          <t>b'3FHL J0757.1+0957 '</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>118.7094268798828</v>
+        <v>119.2889862060547</v>
       </c>
       <c r="D6" t="n">
-        <v>48.38185119628906</v>
+        <v>9.965688705444336</v>
       </c>
       <c r="E6" t="n">
-        <v>1489.98505775128</v>
+        <v>1081.60187099801</v>
       </c>
       <c r="F6" t="n">
-        <v>170.5698825442753</v>
+        <v>211.2949664982855</v>
       </c>
       <c r="G6" t="n">
-        <v>30.15412007607718</v>
+        <v>19.07671444842579</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>b'3FHL J0757.1+0957 '</t>
+          <t>b'3FHL J0809.7+3457 '</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>119.2889862060547</v>
+        <v>122.4298248291016</v>
       </c>
       <c r="D7" t="n">
-        <v>9.965688705444336</v>
+        <v>34.95800018310547</v>
       </c>
       <c r="E7" t="n">
-        <v>1081.60187099801</v>
+        <v>352.4357721162331</v>
       </c>
       <c r="F7" t="n">
-        <v>211.2949664982855</v>
+        <v>186.4471419042782</v>
       </c>
       <c r="G7" t="n">
-        <v>19.07671444842579</v>
+        <v>30.37076642512884</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>b'3FHL J0809.7+3457 '</t>
+          <t>b'3FHL J0809.8+5218 '</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>122.4298248291016</v>
+        <v>122.4586029052734</v>
       </c>
       <c r="D8" t="n">
-        <v>34.95800018310547</v>
+        <v>52.31039428710938</v>
       </c>
       <c r="E8" t="n">
-        <v>352.4357721162331</v>
+        <v>578.6172947152628</v>
       </c>
       <c r="F8" t="n">
-        <v>186.4471419042782</v>
+        <v>166.2520819406516</v>
       </c>
       <c r="G8" t="n">
-        <v>30.37076642512884</v>
+        <v>32.91232473625846</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>b'3FHL J0809.8+5218 '</t>
+          <t>b'3FHL J0816.4+5739 '</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>122.4586029052734</v>
+        <v>124.1090469360352</v>
       </c>
       <c r="D9" t="n">
-        <v>52.31039428710938</v>
+        <v>57.66443634033203</v>
       </c>
       <c r="E9" t="n">
-        <v>578.6172947152628</v>
+        <v>230.7935158149133</v>
       </c>
       <c r="F9" t="n">
-        <v>166.2520819406516</v>
+        <v>159.8473262299431</v>
       </c>
       <c r="G9" t="n">
-        <v>32.91232473625846</v>
+        <v>33.90405576615215</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>b'3FHL J0816.4+5739 '</t>
+          <t>b'3FHL J0816.9+2050 '</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>124.1090469360352</v>
+        <v>124.2364349365234</v>
       </c>
       <c r="D10" t="n">
-        <v>57.66443634033203</v>
+        <v>20.84729194641113</v>
       </c>
       <c r="E10" t="n">
-        <v>230.7935158149133</v>
+        <v>247.6684183724716</v>
       </c>
       <c r="F10" t="n">
-        <v>159.8473262299431</v>
+        <v>202.4247601227709</v>
       </c>
       <c r="G10" t="n">
-        <v>33.90405576615215</v>
+        <v>27.73866668831735</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>b'3FHL J0816.9+2050 '</t>
+          <t>b'3FHL J0818.2+4222 '</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>124.2364349365234</v>
+        <v>124.5621643066406</v>
       </c>
       <c r="D11" t="n">
-        <v>20.84729194641113</v>
+        <v>42.37668228149414</v>
       </c>
       <c r="E11" t="n">
-        <v>247.6684183724716</v>
+        <v>2015.283911619772</v>
       </c>
       <c r="F11" t="n">
-        <v>202.4247601227709</v>
+        <v>178.2303101447942</v>
       </c>
       <c r="G11" t="n">
-        <v>27.73866668831735</v>
+        <v>33.39832911945414</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>b'3FHL J0818.2+4222 '</t>
+          <t>b'3FHL J0820.9+2353 '</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>124.5621643066406</v>
+        <v>125.2343978881836</v>
       </c>
       <c r="D12" t="n">
-        <v>42.37668228149414</v>
+        <v>23.89204978942871</v>
       </c>
       <c r="E12" t="n">
-        <v>2015.283911619772</v>
+        <v>1579.826051622189</v>
       </c>
       <c r="F12" t="n">
-        <v>178.2303101447942</v>
+        <v>199.510479607579</v>
       </c>
       <c r="G12" t="n">
-        <v>33.39832911945414</v>
+        <v>29.63265514420423</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>b'3FHL J0820.9+2353 '</t>
+          <t>b'3FHL J0825.7+0311 '</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>125.2343978881836</v>
+        <v>126.4462661743164</v>
       </c>
       <c r="D13" t="n">
-        <v>23.89204978942871</v>
+        <v>3.194593906402588</v>
       </c>
       <c r="E13" t="n">
-        <v>1579.826051622189</v>
+        <v>1936.049867434469</v>
       </c>
       <c r="F13" t="n">
-        <v>199.510479607579</v>
+        <v>221.1759682227195</v>
       </c>
       <c r="G13" t="n">
-        <v>29.63265514420423</v>
+        <v>22.39409690992864</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>b'3FHL J0825.7+0311 '</t>
+          <t>b'3FHL J0828.3+4153 '</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>126.4462661743164</v>
+        <v>127.0883941650391</v>
       </c>
       <c r="D14" t="n">
-        <v>3.194593906402588</v>
+        <v>41.89826965332031</v>
       </c>
       <c r="E14" t="n">
-        <v>1936.049867434469</v>
+        <v>927.9669661452913</v>
       </c>
       <c r="F14" t="n">
-        <v>221.1759682227195</v>
+        <v>179.0932631579409</v>
       </c>
       <c r="G14" t="n">
-        <v>22.39409690992864</v>
+        <v>35.19544797408459</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>b'3FHL J0828.3+4153 '</t>
+          <t>b'3FHL J0831.8+0429 '</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>127.0883941650391</v>
+        <v>127.9610137939453</v>
       </c>
       <c r="D15" t="n">
-        <v>41.89826965332031</v>
+        <v>4.495641231536865</v>
       </c>
       <c r="E15" t="n">
-        <v>927.9669661452913</v>
+        <v>723.4123895726626</v>
       </c>
       <c r="F15" t="n">
-        <v>179.0932631579409</v>
+        <v>220.6957511158911</v>
       </c>
       <c r="G15" t="n">
-        <v>35.19544797408459</v>
+        <v>24.338949894984</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>b'3FHL J0831.8+0429 '</t>
+          <t>b'3FHL J0847.2+1134 '</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>127.9610137939453</v>
+        <v>131.8077850341797</v>
       </c>
       <c r="D16" t="n">
-        <v>4.495641231536865</v>
+        <v>11.56671619415283</v>
       </c>
       <c r="E16" t="n">
-        <v>723.4123895726626</v>
+        <v>822.4359267571556</v>
       </c>
       <c r="F16" t="n">
-        <v>220.6957511158911</v>
+        <v>215.4547936858709</v>
       </c>
       <c r="G16" t="n">
-        <v>24.338949894984</v>
+        <v>30.89410316823072</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>b'3FHL J0847.2+1134 '</t>
+          <t>b'3FHL J0849.9+5108 '</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>131.8077850341797</v>
+        <v>132.4937896728516</v>
       </c>
       <c r="D17" t="n">
-        <v>11.56671619415283</v>
+        <v>51.141845703125</v>
       </c>
       <c r="E17" t="n">
-        <v>822.4359267571556</v>
+        <v>2186.405655380971</v>
       </c>
       <c r="F17" t="n">
-        <v>215.4547936858709</v>
+        <v>167.6055794666185</v>
       </c>
       <c r="G17" t="n">
-        <v>30.89410316823072</v>
+        <v>39.1364989957745</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>b'3FHL J0849.9+5108 '</t>
+          <t>b'3FHL J0850.6+3454 '</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>132.4937896728516</v>
+        <v>132.6519165039062</v>
       </c>
       <c r="D18" t="n">
-        <v>51.141845703125</v>
+        <v>34.90697479248047</v>
       </c>
       <c r="E18" t="n">
-        <v>2186.405655380971</v>
+        <v>606.9745772102617</v>
       </c>
       <c r="F18" t="n">
-        <v>167.6055794666185</v>
+        <v>188.4881336399034</v>
       </c>
       <c r="G18" t="n">
-        <v>39.1364989957745</v>
+        <v>38.57761892185869</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>b'3FHL J0850.6+3454 '</t>
+          <t>b'3FHL J0854.8+2006 '</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>132.6519165039062</v>
+        <v>133.7121429443359</v>
       </c>
       <c r="D19" t="n">
-        <v>34.90697479248047</v>
+        <v>20.10042953491211</v>
       </c>
       <c r="E19" t="n">
-        <v>606.9745772102617</v>
+        <v>1232.001690836247</v>
       </c>
       <c r="F19" t="n">
-        <v>188.4881336399034</v>
+        <v>206.8248045598298</v>
       </c>
       <c r="G19" t="n">
-        <v>38.57761892185869</v>
+        <v>35.82570420018077</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>b'3FHL J0854.8+2006 '</t>
+          <t>b'3FHL J0908.9+2311 '</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>133.7121429443359</v>
+        <v>137.2379302978516</v>
       </c>
       <c r="D20" t="n">
-        <v>20.10042953491211</v>
+        <v>23.19077682495117</v>
       </c>
       <c r="E20" t="n">
-        <v>1232.001690836247</v>
+        <v>916.3139966249578</v>
       </c>
       <c r="F20" t="n">
-        <v>206.8248045598298</v>
+        <v>204.4006996128279</v>
       </c>
       <c r="G20" t="n">
-        <v>35.82570420018077</v>
+        <v>39.90343163897078</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>b'3FHL J0908.9+2311 '</t>
+          <t>b'3FHL J0910.5+3329 '</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>137.2379302978516</v>
+        <v>137.62841796875</v>
       </c>
       <c r="D21" t="n">
-        <v>23.19077682495117</v>
+        <v>33.48870086669922</v>
       </c>
       <c r="E21" t="n">
-        <v>916.3139966249578</v>
+        <v>1408.222189015081</v>
       </c>
       <c r="F21" t="n">
-        <v>204.4006996128279</v>
+        <v>191.1184013879268</v>
       </c>
       <c r="G21" t="n">
-        <v>39.90343163897078</v>
+        <v>42.44470192240891</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>b'3FHL J0910.5+3329 '</t>
+          <t>b'3FHL J0912.4+1555 '</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>137.62841796875</v>
+        <v>138.1239929199219</v>
       </c>
       <c r="D22" t="n">
-        <v>33.48870086669922</v>
+        <v>15.9302806854248</v>
       </c>
       <c r="E22" t="n">
-        <v>1408.222189015081</v>
+        <v>873.4307914196993</v>
       </c>
       <c r="F22" t="n">
-        <v>191.1184013879268</v>
+        <v>213.5799215954228</v>
       </c>
       <c r="G22" t="n">
-        <v>42.44470192240891</v>
+        <v>38.26181930326724</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>b'3FHL J0912.4+1555 '</t>
+          <t>b'3FHL J0930.4+4952 '</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>138.1239929199219</v>
+        <v>142.6244659423828</v>
       </c>
       <c r="D23" t="n">
-        <v>15.9302806854248</v>
+        <v>49.87545776367188</v>
       </c>
       <c r="E23" t="n">
-        <v>873.4307914196993</v>
+        <v>775.0615269997014</v>
       </c>
       <c r="F23" t="n">
-        <v>213.5799215954228</v>
+        <v>168.0950099107559</v>
       </c>
       <c r="G23" t="n">
-        <v>38.26181930326724</v>
+        <v>45.68697248424435</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>b'3FHL J0930.4+4952 '</t>
+          <t>b'3FHL J0940.5+6149 '</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>142.6244659423828</v>
+        <v>145.1408081054688</v>
       </c>
       <c r="D24" t="n">
-        <v>49.87545776367188</v>
+        <v>61.8179817199707</v>
       </c>
       <c r="E24" t="n">
-        <v>775.0615269997014</v>
+        <v>869.5202016942904</v>
       </c>
       <c r="F24" t="n">
-        <v>168.0950099107559</v>
+        <v>151.5795904696888</v>
       </c>
       <c r="G24" t="n">
-        <v>45.68697248424435</v>
+        <v>43.2124825532333</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>b'3FHL J0940.5+6149 '</t>
+          <t>b'3FHL J0946.2+0104 '</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>145.1408081054688</v>
+        <v>146.5630645751953</v>
       </c>
       <c r="D25" t="n">
-        <v>61.8179817199707</v>
+        <v>1.072644710540771</v>
       </c>
       <c r="E25" t="n">
-        <v>869.5202016942904</v>
+        <v>2167.296925661129</v>
       </c>
       <c r="F25" t="n">
-        <v>151.5795904696888</v>
+        <v>235.3603953607503</v>
       </c>
       <c r="G25" t="n">
-        <v>43.2124825532333</v>
+        <v>38.56086142877915</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>b'3FHL J0946.2+0104 '</t>
+          <t>b'3FHL J0950.3+4553 '</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>146.5630645751953</v>
+        <v>147.5764617919922</v>
       </c>
       <c r="D26" t="n">
-        <v>1.072644710540771</v>
+        <v>45.89204025268555</v>
       </c>
       <c r="E26" t="n">
-        <v>2167.296925661129</v>
+        <v>1569.235152018134</v>
       </c>
       <c r="F26" t="n">
-        <v>235.3603953607503</v>
+        <v>172.8821816193272</v>
       </c>
       <c r="G26" t="n">
-        <v>38.56086142877915</v>
+        <v>49.75183136937554</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>b'3FHL J0950.3+4553 '</t>
+          <t>b'3FHL J0954.2+4912 '</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>147.5764617919922</v>
+        <v>148.5668640136719</v>
       </c>
       <c r="D27" t="n">
-        <v>45.89204025268555</v>
+        <v>49.21414566040039</v>
       </c>
       <c r="E27" t="n">
-        <v>1569.235152018134</v>
+        <v>1501.744593228529</v>
       </c>
       <c r="F27" t="n">
-        <v>172.8821816193272</v>
+        <v>167.6515683277358</v>
       </c>
       <c r="G27" t="n">
-        <v>49.75183136937554</v>
+        <v>49.58651425014828</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>b'3FHL J0954.2+4912 '</t>
+          <t>b'3FHL J1001.2+2910 '</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>148.5668640136719</v>
+        <v>150.3133544921875</v>
       </c>
       <c r="D28" t="n">
-        <v>49.21414566040039</v>
+        <v>29.1705379486084</v>
       </c>
       <c r="E28" t="n">
-        <v>1501.744593228529</v>
+        <v>2106.343909760358</v>
       </c>
       <c r="F28" t="n">
-        <v>167.6515683277358</v>
+        <v>199.5504344044182</v>
       </c>
       <c r="G28" t="n">
-        <v>49.58651425014828</v>
+        <v>52.63416273614697</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>b'3FHL J1001.2+2910 '</t>
+          <t>b'3FHL J1006.9+3455 '</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>150.3133544921875</v>
+        <v>151.7499389648438</v>
       </c>
       <c r="D29" t="n">
-        <v>29.1705379486084</v>
+        <v>34.92112350463867</v>
       </c>
       <c r="E29" t="n">
-        <v>2106.343909760358</v>
+        <v>2277.828672355331</v>
       </c>
       <c r="F29" t="n">
-        <v>199.5504344044182</v>
+        <v>190.0282006580422</v>
       </c>
       <c r="G29" t="n">
-        <v>52.63416273614697</v>
+        <v>54.17913076411402</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>b'3FHL J1006.9+3455 '</t>
+          <t>b'3FHL J1008.0+0622 '</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>151.7499389648438</v>
+        <v>152.0041351318359</v>
       </c>
       <c r="D30" t="n">
-        <v>34.92112350463867</v>
+        <v>6.373631954193115</v>
       </c>
       <c r="E30" t="n">
-        <v>2277.828672355331</v>
+        <v>2395.304963072071</v>
       </c>
       <c r="F30" t="n">
-        <v>190.0282006580422</v>
+        <v>233.50096097581</v>
       </c>
       <c r="G30" t="n">
-        <v>54.17913076411402</v>
+        <v>46.02256622120216</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>b'3FHL J1008.0+0622 '</t>
+          <t>b'3FHL J1012.6+4228 '</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>152.0041351318359</v>
+        <v>153.1730499267578</v>
       </c>
       <c r="D31" t="n">
-        <v>6.373631954193115</v>
+        <v>42.48298263549805</v>
       </c>
       <c r="E31" t="n">
-        <v>2395.304963072071</v>
+        <v>1447.954363211065</v>
       </c>
       <c r="F31" t="n">
-        <v>233.50096097581</v>
+        <v>176.9216254086938</v>
       </c>
       <c r="G31" t="n">
-        <v>46.02256622120216</v>
+        <v>54.39503658450563</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>b'3FHL J1012.6+4228 '</t>
+          <t>b'3FHL J1015.0+4926 '</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>153.1730499267578</v>
+        <v>153.7693176269531</v>
       </c>
       <c r="D32" t="n">
-        <v>42.48298263549805</v>
+        <v>49.43538665771484</v>
       </c>
       <c r="E32" t="n">
-        <v>1447.954363211065</v>
+        <v>873.4307914196993</v>
       </c>
       <c r="F32" t="n">
-        <v>176.9216254086938</v>
+        <v>165.5301745409713</v>
       </c>
       <c r="G32" t="n">
-        <v>54.39503658450563</v>
+        <v>52.7128041733207</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>b'3FHL J1015.0+4926 '</t>
+          <t>b'3FHL J1026.9+0608 '</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>153.7693176269531</v>
+        <v>156.7403564453125</v>
       </c>
       <c r="D33" t="n">
-        <v>49.43538665771484</v>
+        <v>6.142007350921631</v>
       </c>
       <c r="E33" t="n">
-        <v>873.4307914196993</v>
+        <v>1743.428171899722</v>
       </c>
       <c r="F33" t="n">
-        <v>165.5301745409713</v>
+        <v>237.7476753956505</v>
       </c>
       <c r="G33" t="n">
-        <v>52.7128041733207</v>
+        <v>49.78141165294394</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>b'3FHL J1026.9+0608 '</t>
+          <t>b'3FHL J1027.5+6317 '</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>156.7403564453125</v>
+        <v>156.8891754150391</v>
       </c>
       <c r="D34" t="n">
-        <v>6.142007350921631</v>
+        <v>63.29279327392578</v>
       </c>
       <c r="E34" t="n">
-        <v>1743.428171899722</v>
+        <v>2183.225532378438</v>
       </c>
       <c r="F34" t="n">
-        <v>237.7476753956505</v>
+        <v>145.6929541877977</v>
       </c>
       <c r="G34" t="n">
-        <v>49.78141165294394</v>
+        <v>46.97503063890456</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>b'3FHL J1027.5+6317 '</t>
+          <t>b'3FHL J1031.3+5053 '</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>156.8891754150391</v>
+        <v>157.8328399658203</v>
       </c>
       <c r="D35" t="n">
-        <v>63.29279327392578</v>
+        <v>50.88592529296875</v>
       </c>
       <c r="E35" t="n">
-        <v>2183.225532378438</v>
+        <v>1433.534310193219</v>
       </c>
       <c r="F35" t="n">
-        <v>145.6929541877977</v>
+        <v>161.4466616146051</v>
       </c>
       <c r="G35" t="n">
-        <v>46.97503063890456</v>
+        <v>54.44603636948661</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>b'3FHL J1031.3+5053 '</t>
+          <t>b'3FHL J1032.7+3737 '</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>157.8328399658203</v>
+        <v>158.1970977783203</v>
       </c>
       <c r="D36" t="n">
-        <v>50.88592529296875</v>
+        <v>37.62113952636719</v>
       </c>
       <c r="E36" t="n">
-        <v>1433.534310193219</v>
+        <v>2008.723036449022</v>
       </c>
       <c r="F36" t="n">
-        <v>161.4466616146051</v>
+        <v>184.2725657102087</v>
       </c>
       <c r="G36" t="n">
-        <v>54.44603636948661</v>
+        <v>59.11119534742926</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>b'3FHL J1032.7+3737 '</t>
+          <t>b'3FHL J1041.7+3900 '</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>158.1970977783203</v>
+        <v>160.4421539306641</v>
       </c>
       <c r="D37" t="n">
-        <v>37.62113952636719</v>
+        <v>39.00973129272461</v>
       </c>
       <c r="E37" t="n">
-        <v>2008.723036449022</v>
+        <v>865.6075942787213</v>
       </c>
       <c r="F37" t="n">
-        <v>184.2725657102087</v>
+        <v>180.851954975237</v>
       </c>
       <c r="G37" t="n">
-        <v>59.11119534742926</v>
+        <v>60.55262642715537</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>b'3FHL J1041.7+3900 '</t>
+          <t>b'3FHL J1043.1+2409 '</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>160.4421539306641</v>
+        <v>160.7764892578125</v>
       </c>
       <c r="D38" t="n">
-        <v>39.00973129272461</v>
+        <v>24.15542984008789</v>
       </c>
       <c r="E38" t="n">
-        <v>865.6075942787213</v>
+        <v>2112.791679272088</v>
       </c>
       <c r="F38" t="n">
-        <v>180.851954975237</v>
+        <v>211.5515502940325</v>
       </c>
       <c r="G38" t="n">
-        <v>60.55262642715537</v>
+        <v>61.00195275957411</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>b'3FHL J1043.1+2409 '</t>
+          <t>b'3FHL J1051.4+3942 '</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>160.7764892578125</v>
+        <v>162.8575439453125</v>
       </c>
       <c r="D39" t="n">
-        <v>24.15542984008789</v>
+        <v>39.70672988891602</v>
       </c>
       <c r="E39" t="n">
-        <v>2112.791679272088</v>
+        <v>1909.393880329576</v>
       </c>
       <c r="F39" t="n">
-        <v>211.5515502940325</v>
+        <v>178.3920516037439</v>
       </c>
       <c r="G39" t="n">
-        <v>61.00195275957411</v>
+        <v>62.16010539961907</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>b'3FHL J1051.4+3942 '</t>
+          <t>b'3FHL J1053.6+4930 '</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>162.8575439453125</v>
+        <v>163.4012298583984</v>
       </c>
       <c r="D40" t="n">
-        <v>39.70672988891602</v>
+        <v>49.50532150268555</v>
       </c>
       <c r="E40" t="n">
-        <v>1909.393880329576</v>
+        <v>586.7293479424766</v>
       </c>
       <c r="F40" t="n">
-        <v>178.3920516037439</v>
+        <v>160.2472928171692</v>
       </c>
       <c r="G40" t="n">
-        <v>62.16010539961907</v>
+        <v>58.20941647675482</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>b'3FHL J1053.6+4930 '</t>
+          <t>b'3FHL J1058.6+5628 '</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>163.4012298583984</v>
+        <v>164.6645202636719</v>
       </c>
       <c r="D41" t="n">
-        <v>49.50532150268555</v>
+        <v>56.46826171875</v>
       </c>
       <c r="E41" t="n">
-        <v>586.7293479424766</v>
+        <v>598.8824976040644</v>
       </c>
       <c r="F41" t="n">
-        <v>160.2472928171692</v>
+        <v>149.5898498865417</v>
       </c>
       <c r="G41" t="n">
-        <v>58.20941647675482</v>
+        <v>54.42879075775696</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>b'3FHL J1058.6+5628 '</t>
+          <t>b'3FHL J1100.3+4020 '</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>164.6645202636719</v>
+        <v>165.0803070068359</v>
       </c>
       <c r="D42" t="n">
-        <v>56.46826171875</v>
+        <v>40.3358268737793</v>
       </c>
       <c r="E42" t="n">
-        <v>598.8824976040644</v>
+        <v>924.0846438011745</v>
       </c>
       <c r="F42" t="n">
-        <v>149.5898498865417</v>
+        <v>175.8469476326254</v>
       </c>
       <c r="G42" t="n">
-        <v>54.42879075775696</v>
+        <v>63.555059895797</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>b'3FHL J1100.3+4020 '</t>
+          <t>b'3FHL J1104.4+3812 '</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>165.0803070068359</v>
+        <v>166.1207580566406</v>
       </c>
       <c r="D43" t="n">
-        <v>40.3358268737793</v>
+        <v>38.20518112182617</v>
       </c>
       <c r="E43" t="n">
-        <v>924.0846438011745</v>
+        <v>128.9003855881938</v>
       </c>
       <c r="F43" t="n">
-        <v>175.8469476326254</v>
+        <v>179.8357877680561</v>
       </c>
       <c r="G43" t="n">
-        <v>63.555059895797</v>
+        <v>65.03781332953814</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>b'3FHL J1104.4+3812 '</t>
+          <t>b'3FHL J1105.8+3944 '</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>166.1207580566406</v>
+        <v>166.4540252685547</v>
       </c>
       <c r="D44" t="n">
-        <v>38.20518112182617</v>
+        <v>39.74899673461914</v>
       </c>
       <c r="E44" t="n">
-        <v>128.9003855881938</v>
+        <v>418.8482280609101</v>
       </c>
       <c r="F44" t="n">
-        <v>179.8357877680561</v>
+        <v>176.2092588270897</v>
       </c>
       <c r="G44" t="n">
-        <v>65.03781332953814</v>
+        <v>64.74895803570412</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>b'3FHL J1105.8+3944 '</t>
+          <t>b'3FHL J1107.8+1501 '</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>166.4540252685547</v>
+        <v>166.9655914306641</v>
       </c>
       <c r="D45" t="n">
-        <v>39.74899673461914</v>
+        <v>15.02733516693115</v>
       </c>
       <c r="E45" t="n">
-        <v>418.8482280609101</v>
+        <v>2240.185974418625</v>
       </c>
       <c r="F45" t="n">
-        <v>176.2092588270897</v>
+        <v>234.34727958246</v>
       </c>
       <c r="G45" t="n">
-        <v>64.74895803570412</v>
+        <v>63.06038848548737</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>b'3FHL J1107.8+1501 '</t>
+          <t>b'3FHL J1109.7+3735 '</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>166.9655914306641</v>
+        <v>167.4311370849609</v>
       </c>
       <c r="D46" t="n">
-        <v>15.02733516693115</v>
+        <v>37.58807754516602</v>
       </c>
       <c r="E46" t="n">
-        <v>2240.185974418625</v>
+        <v>1563.657198577747</v>
       </c>
       <c r="F46" t="n">
-        <v>234.34727958246</v>
+        <v>180.457347654663</v>
       </c>
       <c r="G46" t="n">
-        <v>63.06038848548737</v>
+        <v>66.2143548292574</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>b'3FHL J1109.7+3735 '</t>
+          <t>b'3FHL J1117.0+2014 '</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>167.4311370849609</v>
+        <v>169.2679595947266</v>
       </c>
       <c r="D47" t="n">
-        <v>37.58807754516602</v>
+        <v>20.23810386657715</v>
       </c>
       <c r="E47" t="n">
-        <v>1563.657198577747</v>
+        <v>578.6172947152628</v>
       </c>
       <c r="F47" t="n">
-        <v>180.457347654663</v>
+        <v>225.5716267064807</v>
       </c>
       <c r="G47" t="n">
-        <v>66.2143548292574</v>
+        <v>67.36670331755562</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>b'3FHL J1117.0+2014 '</t>
+          <t>b'3FHL J1120.8+4212 '</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>169.2679595947266</v>
+        <v>170.2008819580078</v>
       </c>
       <c r="D48" t="n">
-        <v>20.23810386657715</v>
+        <v>42.20166015625</v>
       </c>
       <c r="E48" t="n">
-        <v>578.6172947152628</v>
+        <v>521.6104982541038</v>
       </c>
       <c r="F48" t="n">
-        <v>225.5716267064807</v>
+        <v>167.856902782118</v>
       </c>
       <c r="G48" t="n">
-        <v>67.36670331755562</v>
+        <v>66.16418823817627</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>b'3FHL J1120.8+4212 '</t>
+          <t>b'3FHL J1131.6+5809 '</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>170.2008819580078</v>
+        <v>172.9062042236328</v>
       </c>
       <c r="D49" t="n">
-        <v>42.20166015625</v>
+        <v>58.16561508178711</v>
       </c>
       <c r="E49" t="n">
-        <v>521.6104982541038</v>
+        <v>1429.924347323077</v>
       </c>
       <c r="F49" t="n">
-        <v>167.856902782118</v>
+        <v>141.6893921444634</v>
       </c>
       <c r="G49" t="n">
-        <v>66.16418823817627</v>
+        <v>55.9604528362288</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>b'3FHL J1131.6+5809 '</t>
+          <t>b'3FHL J1136.8+2549 '</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>172.9062042236328</v>
+        <v>174.2185363769531</v>
       </c>
       <c r="D50" t="n">
-        <v>58.16561508178711</v>
+        <v>25.8327808380127</v>
       </c>
       <c r="E50" t="n">
-        <v>1429.924347323077</v>
+        <v>651.3386580792431</v>
       </c>
       <c r="F50" t="n">
-        <v>141.6893921444634</v>
+        <v>213.1465867327724</v>
       </c>
       <c r="G50" t="n">
-        <v>55.9604528362288</v>
+        <v>73.27986298713279</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>b'3FHL J1136.8+2549 '</t>
+          <t>b'3FHL J1140.5+1528 '</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>174.2185363769531</v>
+        <v>175.1320648193359</v>
       </c>
       <c r="D51" t="n">
-        <v>25.8327808380127</v>
+        <v>15.48001480102539</v>
       </c>
       <c r="E51" t="n">
-        <v>651.3386580792431</v>
+        <v>997.5030593997925</v>
       </c>
       <c r="F51" t="n">
-        <v>213.1465867327724</v>
+        <v>244.6038972738466</v>
       </c>
       <c r="G51" t="n">
-        <v>73.27986298713279</v>
+        <v>69.83077528557813</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>b'3FHL J1140.5+1528 '</t>
+          <t>b'3FHL J1142.0+1546 '</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>175.1320648193359</v>
+        <v>175.5173187255859</v>
       </c>
       <c r="D52" t="n">
-        <v>15.48001480102539</v>
+        <v>15.77690410614014</v>
       </c>
       <c r="E52" t="n">
-        <v>997.5030593997925</v>
+        <v>1205.915061750614</v>
       </c>
       <c r="F52" t="n">
-        <v>244.6038972738466</v>
+        <v>244.5908969669972</v>
       </c>
       <c r="G52" t="n">
-        <v>69.83077528557813</v>
+        <v>70.30592729967964</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>b'3FHL J1142.0+1546 '</t>
+          <t>b'3FHL J1143.1+6121 '</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>175.5173187255859</v>
+        <v>175.7978515625</v>
       </c>
       <c r="D53" t="n">
-        <v>15.77690410614014</v>
+        <v>61.35290145874023</v>
       </c>
       <c r="E53" t="n">
-        <v>1205.915061750614</v>
+        <v>209.6566093130006</v>
       </c>
       <c r="F53" t="n">
-        <v>244.5908969669972</v>
+        <v>136.7459514614812</v>
       </c>
       <c r="G53" t="n">
-        <v>70.30592729967964</v>
+        <v>53.90689117248857</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>b'3FHL J1143.1+6121 '</t>
+          <t>b'3FHL J1145.0+1935 '</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>175.7978515625</v>
+        <v>176.2684783935547</v>
       </c>
       <c r="D54" t="n">
-        <v>61.35290145874023</v>
+        <v>19.5903205871582</v>
       </c>
       <c r="E54" t="n">
-        <v>209.6566093130006</v>
+        <v>93.48446529540507</v>
       </c>
       <c r="F54" t="n">
-        <v>136.7459514614812</v>
+        <v>235.771105621029</v>
       </c>
       <c r="G54" t="n">
-        <v>53.90689117248857</v>
+        <v>73.02859819966865</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>b'3FHL J1145.0+1935 '</t>
+          <t>b'3FHL J1150.3+2418 '</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>176.2684783935547</v>
+        <v>177.5877227783203</v>
       </c>
       <c r="D55" t="n">
-        <v>19.5903205871582</v>
+        <v>24.30084228515625</v>
       </c>
       <c r="E55" t="n">
-        <v>93.48446529540507</v>
+        <v>826.3707136061979</v>
       </c>
       <c r="F55" t="n">
-        <v>235.771105621029</v>
+        <v>221.1457388558182</v>
       </c>
       <c r="G55" t="n">
-        <v>73.02859819966865</v>
+        <v>75.96302613210874</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>b'3FHL J1150.3+2418 '</t>
+          <t>b'3FHL J1153.2+4929 '</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>177.5877227783203</v>
+        <v>178.3224639892578</v>
       </c>
       <c r="D56" t="n">
-        <v>24.30084228515625</v>
+        <v>49.49262237548828</v>
       </c>
       <c r="E56" t="n">
-        <v>826.3707136061979</v>
+        <v>1335.3602067056</v>
       </c>
       <c r="F56" t="n">
-        <v>221.1457388558182</v>
+        <v>145.6204816776282</v>
       </c>
       <c r="G56" t="n">
-        <v>75.96302613210874</v>
+        <v>64.99564919843898</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>b'3FHL J1153.2+4929 '</t>
+          <t>b'3FHL J1203.1+6030 '</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>178.3224639892578</v>
+        <v>180.7808227539062</v>
       </c>
       <c r="D57" t="n">
-        <v>49.49262237548828</v>
+        <v>60.51219177246094</v>
       </c>
       <c r="E57" t="n">
-        <v>1335.3602067056</v>
+        <v>277.125303444809</v>
       </c>
       <c r="F57" t="n">
-        <v>145.6204816776282</v>
+        <v>133.4418834029724</v>
       </c>
       <c r="G57" t="n">
-        <v>64.99564919843898</v>
+        <v>55.61926798865239</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>b'3FHL J1203.1+6030 '</t>
+          <t>b'3FHL J1208.1+6120 '</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>180.7808227539062</v>
+        <v>182.0427551269531</v>
       </c>
       <c r="D58" t="n">
-        <v>60.51219177246094</v>
+        <v>61.34061431884766</v>
       </c>
       <c r="E58" t="n">
-        <v>277.125303444809</v>
+        <v>1115.723809237682</v>
       </c>
       <c r="F58" t="n">
-        <v>133.4418834029724</v>
+        <v>131.9651880062851</v>
       </c>
       <c r="G58" t="n">
-        <v>55.61926798865239</v>
+        <v>55.02232038849426</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>b'3FHL J1208.1+6120 '</t>
+          <t>b'3FHL J1216.0-0242 '</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>182.0427551269531</v>
+        <v>184.0193023681641</v>
       </c>
       <c r="D59" t="n">
-        <v>61.34061431884766</v>
+        <v>-2.713768005371094</v>
       </c>
       <c r="E59" t="n">
-        <v>1115.723809237682</v>
+        <v>1426.312274688342</v>
       </c>
       <c r="F59" t="n">
-        <v>131.9651880062851</v>
+        <v>285.6103354390478</v>
       </c>
       <c r="G59" t="n">
-        <v>55.02232038849426</v>
+        <v>58.96364214349016</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>b'3FHL J1216.0-0242 '</t>
+          <t>b'3FHL J1217.9+3006 '</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>184.0193023681641</v>
+        <v>184.4772338867188</v>
       </c>
       <c r="D60" t="n">
-        <v>-2.713768005371094</v>
+        <v>30.11482238769531</v>
       </c>
       <c r="E60" t="n">
-        <v>1426.312274688342</v>
+        <v>546.0896141426656</v>
       </c>
       <c r="F60" t="n">
-        <v>285.6103354390478</v>
+        <v>188.8666537572836</v>
       </c>
       <c r="G60" t="n">
-        <v>58.96364214349016</v>
+        <v>82.06187773446577</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>b'3FHL J1217.9+3006 '</t>
+          <t>b'3FHL J1218.0-0028 '</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>184.4772338867188</v>
+        <v>184.51953125</v>
       </c>
       <c r="D61" t="n">
-        <v>30.11482238769531</v>
+        <v>-0.4782386422157288</v>
       </c>
       <c r="E61" t="n">
-        <v>546.0896141426656</v>
+        <v>1639.503972536957</v>
       </c>
       <c r="F61" t="n">
-        <v>188.8666537572836</v>
+        <v>285.3804349262129</v>
       </c>
       <c r="G61" t="n">
-        <v>82.06187773446577</v>
+        <v>61.25154181229235</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>b'3FHL J1218.0-0028 '</t>
+          <t>b'3FHL J1219.7-0312 '</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>184.51953125</v>
+        <v>184.9271392822266</v>
       </c>
       <c r="D62" t="n">
-        <v>-0.4782386422157288</v>
+        <v>-3.212921857833862</v>
       </c>
       <c r="E62" t="n">
-        <v>1639.503972536957</v>
+        <v>1205.915061750614</v>
       </c>
       <c r="F62" t="n">
-        <v>285.3804349262129</v>
+        <v>287.5483319154165</v>
       </c>
       <c r="G62" t="n">
-        <v>61.25154181229235</v>
+        <v>58.70790553974744</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>b'3FHL J1219.7-0312 '</t>
+          <t>b'3FHL J1221.3+3010 '</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>184.9271392822266</v>
+        <v>185.3371734619141</v>
       </c>
       <c r="D63" t="n">
-        <v>-3.212921857833862</v>
+        <v>30.16693115234375</v>
       </c>
       <c r="E63" t="n">
-        <v>1205.915061750614</v>
+        <v>763.1726232934241</v>
       </c>
       <c r="F63" t="n">
-        <v>287.5483319154165</v>
+        <v>186.4431504600458</v>
       </c>
       <c r="G63" t="n">
-        <v>58.70790553974744</v>
+        <v>82.7350715996196</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>b'3FHL J1221.3+3010 '</t>
+          <t>b'3FHL J1221.5+2813 '</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>185.3371734619141</v>
+        <v>185.3848114013672</v>
       </c>
       <c r="D64" t="n">
-        <v>30.16693115234375</v>
+        <v>28.23212242126465</v>
       </c>
       <c r="E64" t="n">
-        <v>763.1726232934241</v>
+        <v>431.2447065513599</v>
       </c>
       <c r="F64" t="n">
-        <v>186.4431504600458</v>
+        <v>201.7391806851846</v>
       </c>
       <c r="G64" t="n">
-        <v>82.7350715996196</v>
+        <v>83.29053790221776</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>b'3FHL J1221.5+2813 '</t>
+          <t>b'3FHL J1224.4+2436 '</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>185.3848114013672</v>
+        <v>186.1085205078125</v>
       </c>
       <c r="D65" t="n">
-        <v>28.23212242126465</v>
+        <v>24.6070442199707</v>
       </c>
       <c r="E65" t="n">
-        <v>431.2447065513599</v>
+        <v>900.7483492023172</v>
       </c>
       <c r="F65" t="n">
-        <v>201.7391806851846</v>
+        <v>233.9729892145359</v>
       </c>
       <c r="G65" t="n">
-        <v>83.29053790221776</v>
+        <v>83.42441521408441</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>b'3FHL J1224.4+2436 '</t>
+          <t>b'3FHL J1224.9+2122 '</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>186.1085205078125</v>
+        <v>186.2270355224609</v>
       </c>
       <c r="D66" t="n">
-        <v>24.6070442199707</v>
+        <v>21.38190269470215</v>
       </c>
       <c r="E66" t="n">
-        <v>900.7483492023172</v>
+        <v>1691.687106632469</v>
       </c>
       <c r="F66" t="n">
-        <v>233.9729892145359</v>
+        <v>255.0624608818417</v>
       </c>
       <c r="G66" t="n">
-        <v>83.42441521408441</v>
+        <v>81.66152573596764</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>b'3FHL J1224.9+2122 '</t>
+          <t>b'3FHL J1229.2+0201 '</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>186.2270355224609</v>
+        <v>187.3038330078125</v>
       </c>
       <c r="D67" t="n">
-        <v>21.38190269470215</v>
+        <v>2.024992942810059</v>
       </c>
       <c r="E67" t="n">
-        <v>1691.687106632469</v>
+        <v>659.3789000935117</v>
       </c>
       <c r="F67" t="n">
-        <v>255.0624608818417</v>
+        <v>290.0221226405291</v>
       </c>
       <c r="G67" t="n">
-        <v>81.66152573596764</v>
+        <v>64.33829691205085</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>b'3FHL J1229.2+0201 '</t>
+          <t>b'3FHL J1230.2+2517 '</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>187.3038330078125</v>
+        <v>187.5732727050781</v>
       </c>
       <c r="D68" t="n">
-        <v>2.024992942810059</v>
+        <v>25.29787635803223</v>
       </c>
       <c r="E68" t="n">
-        <v>659.3789000935117</v>
+        <v>566.434356575713</v>
       </c>
       <c r="F68" t="n">
-        <v>290.0221226405291</v>
+        <v>232.8530732554522</v>
       </c>
       <c r="G68" t="n">
-        <v>64.33829691205085</v>
+        <v>84.91711617677194</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>b'3FHL J1230.2+2517 '</t>
+          <t>b'3FHL J1230.8+1223 '</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>187.5732727050781</v>
+        <v>187.7033386230469</v>
       </c>
       <c r="D69" t="n">
-        <v>25.29787635803223</v>
+        <v>12.38887977600098</v>
       </c>
       <c r="E69" t="n">
-        <v>566.434356575713</v>
+        <v>18.50588103089174</v>
       </c>
       <c r="F69" t="n">
-        <v>232.8530732554522</v>
+        <v>283.7712082555389</v>
       </c>
       <c r="G69" t="n">
-        <v>84.91711617677194</v>
+        <v>74.48825666506053</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>b'3FHL J1230.8+1223 '</t>
+          <t>b'3FHL J1231.4+1422 '</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>187.7033386230469</v>
+        <v>187.8662414550781</v>
       </c>
       <c r="D70" t="n">
-        <v>12.38887977600098</v>
+        <v>14.3680305480957</v>
       </c>
       <c r="E70" t="n">
-        <v>18.50588103089174</v>
+        <v>1043.496525858729</v>
       </c>
       <c r="F70" t="n">
-        <v>283.7712082555389</v>
+        <v>281.8921172763349</v>
       </c>
       <c r="G70" t="n">
-        <v>74.48825666506053</v>
+        <v>76.41707829778731</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>b'3FHL J1231.4+1422 '</t>
+          <t>b'3FHL J1231.6+6415 '</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>187.8662414550781</v>
+        <v>187.9054565429688</v>
       </c>
       <c r="D71" t="n">
-        <v>14.3680305480957</v>
+        <v>64.26630401611328</v>
       </c>
       <c r="E71" t="n">
-        <v>1043.496525858729</v>
+        <v>679.4444413307867</v>
       </c>
       <c r="F71" t="n">
-        <v>281.8921172763349</v>
+        <v>126.4813572877882</v>
       </c>
       <c r="G71" t="n">
-        <v>76.41707829778731</v>
+        <v>52.72516890602747</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>b'3FHL J1231.6+6415 '</t>
+          <t>b'3FHL J1231.7+2847 '</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>187.9054565429688</v>
+        <v>187.9381866455078</v>
       </c>
       <c r="D72" t="n">
-        <v>64.26630401611328</v>
+        <v>28.79290008544922</v>
       </c>
       <c r="E72" t="n">
-        <v>679.4444413307867</v>
+        <v>968.4201348245213</v>
       </c>
       <c r="F72" t="n">
-        <v>126.4813572877882</v>
+        <v>190.8352813272477</v>
       </c>
       <c r="G72" t="n">
-        <v>52.72516890602747</v>
+        <v>85.34586086634012</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>b'3FHL J1231.7+2847 '</t>
+          <t>b'3FHL J1247.0+4421 '</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>187.9381866455078</v>
+        <v>191.7523803710938</v>
       </c>
       <c r="D73" t="n">
-        <v>28.79290008544922</v>
+        <v>44.35237503051758</v>
       </c>
       <c r="E73" t="n">
-        <v>968.4201348245213</v>
+        <v>2240.185974418625</v>
       </c>
       <c r="F73" t="n">
-        <v>190.8352813272477</v>
+        <v>125.6027117904971</v>
       </c>
       <c r="G73" t="n">
-        <v>85.34586086634012</v>
+        <v>72.75290303465637</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>b'3FHL J1247.0+4421 '</t>
+          <t>b'3FHL J1253.7+0328 '</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>191.7523803710938</v>
+        <v>193.4472503662109</v>
       </c>
       <c r="D74" t="n">
-        <v>44.35237503051758</v>
+        <v>3.473009824752808</v>
       </c>
       <c r="E74" t="n">
-        <v>2240.185974418625</v>
+        <v>281.3257125002922</v>
       </c>
       <c r="F74" t="n">
-        <v>125.6027117904971</v>
+        <v>304.3938914960014</v>
       </c>
       <c r="G74" t="n">
-        <v>72.75290303465637</v>
+        <v>66.33808457924333</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>b'3FHL J1253.7+0328 '</t>
+          <t>b'3FHL J1254.4+2210 '</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>193.4472503662109</v>
+        <v>193.6058959960938</v>
       </c>
       <c r="D75" t="n">
-        <v>3.473009824752808</v>
+        <v>22.18258476257324</v>
       </c>
       <c r="E75" t="n">
-        <v>281.3257125002922</v>
+        <v>1946.014319805091</v>
       </c>
       <c r="F75" t="n">
-        <v>304.3938914960014</v>
+        <v>310.9003864000454</v>
       </c>
       <c r="G75" t="n">
-        <v>66.33808457924333</v>
+        <v>85.00807392479871</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>b'3FHL J1254.4+2210 '</t>
+          <t>b'3FHL J1256.1-0547 '</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>193.6058959960938</v>
+        <v>194.0442810058594</v>
       </c>
       <c r="D76" t="n">
-        <v>22.18258476257324</v>
+        <v>-5.79459285736084</v>
       </c>
       <c r="E76" t="n">
-        <v>1946.014319805091</v>
+        <v>2034.921432753547</v>
       </c>
       <c r="F76" t="n">
-        <v>310.9003864000454</v>
+        <v>305.0998846118308</v>
       </c>
       <c r="G76" t="n">
-        <v>85.00807392479871</v>
+        <v>57.05720524664127</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>b'3FHL J1256.1-0547 '</t>
+          <t>b'3FHL J1258.3+6121 '</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>194.0442810058594</v>
+        <v>194.5815887451172</v>
       </c>
       <c r="D77" t="n">
-        <v>-5.79459285736084</v>
+        <v>61.36655807495117</v>
       </c>
       <c r="E77" t="n">
-        <v>2034.921432753547</v>
+        <v>920.2003591656152</v>
       </c>
       <c r="F77" t="n">
-        <v>305.0998846118308</v>
+        <v>121.4659798152458</v>
       </c>
       <c r="G77" t="n">
-        <v>57.05720524664127</v>
+        <v>55.7420815224022</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>b'3FHL J1258.3+6121 '</t>
+          <t>b'3FHL J1312.6+4828 '</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>194.5815887451172</v>
+        <v>198.1574249267578</v>
       </c>
       <c r="D78" t="n">
-        <v>61.36655807495117</v>
+        <v>48.47776031494141</v>
       </c>
       <c r="E78" t="n">
-        <v>920.2003591656152</v>
+        <v>1919.40425528274</v>
       </c>
       <c r="F78" t="n">
-        <v>121.4659798152458</v>
+        <v>113.4210086615013</v>
       </c>
       <c r="G78" t="n">
-        <v>55.7420815224022</v>
+        <v>68.25727662537837</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>b'3FHL J1312.6+4828 '</t>
+          <t>b'3FHL J1319.5+1404 '</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>198.1574249267578</v>
+        <v>199.8961791992188</v>
       </c>
       <c r="D79" t="n">
-        <v>48.47776031494141</v>
+        <v>14.07064819335938</v>
       </c>
       <c r="E79" t="n">
-        <v>1919.40425528274</v>
+        <v>2154.520586195584</v>
       </c>
       <c r="F79" t="n">
-        <v>113.4210086615013</v>
+        <v>331.0264520499293</v>
       </c>
       <c r="G79" t="n">
-        <v>68.25727662537837</v>
+        <v>75.38452389248357</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>b'3FHL J1319.5+1404 '</t>
+          <t>b'3FHL J1340.5+4410 '</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>199.8961791992188</v>
+        <v>205.1303100585938</v>
       </c>
       <c r="D80" t="n">
-        <v>14.07064819335938</v>
+        <v>44.18074798583984</v>
       </c>
       <c r="E80" t="n">
-        <v>2154.520586195584</v>
+        <v>2067.499118066273</v>
       </c>
       <c r="F80" t="n">
-        <v>331.0264520499293</v>
+        <v>96.05410900986132</v>
       </c>
       <c r="G80" t="n">
-        <v>75.38452389248357</v>
+        <v>70.29735077732514</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>b'3FHL J1340.5+4410 '</t>
+          <t>b'3FHL J1341.2+3959 '</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>205.1303100585938</v>
+        <v>205.3132781982422</v>
       </c>
       <c r="D81" t="n">
-        <v>44.18074798583984</v>
+        <v>39.98970031738281</v>
       </c>
       <c r="E81" t="n">
-        <v>2067.499118066273</v>
+        <v>715.4362988699944</v>
       </c>
       <c r="F81" t="n">
-        <v>96.05410900986132</v>
+        <v>87.33566812682206</v>
       </c>
       <c r="G81" t="n">
-        <v>70.29735077732514</v>
+        <v>73.50951317099407</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>b'3FHL J1341.2+3959 '</t>
+          <t>b'3FHL J1402.6+1559 '</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>205.3132781982422</v>
+        <v>210.6538238525391</v>
       </c>
       <c r="D82" t="n">
-        <v>39.98970031738281</v>
+        <v>15.98397254943848</v>
       </c>
       <c r="E82" t="n">
-        <v>715.4362988699944</v>
+        <v>997.5030593997925</v>
       </c>
       <c r="F82" t="n">
-        <v>87.33566812682206</v>
+        <v>2.539795875341265</v>
       </c>
       <c r="G82" t="n">
-        <v>73.50951317099407</v>
+        <v>70.08723433248876</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>b'3FHL J1402.6+1559 '</t>
+          <t>b'3FHL J1404.9+0401 '</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>210.6538238525391</v>
+        <v>211.2331237792969</v>
       </c>
       <c r="D83" t="n">
-        <v>15.98397254943848</v>
+        <v>4.028957843780518</v>
       </c>
       <c r="E83" t="n">
-        <v>997.5030593997925</v>
+        <v>1371.891644524125</v>
       </c>
       <c r="F83" t="n">
-        <v>2.539795875341265</v>
+        <v>343.356454326494</v>
       </c>
       <c r="G83" t="n">
-        <v>70.08723433248876</v>
+        <v>60.99387507635056</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>b'3FHL J1404.9+0401 '</t>
+          <t>b'3FHL J1411.8+5249 '</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>211.2331237792969</v>
+        <v>212.9649963378906</v>
       </c>
       <c r="D84" t="n">
-        <v>4.028957843780518</v>
+        <v>52.82292938232422</v>
       </c>
       <c r="E84" t="n">
-        <v>1371.891644524125</v>
+        <v>325.2711537377689</v>
       </c>
       <c r="F84" t="n">
-        <v>343.356454326494</v>
+        <v>98.17146981808737</v>
       </c>
       <c r="G84" t="n">
-        <v>60.99387507635056</v>
+        <v>60.26679845594848</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>b'3FHL J1411.8+5249 '</t>
+          <t>b'3FHL J1415.6+4830 '</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>212.9649963378906</v>
+        <v>213.9147796630859</v>
       </c>
       <c r="D85" t="n">
-        <v>52.82292938232422</v>
+        <v>48.51522445678711</v>
       </c>
       <c r="E85" t="n">
-        <v>325.2711537377689</v>
+        <v>1902.710656439457</v>
       </c>
       <c r="F85" t="n">
-        <v>98.17146981808737</v>
+        <v>91.19850370499088</v>
       </c>
       <c r="G85" t="n">
-        <v>60.26679845594848</v>
+        <v>63.09742003770977</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>b'3FHL J1415.6+4830 '</t>
+          <t>b'3FHL J1418.0+2543 '</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>213.9147796630859</v>
+        <v>214.5009460449219</v>
       </c>
       <c r="D86" t="n">
-        <v>48.51522445678711</v>
+        <v>25.7291259765625</v>
       </c>
       <c r="E86" t="n">
-        <v>1902.710656439457</v>
+        <v>970.5390841006508</v>
       </c>
       <c r="F86" t="n">
-        <v>91.19850370499088</v>
+        <v>33.71460610300097</v>
       </c>
       <c r="G86" t="n">
-        <v>63.09742003770977</v>
+        <v>70.59372559903728</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>b'3FHL J1418.0+2543 '</t>
+          <t>b'3FHL J1419.4+0444 '</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>214.5009460449219</v>
+        <v>214.8675231933594</v>
       </c>
       <c r="D87" t="n">
-        <v>25.7291259765625</v>
+        <v>4.745282173156738</v>
       </c>
       <c r="E87" t="n">
-        <v>970.5390841006508</v>
+        <v>598.8824976040644</v>
       </c>
       <c r="F87" t="n">
-        <v>33.71460610300097</v>
+        <v>349.978509379617</v>
       </c>
       <c r="G87" t="n">
-        <v>70.59372559903728</v>
+        <v>59.3198698029064</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>b'3FHL J1419.4+0444 '</t>
+          <t>b'3FHL J1419.7+5423 '</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>214.8675231933594</v>
+        <v>214.9465789794922</v>
       </c>
       <c r="D88" t="n">
-        <v>4.745282173156738</v>
+        <v>54.39066696166992</v>
       </c>
       <c r="E88" t="n">
-        <v>598.8824976040644</v>
+        <v>639.2633050973789</v>
       </c>
       <c r="F88" t="n">
-        <v>349.978509379617</v>
+        <v>98.30243691724219</v>
       </c>
       <c r="G88" t="n">
-        <v>59.3198698029064</v>
+        <v>58.30848489225325</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>b'3FHL J1419.7+5423 '</t>
+          <t>b'3FHL J1422.6+5801 '</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>214.9465789794922</v>
+        <v>215.6541900634766</v>
       </c>
       <c r="D89" t="n">
-        <v>54.39066696166992</v>
+        <v>58.01887893676758</v>
       </c>
       <c r="E89" t="n">
-        <v>639.2633050973789</v>
+        <v>2349.244257634401</v>
       </c>
       <c r="F89" t="n">
-        <v>98.30243691724219</v>
+        <v>101.8492086867801</v>
       </c>
       <c r="G89" t="n">
-        <v>58.30848489225325</v>
+        <v>55.21857129706387</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>b'3FHL J1422.6+5801 '</t>
+          <t>b'3FHL J1428.5+4240 '</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>215.6541900634766</v>
+        <v>217.1364593505859</v>
       </c>
       <c r="D90" t="n">
-        <v>58.01887893676758</v>
+        <v>42.67203521728516</v>
       </c>
       <c r="E90" t="n">
-        <v>2349.244257634401</v>
+        <v>542.0147093189177</v>
       </c>
       <c r="F90" t="n">
-        <v>101.8492086867801</v>
+        <v>77.48566790521888</v>
       </c>
       <c r="G90" t="n">
-        <v>55.21857129706387</v>
+        <v>64.8988126310412</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>b'3FHL J1428.5+4240 '</t>
+          <t>b'3FHL J1436.9+5639 '</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>217.1364593505859</v>
+        <v>219.2470092773438</v>
       </c>
       <c r="D91" t="n">
-        <v>42.67203521728516</v>
+        <v>56.66003799438477</v>
       </c>
       <c r="E91" t="n">
-        <v>542.0147093189177</v>
+        <v>627.1700359849448</v>
       </c>
       <c r="F91" t="n">
-        <v>77.48566790521888</v>
+        <v>97.72870692965985</v>
       </c>
       <c r="G91" t="n">
-        <v>64.8988126310412</v>
+        <v>54.99658828453175</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>b'3FHL J1436.9+5639 '</t>
+          <t>b'3FHL J1439.3+3931 '</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>219.2470092773438</v>
+        <v>219.8288269042969</v>
       </c>
       <c r="D92" t="n">
-        <v>56.66003799438477</v>
+        <v>39.52298355102539</v>
       </c>
       <c r="E92" t="n">
-        <v>627.1700359849448</v>
+        <v>1371.891644524125</v>
       </c>
       <c r="F92" t="n">
-        <v>97.72870692965985</v>
+        <v>68.79583747417368</v>
       </c>
       <c r="G92" t="n">
-        <v>54.99658828453175</v>
+        <v>64.42668452711504</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>b'3FHL J1439.3+3931 '</t>
+          <t>b'3FHL J1440.9+0610 '</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>219.8288269042969</v>
+        <v>220.2337188720703</v>
       </c>
       <c r="D93" t="n">
-        <v>39.52298355102539</v>
+        <v>6.175134658813477</v>
       </c>
       <c r="E93" t="n">
-        <v>1371.891644524125</v>
+        <v>1558.62649529763</v>
       </c>
       <c r="F93" t="n">
-        <v>68.79583747417368</v>
+        <v>359.0613035363558</v>
       </c>
       <c r="G93" t="n">
-        <v>64.42668452711504</v>
+        <v>56.59426497141165</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>b'3FHL J1440.9+0610 '</t>
+          <t>b'3FHL J1442.8+1200 '</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>220.2337188720703</v>
+        <v>220.7103729248047</v>
       </c>
       <c r="D94" t="n">
-        <v>6.175134658813477</v>
+        <v>12.00308227539062</v>
       </c>
       <c r="E94" t="n">
-        <v>1558.62649529763</v>
+        <v>679.4444413307867</v>
       </c>
       <c r="F94" t="n">
-        <v>359.0613035363558</v>
+        <v>8.326391244799357</v>
       </c>
       <c r="G94" t="n">
-        <v>56.59426497141165</v>
+        <v>59.82810578059493</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>b'3FHL J1442.8+1200 '</t>
+          <t>b'3FHL J1443.5+2515 '</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>220.7103729248047</v>
+        <v>220.8969116210938</v>
       </c>
       <c r="D95" t="n">
-        <v>12.00308227539062</v>
+        <v>25.26393508911133</v>
       </c>
       <c r="E95" t="n">
-        <v>679.4444413307867</v>
+        <v>2012.076573556624</v>
       </c>
       <c r="F95" t="n">
-        <v>8.326391244799357</v>
+        <v>35.06898725925156</v>
       </c>
       <c r="G95" t="n">
-        <v>59.82810578059493</v>
+        <v>64.8249872712824</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>b'3FHL J1443.5+2515 '</t>
+          <t>b'3FHL J1449.5+2745 '</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>220.8969116210938</v>
+        <v>222.3851776123047</v>
       </c>
       <c r="D96" t="n">
-        <v>25.26393508911133</v>
+        <v>27.75633811950684</v>
       </c>
       <c r="E96" t="n">
-        <v>2012.076573556624</v>
+        <v>931.8472681578297</v>
       </c>
       <c r="F96" t="n">
-        <v>35.06898725925156</v>
+        <v>41.19890036398075</v>
       </c>
       <c r="G96" t="n">
-        <v>64.8249872712824</v>
+        <v>63.8522071735304</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>b'3FHL J1449.5+2745 '</t>
+          <t>b'3FHL J1458.7+3722 '</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>222.3851776123047</v>
+        <v>224.6948089599609</v>
       </c>
       <c r="D97" t="n">
-        <v>27.75633811950684</v>
+        <v>37.36803436279297</v>
       </c>
       <c r="E97" t="n">
-        <v>931.8472681578297</v>
+        <v>1331.696061964219</v>
       </c>
       <c r="F97" t="n">
-        <v>41.19890036398075</v>
+        <v>61.92235747685517</v>
       </c>
       <c r="G97" t="n">
-        <v>63.8522071735304</v>
+        <v>61.36237350674613</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>b'3FHL J1458.7+3722 '</t>
+          <t>b'3FHL J1500.9+2238 '</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>224.6948089599609</v>
+        <v>225.2482757568359</v>
       </c>
       <c r="D98" t="n">
-        <v>37.36803436279297</v>
+        <v>22.64022445678711</v>
       </c>
       <c r="E98" t="n">
-        <v>1331.696061964219</v>
+        <v>962.8168789726126</v>
       </c>
       <c r="F98" t="n">
-        <v>61.92235747685517</v>
+        <v>31.45102290888001</v>
       </c>
       <c r="G98" t="n">
-        <v>61.36237350674613</v>
+        <v>60.35999634319712</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>b'3FHL J1500.9+2238 '</t>
+          <t>b'3FHL J1503.3+4758 '</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>225.2482757568359</v>
+        <v>225.8384399414062</v>
       </c>
       <c r="D99" t="n">
-        <v>22.64022445678711</v>
+        <v>47.97346878051758</v>
       </c>
       <c r="E99" t="n">
-        <v>962.8168789726126</v>
+        <v>1371.891644524125</v>
       </c>
       <c r="F99" t="n">
-        <v>31.45102290888001</v>
+        <v>80.9535755751856</v>
       </c>
       <c r="G99" t="n">
-        <v>60.35999634319712</v>
+        <v>56.98629153475792</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>b'3FHL J1503.3+4758 '</t>
+          <t>b'3FHL J1506.0+3732 '</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>225.8384399414062</v>
+        <v>226.5228424072266</v>
       </c>
       <c r="D100" t="n">
-        <v>47.97346878051758</v>
+        <v>37.54251480102539</v>
       </c>
       <c r="E100" t="n">
-        <v>1371.891644524125</v>
+        <v>2465.150914639177</v>
       </c>
       <c r="F100" t="n">
-        <v>80.9535755751856</v>
+        <v>61.70862488595789</v>
       </c>
       <c r="G100" t="n">
-        <v>56.98629153475792</v>
+        <v>59.90456332383156</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>b'3FHL J1506.0+3732 '</t>
+          <t>b'3FHL J1506.7+0813 '</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>226.5228424072266</v>
+        <v>226.6905822753906</v>
       </c>
       <c r="D101" t="n">
-        <v>37.54251480102539</v>
+        <v>8.218801498413086</v>
       </c>
       <c r="E101" t="n">
-        <v>2465.150914639177</v>
+        <v>1487.444413390686</v>
       </c>
       <c r="F101" t="n">
-        <v>61.70862488595789</v>
+        <v>8.730330769087979</v>
       </c>
       <c r="G101" t="n">
-        <v>59.90456332383156</v>
+        <v>52.83404159105811</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>b'3FHL J1506.7+0813 '</t>
+          <t>b'3FHL J1507.2+1722 '</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>226.6905822753906</v>
+        <v>226.8249816894531</v>
       </c>
       <c r="D102" t="n">
-        <v>8.218801498413086</v>
+        <v>17.36773490905762</v>
       </c>
       <c r="E102" t="n">
-        <v>1487.444413390686</v>
+        <v>2129.778114886851</v>
       </c>
       <c r="F102" t="n">
-        <v>8.730330769087979</v>
+        <v>22.80134452177674</v>
       </c>
       <c r="G102" t="n">
-        <v>52.83404159105811</v>
+        <v>57.20281900749549</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>b'3FHL J1507.2+1722 '</t>
+          <t>b'3FHL J1508.7+2708 '</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>226.8249816894531</v>
+        <v>227.1883544921875</v>
       </c>
       <c r="D103" t="n">
-        <v>17.36773490905762</v>
+        <v>27.14417457580566</v>
       </c>
       <c r="E103" t="n">
-        <v>2129.778114886851</v>
+        <v>1096.787424633644</v>
       </c>
       <c r="F103" t="n">
-        <v>22.80134452177674</v>
+        <v>40.97986187978024</v>
       </c>
       <c r="G103" t="n">
-        <v>57.20281900749549</v>
+        <v>59.54763194954369</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>b'3FHL J1508.7+2708 '</t>
+          <t>b'3FHL J1512.2+0203 '</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>227.1883544921875</v>
+        <v>228.0720062255859</v>
       </c>
       <c r="D104" t="n">
-        <v>27.14417457580566</v>
+        <v>2.060366868972778</v>
       </c>
       <c r="E104" t="n">
-        <v>1096.787424633644</v>
+        <v>904.6427903224928</v>
       </c>
       <c r="F104" t="n">
-        <v>40.97986187978024</v>
+        <v>2.367075362555521</v>
       </c>
       <c r="G104" t="n">
-        <v>59.54763194954369</v>
+        <v>47.99279308444518</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>b'3FHL J1512.2+0203 '</t>
+          <t>b'3FHL J1518.5+4044 '</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>228.0720062255859</v>
+        <v>229.6453247070312</v>
       </c>
       <c r="D105" t="n">
-        <v>2.060366868972778</v>
+        <v>40.73994827270508</v>
       </c>
       <c r="E105" t="n">
-        <v>904.6427903224928</v>
+        <v>277.125303444809</v>
       </c>
       <c r="F105" t="n">
-        <v>2.367075362555521</v>
+        <v>66.76651396705567</v>
       </c>
       <c r="G105" t="n">
-        <v>47.99279308444518</v>
+        <v>56.89182212745664</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>b'3FHL J1518.5+4044 '</t>
+          <t>b'3FHL J1531.9+3016 '</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>229.6453247070312</v>
+        <v>232.9860992431641</v>
       </c>
       <c r="D106" t="n">
-        <v>40.73994827270508</v>
+        <v>30.27317047119141</v>
       </c>
       <c r="E106" t="n">
         <v>277.125303444809</v>
       </c>
       <c r="F106" t="n">
-        <v>66.76651396705567</v>
+        <v>47.77962265205297</v>
       </c>
       <c r="G106" t="n">
-        <v>56.89182212745664</v>
+        <v>54.84301768980958</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>b'3FHL J1531.9+3016 '</t>
+          <t>b'3FHL J1533.2+1855 '</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>232.9860992431641</v>
+        <v>233.3144226074219</v>
       </c>
       <c r="D107" t="n">
-        <v>30.27317047119141</v>
+        <v>18.93068313598633</v>
       </c>
       <c r="E107" t="n">
-        <v>277.125303444809</v>
+        <v>1235.720342438146</v>
       </c>
       <c r="F107" t="n">
-        <v>47.77962265205297</v>
+        <v>29.25278554792897</v>
       </c>
       <c r="G107" t="n">
-        <v>54.84301768980958</v>
+        <v>52.0464613686915</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>b'3FHL J1533.2+1855 '</t>
+          <t>b'3FHL J1540.7+1448 '</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>233.3144226074219</v>
+        <v>235.1949615478516</v>
       </c>
       <c r="D108" t="n">
-        <v>18.93068313598633</v>
+        <v>14.81568145751953</v>
       </c>
       <c r="E108" t="n">
-        <v>1235.720342438146</v>
+        <v>2255.902501594245</v>
       </c>
       <c r="F108" t="n">
-        <v>29.25278554792897</v>
+        <v>24.34762000956751</v>
       </c>
       <c r="G108" t="n">
-        <v>52.0464613686915</v>
+        <v>48.81774577195303</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>b'3FHL J1540.7+1448 '</t>
+          <t>b'3FHL J1543.6+0452 '</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>235.1949615478516</v>
+        <v>235.9000091552734</v>
       </c>
       <c r="D109" t="n">
-        <v>14.81568145751953</v>
+        <v>4.879972457885742</v>
       </c>
       <c r="E109" t="n">
-        <v>2255.902501594245</v>
+        <v>171.3237639398314</v>
       </c>
       <c r="F109" t="n">
-        <v>24.34762000956751</v>
+        <v>12.27756886738662</v>
       </c>
       <c r="G109" t="n">
-        <v>48.81774577195303</v>
+        <v>43.38510723073886</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>b'3FHL J1543.6+0452 '</t>
+          <t>b'3FHL J1554.2+2010 '</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>235.9000091552734</v>
+        <v>238.5714263916016</v>
       </c>
       <c r="D110" t="n">
-        <v>4.879972457885742</v>
+        <v>20.17705154418945</v>
       </c>
       <c r="E110" t="n">
-        <v>171.3237639398314</v>
+        <v>912.4256141983458</v>
       </c>
       <c r="F110" t="n">
-        <v>12.27756886738662</v>
+        <v>33.62416920162958</v>
       </c>
       <c r="G110" t="n">
-        <v>43.38510723073886</v>
+        <v>47.78168755695976</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>b'3FHL J1554.2+2010 '</t>
+          <t>b'3FHL J1558.8+5626 '</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>238.5714263916016</v>
+        <v>239.7223358154297</v>
       </c>
       <c r="D111" t="n">
-        <v>20.17705154418945</v>
+        <v>56.44340133666992</v>
       </c>
       <c r="E111" t="n">
-        <v>912.4256141983458</v>
+        <v>1209.647842624998</v>
       </c>
       <c r="F111" t="n">
-        <v>33.62416920162958</v>
+        <v>87.61477950088891</v>
       </c>
       <c r="G111" t="n">
-        <v>47.78168755695976</v>
+        <v>45.75468964677962</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>b'3FHL J1558.8+5626 '</t>
+          <t>b'3FHL J1603.8+1103 '</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>239.7223358154297</v>
+        <v>240.9507446289062</v>
       </c>
       <c r="D112" t="n">
-        <v>56.44340133666992</v>
+        <v>11.0573263168335</v>
       </c>
       <c r="E112" t="n">
-        <v>1209.647842624998</v>
+        <v>598.8824976040644</v>
       </c>
       <c r="F112" t="n">
-        <v>87.61477950088891</v>
+        <v>22.97464182629868</v>
       </c>
       <c r="G112" t="n">
-        <v>45.75468964677962</v>
+        <v>42.13516682302727</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>b'3FHL J1603.8+1103 '</t>
+          <t>b'3FHL J1603.8+5010 '</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>240.9507446289062</v>
+        <v>240.9585723876953</v>
       </c>
       <c r="D113" t="n">
-        <v>11.0573263168335</v>
+        <v>50.16685104370117</v>
       </c>
       <c r="E113" t="n">
-        <v>598.8824976040644</v>
+        <v>2305.888248308498</v>
       </c>
       <c r="F113" t="n">
-        <v>22.97464182629868</v>
+        <v>78.62070005851318</v>
       </c>
       <c r="G113" t="n">
-        <v>42.13516682302727</v>
+        <v>46.96057254045356</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>b'3FHL J1603.8+5010 '</t>
+          <t>b'3FHL J1606.2+5629 '</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>240.9585723876953</v>
+        <v>241.56298828125</v>
       </c>
       <c r="D114" t="n">
-        <v>50.16685104370117</v>
+        <v>56.4957389831543</v>
       </c>
       <c r="E114" t="n">
-        <v>2305.888248308498</v>
+        <v>1746.861857496495</v>
       </c>
       <c r="F114" t="n">
-        <v>78.62070005851318</v>
+        <v>87.17804013571619</v>
       </c>
       <c r="G114" t="n">
-        <v>46.96057254045356</v>
+        <v>44.78413662138935</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>b'3FHL J1606.2+5629 '</t>
+          <t>b'3FHL J1607.0+1550 '</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>241.56298828125</v>
+        <v>241.7560882568359</v>
       </c>
       <c r="D115" t="n">
-        <v>56.4957389831543</v>
+        <v>15.83572101593018</v>
       </c>
       <c r="E115" t="n">
-        <v>1746.861857496495</v>
+        <v>1902.710656439457</v>
       </c>
       <c r="F115" t="n">
-        <v>87.17804013571619</v>
+        <v>29.33763480478526</v>
       </c>
       <c r="G115" t="n">
-        <v>44.78413662138935</v>
+        <v>43.41828545322375</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>b'3FHL J1607.0+1550 '</t>
+          <t>b'3FHL J1615.4+4711 '</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>241.7560882568359</v>
+        <v>243.8666687011719</v>
       </c>
       <c r="D116" t="n">
-        <v>15.83572101593018</v>
+        <v>47.19518280029297</v>
       </c>
       <c r="E116" t="n">
-        <v>1902.710656439457</v>
+        <v>820.9795643094412</v>
       </c>
       <c r="F116" t="n">
-        <v>29.33763480478526</v>
+        <v>73.86428573709217</v>
       </c>
       <c r="G116" t="n">
-        <v>43.41828545322375</v>
+        <v>45.64854529020995</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>b'3FHL J1615.4+4711 '</t>
+          <t>b'3FHL J1626.2+3515 '</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>243.8666687011719</v>
+        <v>246.5747680664062</v>
       </c>
       <c r="D117" t="n">
-        <v>47.19518280029297</v>
+        <v>35.26229095458984</v>
       </c>
       <c r="E117" t="n">
-        <v>820.9795643094412</v>
+        <v>1907.322882417562</v>
       </c>
       <c r="F117" t="n">
-        <v>73.86428573709217</v>
+        <v>56.96303155478957</v>
       </c>
       <c r="G117" t="n">
-        <v>45.64854529020995</v>
+        <v>43.8921473549683</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>b'3FHL J1626.2+3515 '</t>
+          <t>b'3FHL J1642.9+3948 '</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>246.5747680664062</v>
+        <v>250.7349090576172</v>
       </c>
       <c r="D118" t="n">
-        <v>35.26229095458984</v>
+        <v>39.81490707397461</v>
       </c>
       <c r="E118" t="n">
-        <v>1907.322882417562</v>
+        <v>2218.105585899384</v>
       </c>
       <c r="F118" t="n">
-        <v>56.96303155478957</v>
+        <v>63.46049227208619</v>
       </c>
       <c r="G118" t="n">
-        <v>43.8921473549683</v>
+        <v>40.95690199972307</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>b'3FHL J1642.9+3948 '</t>
+          <t>b'3FHL J1647.6+4950 '</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>250.7349090576172</v>
+        <v>251.9024505615234</v>
       </c>
       <c r="D119" t="n">
-        <v>39.81490707397461</v>
+        <v>49.84615325927734</v>
       </c>
       <c r="E119" t="n">
-        <v>2218.105585899384</v>
+        <v>201.1884205905175</v>
       </c>
       <c r="F119" t="n">
-        <v>63.46049227208619</v>
+        <v>76.66087340567729</v>
       </c>
       <c r="G119" t="n">
-        <v>40.95690199972307</v>
+        <v>40.07035923704507</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>b'3FHL J1647.6+4950 '</t>
+          <t>b'3FHL J1652.7+4024 '</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>251.9024505615234</v>
+        <v>253.1941070556641</v>
       </c>
       <c r="D120" t="n">
-        <v>49.84615325927734</v>
+        <v>40.40338897705078</v>
       </c>
       <c r="E120" t="n">
-        <v>201.1884205905175</v>
+        <v>982.1071720326452</v>
       </c>
       <c r="F120" t="n">
-        <v>76.66087340567729</v>
+        <v>64.40155662759337</v>
       </c>
       <c r="G120" t="n">
-        <v>40.07035923704507</v>
+        <v>39.12261782369705</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>b'3FHL J1652.7+4024 '</t>
+          <t>b'3FHL J1653.8+3945 '</t>
         </is>
       </c>
       <c r="C121" t="n">
-        <v>253.1941070556641</v>
+        <v>253.4710998535156</v>
       </c>
       <c r="D121" t="n">
-        <v>40.40338897705078</v>
+        <v>39.75818634033203</v>
       </c>
       <c r="E121" t="n">
-        <v>982.1071720326452</v>
+        <v>141.697084695296</v>
       </c>
       <c r="F121" t="n">
-        <v>64.40155662759337</v>
+        <v>63.59781706285712</v>
       </c>
       <c r="G121" t="n">
-        <v>39.12261782369705</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" s="1" t="n">
-        <v>275</v>
-      </c>
-      <c r="B122" t="inlineStr">
-        <is>
-          <t>b'3FHL J1653.8+3945 '</t>
-        </is>
-      </c>
-      <c r="C122" t="n">
-        <v>253.4710998535156</v>
-      </c>
-      <c r="D122" t="n">
-        <v>39.75818634033203</v>
-      </c>
-      <c r="E122" t="n">
-        <v>141.697084695296</v>
-      </c>
-      <c r="F122" t="n">
-        <v>63.59781706285712</v>
-      </c>
-      <c r="G122" t="n">
         <v>38.85626839795113</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Manually filtered gamma-ray sources for Sutter void footprint
</commit_message>
<xml_diff>
--- a/cel_obj_table.xlsx
+++ b/cel_obj_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G121"/>
+  <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,3001 +467,2476 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>b'3FHL J0730.4+3307 '</t>
+          <t>b'3FHL J0754.8+4822 '</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>112.6081008911133</v>
+        <v>118.7094268798828</v>
       </c>
       <c r="D2" t="n">
-        <v>33.12022399902344</v>
+        <v>48.38185119628906</v>
       </c>
       <c r="E2" t="n">
-        <v>472.4384783695589</v>
+        <v>1489.98505775128</v>
       </c>
       <c r="F2" t="n">
-        <v>185.874446883025</v>
+        <v>170.5698825442753</v>
       </c>
       <c r="G2" t="n">
-        <v>22.04667824967751</v>
+        <v>30.15412007607718</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>b'3FHL J0738.1+1742 '</t>
+          <t>b'3FHL J0809.7+3457 '</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>114.5327682495117</v>
+        <v>122.4298248291016</v>
       </c>
       <c r="D3" t="n">
-        <v>17.71304893493652</v>
+        <v>34.95800018310547</v>
       </c>
       <c r="E3" t="n">
-        <v>1656.947604950266</v>
+        <v>352.4357721162331</v>
       </c>
       <c r="F3" t="n">
-        <v>201.8397573898806</v>
+        <v>186.4471419042782</v>
       </c>
       <c r="G3" t="n">
-        <v>18.07539141955594</v>
+        <v>30.37076642512884</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>b'3FHL J0753.1+5354 '</t>
+          <t>b'3FHL J0809.8+5218 '</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>118.2864151000977</v>
+        <v>122.4586029052734</v>
       </c>
       <c r="D4" t="n">
-        <v>53.90745544433594</v>
+        <v>52.31039428710938</v>
       </c>
       <c r="E4" t="n">
-        <v>826.3707136061979</v>
+        <v>578.6172947152628</v>
       </c>
       <c r="F4" t="n">
-        <v>164.1736930995773</v>
+        <v>166.2520819406516</v>
       </c>
       <c r="G4" t="n">
-        <v>30.52602863281245</v>
+        <v>32.91232473625846</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>b'3FHL J0754.8+4822 '</t>
+          <t>b'3FHL J0816.9+2050 '</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>118.7094268798828</v>
+        <v>124.2364349365234</v>
       </c>
       <c r="D5" t="n">
-        <v>48.38185119628906</v>
+        <v>20.84729194641113</v>
       </c>
       <c r="E5" t="n">
-        <v>1489.98505775128</v>
+        <v>247.6684183724716</v>
       </c>
       <c r="F5" t="n">
-        <v>170.5698825442753</v>
+        <v>202.4247601227709</v>
       </c>
       <c r="G5" t="n">
-        <v>30.15412007607718</v>
+        <v>27.73866668831735</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>b'3FHL J0757.1+0957 '</t>
+          <t>b'3FHL J0818.2+4222 '</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>119.2889862060547</v>
+        <v>124.5621643066406</v>
       </c>
       <c r="D6" t="n">
-        <v>9.965688705444336</v>
+        <v>42.37668228149414</v>
       </c>
       <c r="E6" t="n">
-        <v>1081.60187099801</v>
+        <v>2015.283911619772</v>
       </c>
       <c r="F6" t="n">
-        <v>211.2949664982855</v>
+        <v>178.2303101447942</v>
       </c>
       <c r="G6" t="n">
-        <v>19.07671444842579</v>
+        <v>33.39832911945414</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>b'3FHL J0809.7+3457 '</t>
+          <t>b'3FHL J0820.9+2353 '</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>122.4298248291016</v>
+        <v>125.2343978881836</v>
       </c>
       <c r="D7" t="n">
-        <v>34.95800018310547</v>
+        <v>23.89204978942871</v>
       </c>
       <c r="E7" t="n">
-        <v>352.4357721162331</v>
+        <v>1579.826051622189</v>
       </c>
       <c r="F7" t="n">
-        <v>186.4471419042782</v>
+        <v>199.510479607579</v>
       </c>
       <c r="G7" t="n">
-        <v>30.37076642512884</v>
+        <v>29.63265514420423</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>b'3FHL J0809.8+5218 '</t>
+          <t>b'3FHL J0825.7+0311 '</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>122.4586029052734</v>
+        <v>126.4462661743164</v>
       </c>
       <c r="D8" t="n">
-        <v>52.31039428710938</v>
+        <v>3.194593906402588</v>
       </c>
       <c r="E8" t="n">
-        <v>578.6172947152628</v>
+        <v>1936.049867434469</v>
       </c>
       <c r="F8" t="n">
-        <v>166.2520819406516</v>
+        <v>221.1759682227195</v>
       </c>
       <c r="G8" t="n">
-        <v>32.91232473625846</v>
+        <v>22.39409690992864</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>b'3FHL J0816.4+5739 '</t>
+          <t>b'3FHL J0828.3+4153 '</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>124.1090469360352</v>
+        <v>127.0883941650391</v>
       </c>
       <c r="D9" t="n">
-        <v>57.66443634033203</v>
+        <v>41.89826965332031</v>
       </c>
       <c r="E9" t="n">
-        <v>230.7935158149133</v>
+        <v>927.9669661452913</v>
       </c>
       <c r="F9" t="n">
-        <v>159.8473262299431</v>
+        <v>179.0932631579409</v>
       </c>
       <c r="G9" t="n">
-        <v>33.90405576615215</v>
+        <v>35.19544797408459</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>b'3FHL J0816.9+2050 '</t>
+          <t>b'3FHL J0847.2+1134 '</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>124.2364349365234</v>
+        <v>131.8077850341797</v>
       </c>
       <c r="D10" t="n">
-        <v>20.84729194641113</v>
+        <v>11.56671619415283</v>
       </c>
       <c r="E10" t="n">
-        <v>247.6684183724716</v>
+        <v>822.4359267571556</v>
       </c>
       <c r="F10" t="n">
-        <v>202.4247601227709</v>
+        <v>215.4547936858709</v>
       </c>
       <c r="G10" t="n">
-        <v>27.73866668831735</v>
+        <v>30.89410316823072</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>b'3FHL J0818.2+4222 '</t>
+          <t>b'3FHL J0849.9+5108 '</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>124.5621643066406</v>
+        <v>132.4937896728516</v>
       </c>
       <c r="D11" t="n">
-        <v>42.37668228149414</v>
+        <v>51.141845703125</v>
       </c>
       <c r="E11" t="n">
-        <v>2015.283911619772</v>
+        <v>2186.405655380971</v>
       </c>
       <c r="F11" t="n">
-        <v>178.2303101447942</v>
+        <v>167.6055794666185</v>
       </c>
       <c r="G11" t="n">
-        <v>33.39832911945414</v>
+        <v>39.1364989957745</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>b'3FHL J0820.9+2353 '</t>
+          <t>b'3FHL J0850.6+3454 '</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>125.2343978881836</v>
+        <v>132.6519165039062</v>
       </c>
       <c r="D12" t="n">
-        <v>23.89204978942871</v>
+        <v>34.90697479248047</v>
       </c>
       <c r="E12" t="n">
-        <v>1579.826051622189</v>
+        <v>606.9745772102617</v>
       </c>
       <c r="F12" t="n">
-        <v>199.510479607579</v>
+        <v>188.4881336399034</v>
       </c>
       <c r="G12" t="n">
-        <v>29.63265514420423</v>
+        <v>38.57761892185869</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>b'3FHL J0825.7+0311 '</t>
+          <t>b'3FHL J0854.8+2006 '</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>126.4462661743164</v>
+        <v>133.7121429443359</v>
       </c>
       <c r="D13" t="n">
-        <v>3.194593906402588</v>
+        <v>20.10042953491211</v>
       </c>
       <c r="E13" t="n">
-        <v>1936.049867434469</v>
+        <v>1232.001690836247</v>
       </c>
       <c r="F13" t="n">
-        <v>221.1759682227195</v>
+        <v>206.8248045598298</v>
       </c>
       <c r="G13" t="n">
-        <v>22.39409690992864</v>
+        <v>35.82570420018077</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>b'3FHL J0828.3+4153 '</t>
+          <t>b'3FHL J0908.9+2311 '</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>127.0883941650391</v>
+        <v>137.2379302978516</v>
       </c>
       <c r="D14" t="n">
-        <v>41.89826965332031</v>
+        <v>23.19077682495117</v>
       </c>
       <c r="E14" t="n">
-        <v>927.9669661452913</v>
+        <v>916.3139966249578</v>
       </c>
       <c r="F14" t="n">
-        <v>179.0932631579409</v>
+        <v>204.4006996128279</v>
       </c>
       <c r="G14" t="n">
-        <v>35.19544797408459</v>
+        <v>39.90343163897078</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>b'3FHL J0831.8+0429 '</t>
+          <t>b'3FHL J0910.5+3329 '</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>127.9610137939453</v>
+        <v>137.62841796875</v>
       </c>
       <c r="D15" t="n">
-        <v>4.495641231536865</v>
+        <v>33.48870086669922</v>
       </c>
       <c r="E15" t="n">
-        <v>723.4123895726626</v>
+        <v>1408.222189015081</v>
       </c>
       <c r="F15" t="n">
-        <v>220.6957511158911</v>
+        <v>191.1184013879268</v>
       </c>
       <c r="G15" t="n">
-        <v>24.338949894984</v>
+        <v>42.44470192240891</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>b'3FHL J0847.2+1134 '</t>
+          <t>b'3FHL J0912.4+1555 '</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>131.8077850341797</v>
+        <v>138.1239929199219</v>
       </c>
       <c r="D16" t="n">
-        <v>11.56671619415283</v>
+        <v>15.9302806854248</v>
       </c>
       <c r="E16" t="n">
-        <v>822.4359267571556</v>
+        <v>873.4307914196993</v>
       </c>
       <c r="F16" t="n">
-        <v>215.4547936858709</v>
+        <v>213.5799215954228</v>
       </c>
       <c r="G16" t="n">
-        <v>30.89410316823072</v>
+        <v>38.26181930326724</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>b'3FHL J0849.9+5108 '</t>
+          <t>b'3FHL J0930.4+4952 '</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>132.4937896728516</v>
+        <v>142.6244659423828</v>
       </c>
       <c r="D17" t="n">
-        <v>51.141845703125</v>
+        <v>49.87545776367188</v>
       </c>
       <c r="E17" t="n">
-        <v>2186.405655380971</v>
+        <v>775.0615269997014</v>
       </c>
       <c r="F17" t="n">
-        <v>167.6055794666185</v>
+        <v>168.0950099107559</v>
       </c>
       <c r="G17" t="n">
-        <v>39.1364989957745</v>
+        <v>45.68697248424435</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>b'3FHL J0850.6+3454 '</t>
+          <t>b'3FHL J0946.2+0104 '</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>132.6519165039062</v>
+        <v>146.5630645751953</v>
       </c>
       <c r="D18" t="n">
-        <v>34.90697479248047</v>
+        <v>1.072644710540771</v>
       </c>
       <c r="E18" t="n">
-        <v>606.9745772102617</v>
+        <v>2167.296925661129</v>
       </c>
       <c r="F18" t="n">
-        <v>188.4881336399034</v>
+        <v>235.3603953607503</v>
       </c>
       <c r="G18" t="n">
-        <v>38.57761892185869</v>
+        <v>38.56086142877915</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>b'3FHL J0854.8+2006 '</t>
+          <t>b'3FHL J0950.3+4553 '</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>133.7121429443359</v>
+        <v>147.5764617919922</v>
       </c>
       <c r="D19" t="n">
-        <v>20.10042953491211</v>
+        <v>45.89204025268555</v>
       </c>
       <c r="E19" t="n">
-        <v>1232.001690836247</v>
+        <v>1569.235152018134</v>
       </c>
       <c r="F19" t="n">
-        <v>206.8248045598298</v>
+        <v>172.8821816193272</v>
       </c>
       <c r="G19" t="n">
-        <v>35.82570420018077</v>
+        <v>49.75183136937554</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>b'3FHL J0908.9+2311 '</t>
+          <t>b'3FHL J0954.2+4912 '</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>137.2379302978516</v>
+        <v>148.5668640136719</v>
       </c>
       <c r="D20" t="n">
-        <v>23.19077682495117</v>
+        <v>49.21414566040039</v>
       </c>
       <c r="E20" t="n">
-        <v>916.3139966249578</v>
+        <v>1501.744593228529</v>
       </c>
       <c r="F20" t="n">
-        <v>204.4006996128279</v>
+        <v>167.6515683277358</v>
       </c>
       <c r="G20" t="n">
-        <v>39.90343163897078</v>
+        <v>49.58651425014828</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>b'3FHL J0910.5+3329 '</t>
+          <t>b'3FHL J1001.2+2910 '</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>137.62841796875</v>
+        <v>150.3133544921875</v>
       </c>
       <c r="D21" t="n">
-        <v>33.48870086669922</v>
+        <v>29.1705379486084</v>
       </c>
       <c r="E21" t="n">
-        <v>1408.222189015081</v>
+        <v>2106.343909760358</v>
       </c>
       <c r="F21" t="n">
-        <v>191.1184013879268</v>
+        <v>199.5504344044182</v>
       </c>
       <c r="G21" t="n">
-        <v>42.44470192240891</v>
+        <v>52.63416273614697</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>b'3FHL J0912.4+1555 '</t>
+          <t>b'3FHL J1006.9+3455 '</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>138.1239929199219</v>
+        <v>151.7499389648438</v>
       </c>
       <c r="D22" t="n">
-        <v>15.9302806854248</v>
+        <v>34.92112350463867</v>
       </c>
       <c r="E22" t="n">
-        <v>873.4307914196993</v>
+        <v>2277.828672355331</v>
       </c>
       <c r="F22" t="n">
-        <v>213.5799215954228</v>
+        <v>190.0282006580422</v>
       </c>
       <c r="G22" t="n">
-        <v>38.26181930326724</v>
+        <v>54.17913076411402</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>b'3FHL J0930.4+4952 '</t>
+          <t>b'3FHL J1008.0+0622 '</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>142.6244659423828</v>
+        <v>152.0041351318359</v>
       </c>
       <c r="D23" t="n">
-        <v>49.87545776367188</v>
+        <v>6.373631954193115</v>
       </c>
       <c r="E23" t="n">
-        <v>775.0615269997014</v>
+        <v>2395.304963072071</v>
       </c>
       <c r="F23" t="n">
-        <v>168.0950099107559</v>
+        <v>233.50096097581</v>
       </c>
       <c r="G23" t="n">
-        <v>45.68697248424435</v>
+        <v>46.02256622120216</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>b'3FHL J0940.5+6149 '</t>
+          <t>b'3FHL J1012.6+4228 '</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>145.1408081054688</v>
+        <v>153.1730499267578</v>
       </c>
       <c r="D24" t="n">
-        <v>61.8179817199707</v>
+        <v>42.48298263549805</v>
       </c>
       <c r="E24" t="n">
-        <v>869.5202016942904</v>
+        <v>1447.954363211065</v>
       </c>
       <c r="F24" t="n">
-        <v>151.5795904696888</v>
+        <v>176.9216254086938</v>
       </c>
       <c r="G24" t="n">
-        <v>43.2124825532333</v>
+        <v>54.39503658450563</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>b'3FHL J0946.2+0104 '</t>
+          <t>b'3FHL J1015.0+4926 '</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>146.5630645751953</v>
+        <v>153.7693176269531</v>
       </c>
       <c r="D25" t="n">
-        <v>1.072644710540771</v>
+        <v>49.43538665771484</v>
       </c>
       <c r="E25" t="n">
-        <v>2167.296925661129</v>
+        <v>873.4307914196993</v>
       </c>
       <c r="F25" t="n">
-        <v>235.3603953607503</v>
+        <v>165.5301745409713</v>
       </c>
       <c r="G25" t="n">
-        <v>38.56086142877915</v>
+        <v>52.7128041733207</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>b'3FHL J0950.3+4553 '</t>
+          <t>b'3FHL J1026.9+0608 '</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>147.5764617919922</v>
+        <v>156.7403564453125</v>
       </c>
       <c r="D26" t="n">
-        <v>45.89204025268555</v>
+        <v>6.142007350921631</v>
       </c>
       <c r="E26" t="n">
-        <v>1569.235152018134</v>
+        <v>1743.428171899722</v>
       </c>
       <c r="F26" t="n">
-        <v>172.8821816193272</v>
+        <v>237.7476753956505</v>
       </c>
       <c r="G26" t="n">
-        <v>49.75183136937554</v>
+        <v>49.78141165294394</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>b'3FHL J0954.2+4912 '</t>
+          <t>b'3FHL J1031.3+5053 '</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>148.5668640136719</v>
+        <v>157.8328399658203</v>
       </c>
       <c r="D27" t="n">
-        <v>49.21414566040039</v>
+        <v>50.88592529296875</v>
       </c>
       <c r="E27" t="n">
-        <v>1501.744593228529</v>
+        <v>1433.534310193219</v>
       </c>
       <c r="F27" t="n">
-        <v>167.6515683277358</v>
+        <v>161.4466616146051</v>
       </c>
       <c r="G27" t="n">
-        <v>49.58651425014828</v>
+        <v>54.44603636948661</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>b'3FHL J1001.2+2910 '</t>
+          <t>b'3FHL J1032.7+3737 '</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>150.3133544921875</v>
+        <v>158.1970977783203</v>
       </c>
       <c r="D28" t="n">
-        <v>29.1705379486084</v>
+        <v>37.62113952636719</v>
       </c>
       <c r="E28" t="n">
-        <v>2106.343909760358</v>
+        <v>2008.723036449022</v>
       </c>
       <c r="F28" t="n">
-        <v>199.5504344044182</v>
+        <v>184.2725657102087</v>
       </c>
       <c r="G28" t="n">
-        <v>52.63416273614697</v>
+        <v>59.11119534742926</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>b'3FHL J1006.9+3455 '</t>
+          <t>b'3FHL J1041.7+3900 '</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>151.7499389648438</v>
+        <v>160.4421539306641</v>
       </c>
       <c r="D29" t="n">
-        <v>34.92112350463867</v>
+        <v>39.00973129272461</v>
       </c>
       <c r="E29" t="n">
-        <v>2277.828672355331</v>
+        <v>865.6075942787213</v>
       </c>
       <c r="F29" t="n">
-        <v>190.0282006580422</v>
+        <v>180.851954975237</v>
       </c>
       <c r="G29" t="n">
-        <v>54.17913076411402</v>
+        <v>60.55262642715537</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>b'3FHL J1008.0+0622 '</t>
+          <t>b'3FHL J1043.1+2409 '</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>152.0041351318359</v>
+        <v>160.7764892578125</v>
       </c>
       <c r="D30" t="n">
-        <v>6.373631954193115</v>
+        <v>24.15542984008789</v>
       </c>
       <c r="E30" t="n">
-        <v>2395.304963072071</v>
+        <v>2112.791679272088</v>
       </c>
       <c r="F30" t="n">
-        <v>233.50096097581</v>
+        <v>211.5515502940325</v>
       </c>
       <c r="G30" t="n">
-        <v>46.02256622120216</v>
+        <v>61.00195275957411</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>b'3FHL J1012.6+4228 '</t>
+          <t>b'3FHL J1051.4+3942 '</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>153.1730499267578</v>
+        <v>162.8575439453125</v>
       </c>
       <c r="D31" t="n">
-        <v>42.48298263549805</v>
+        <v>39.70672988891602</v>
       </c>
       <c r="E31" t="n">
-        <v>1447.954363211065</v>
+        <v>1909.393880329576</v>
       </c>
       <c r="F31" t="n">
-        <v>176.9216254086938</v>
+        <v>178.3920516037439</v>
       </c>
       <c r="G31" t="n">
-        <v>54.39503658450563</v>
+        <v>62.16010539961907</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>b'3FHL J1015.0+4926 '</t>
+          <t>b'3FHL J1053.6+4930 '</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>153.7693176269531</v>
+        <v>163.4012298583984</v>
       </c>
       <c r="D32" t="n">
-        <v>49.43538665771484</v>
+        <v>49.50532150268555</v>
       </c>
       <c r="E32" t="n">
-        <v>873.4307914196993</v>
+        <v>586.7293479424766</v>
       </c>
       <c r="F32" t="n">
-        <v>165.5301745409713</v>
+        <v>160.2472928171692</v>
       </c>
       <c r="G32" t="n">
-        <v>52.7128041733207</v>
+        <v>58.20941647675482</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>b'3FHL J1026.9+0608 '</t>
+          <t>b'3FHL J1058.6+5628 '</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>156.7403564453125</v>
+        <v>164.6645202636719</v>
       </c>
       <c r="D33" t="n">
-        <v>6.142007350921631</v>
+        <v>56.46826171875</v>
       </c>
       <c r="E33" t="n">
-        <v>1743.428171899722</v>
+        <v>598.8824976040644</v>
       </c>
       <c r="F33" t="n">
-        <v>237.7476753956505</v>
+        <v>149.5898498865417</v>
       </c>
       <c r="G33" t="n">
-        <v>49.78141165294394</v>
+        <v>54.42879075775696</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>b'3FHL J1027.5+6317 '</t>
+          <t>b'3FHL J1100.3+4020 '</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>156.8891754150391</v>
+        <v>165.0803070068359</v>
       </c>
       <c r="D34" t="n">
-        <v>63.29279327392578</v>
+        <v>40.3358268737793</v>
       </c>
       <c r="E34" t="n">
-        <v>2183.225532378438</v>
+        <v>924.0846438011745</v>
       </c>
       <c r="F34" t="n">
-        <v>145.6929541877977</v>
+        <v>175.8469476326254</v>
       </c>
       <c r="G34" t="n">
-        <v>46.97503063890456</v>
+        <v>63.555059895797</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>b'3FHL J1031.3+5053 '</t>
+          <t>b'3FHL J1104.4+3812 '</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>157.8328399658203</v>
+        <v>166.1207580566406</v>
       </c>
       <c r="D35" t="n">
-        <v>50.88592529296875</v>
+        <v>38.20518112182617</v>
       </c>
       <c r="E35" t="n">
-        <v>1433.534310193219</v>
+        <v>128.9003855881938</v>
       </c>
       <c r="F35" t="n">
-        <v>161.4466616146051</v>
+        <v>179.8357877680561</v>
       </c>
       <c r="G35" t="n">
-        <v>54.44603636948661</v>
+        <v>65.03781332953814</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>b'3FHL J1032.7+3737 '</t>
+          <t>b'3FHL J1105.8+3944 '</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>158.1970977783203</v>
+        <v>166.4540252685547</v>
       </c>
       <c r="D36" t="n">
-        <v>37.62113952636719</v>
+        <v>39.74899673461914</v>
       </c>
       <c r="E36" t="n">
-        <v>2008.723036449022</v>
+        <v>418.8482280609101</v>
       </c>
       <c r="F36" t="n">
-        <v>184.2725657102087</v>
+        <v>176.2092588270897</v>
       </c>
       <c r="G36" t="n">
-        <v>59.11119534742926</v>
+        <v>64.74895803570412</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>b'3FHL J1041.7+3900 '</t>
+          <t>b'3FHL J1107.8+1501 '</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>160.4421539306641</v>
+        <v>166.9655914306641</v>
       </c>
       <c r="D37" t="n">
-        <v>39.00973129272461</v>
+        <v>15.02733516693115</v>
       </c>
       <c r="E37" t="n">
-        <v>865.6075942787213</v>
+        <v>2240.185974418625</v>
       </c>
       <c r="F37" t="n">
-        <v>180.851954975237</v>
+        <v>234.34727958246</v>
       </c>
       <c r="G37" t="n">
-        <v>60.55262642715537</v>
+        <v>63.06038848548737</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>b'3FHL J1043.1+2409 '</t>
+          <t>b'3FHL J1109.7+3735 '</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>160.7764892578125</v>
+        <v>167.4311370849609</v>
       </c>
       <c r="D38" t="n">
-        <v>24.15542984008789</v>
+        <v>37.58807754516602</v>
       </c>
       <c r="E38" t="n">
-        <v>2112.791679272088</v>
+        <v>1563.657198577747</v>
       </c>
       <c r="F38" t="n">
-        <v>211.5515502940325</v>
+        <v>180.457347654663</v>
       </c>
       <c r="G38" t="n">
-        <v>61.00195275957411</v>
+        <v>66.2143548292574</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>b'3FHL J1051.4+3942 '</t>
+          <t>b'3FHL J1117.0+2014 '</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>162.8575439453125</v>
+        <v>169.2679595947266</v>
       </c>
       <c r="D39" t="n">
-        <v>39.70672988891602</v>
+        <v>20.23810386657715</v>
       </c>
       <c r="E39" t="n">
-        <v>1909.393880329576</v>
+        <v>578.6172947152628</v>
       </c>
       <c r="F39" t="n">
-        <v>178.3920516037439</v>
+        <v>225.5716267064807</v>
       </c>
       <c r="G39" t="n">
-        <v>62.16010539961907</v>
+        <v>67.36670331755562</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>b'3FHL J1053.6+4930 '</t>
+          <t>b'3FHL J1120.8+4212 '</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>163.4012298583984</v>
+        <v>170.2008819580078</v>
       </c>
       <c r="D40" t="n">
-        <v>49.50532150268555</v>
+        <v>42.20166015625</v>
       </c>
       <c r="E40" t="n">
-        <v>586.7293479424766</v>
+        <v>521.6104982541038</v>
       </c>
       <c r="F40" t="n">
-        <v>160.2472928171692</v>
+        <v>167.856902782118</v>
       </c>
       <c r="G40" t="n">
-        <v>58.20941647675482</v>
+        <v>66.16418823817627</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>b'3FHL J1058.6+5628 '</t>
+          <t>b'3FHL J1131.6+5809 '</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>164.6645202636719</v>
+        <v>172.9062042236328</v>
       </c>
       <c r="D41" t="n">
-        <v>56.46826171875</v>
+        <v>58.16561508178711</v>
       </c>
       <c r="E41" t="n">
-        <v>598.8824976040644</v>
+        <v>1429.924347323077</v>
       </c>
       <c r="F41" t="n">
-        <v>149.5898498865417</v>
+        <v>141.6893921444634</v>
       </c>
       <c r="G41" t="n">
-        <v>54.42879075775696</v>
+        <v>55.9604528362288</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>155</v>
+        <v>169</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>b'3FHL J1100.3+4020 '</t>
+          <t>b'3FHL J1136.8+2549 '</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>165.0803070068359</v>
+        <v>174.2185363769531</v>
       </c>
       <c r="D42" t="n">
-        <v>40.3358268737793</v>
+        <v>25.8327808380127</v>
       </c>
       <c r="E42" t="n">
-        <v>924.0846438011745</v>
+        <v>651.3386580792431</v>
       </c>
       <c r="F42" t="n">
-        <v>175.8469476326254</v>
+        <v>213.1465867327724</v>
       </c>
       <c r="G42" t="n">
-        <v>63.555059895797</v>
+        <v>73.27986298713279</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>b'3FHL J1104.4+3812 '</t>
+          <t>b'3FHL J1140.5+1528 '</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>166.1207580566406</v>
+        <v>175.1320648193359</v>
       </c>
       <c r="D43" t="n">
-        <v>38.20518112182617</v>
+        <v>15.48001480102539</v>
       </c>
       <c r="E43" t="n">
-        <v>128.9003855881938</v>
+        <v>997.5030593997925</v>
       </c>
       <c r="F43" t="n">
-        <v>179.8357877680561</v>
+        <v>244.6038972738466</v>
       </c>
       <c r="G43" t="n">
-        <v>65.03781332953814</v>
+        <v>69.83077528557813</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>b'3FHL J1105.8+3944 '</t>
+          <t>b'3FHL J1142.0+1546 '</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>166.4540252685547</v>
+        <v>175.5173187255859</v>
       </c>
       <c r="D44" t="n">
-        <v>39.74899673461914</v>
+        <v>15.77690410614014</v>
       </c>
       <c r="E44" t="n">
-        <v>418.8482280609101</v>
+        <v>1205.915061750614</v>
       </c>
       <c r="F44" t="n">
-        <v>176.2092588270897</v>
+        <v>244.5908969669972</v>
       </c>
       <c r="G44" t="n">
-        <v>64.74895803570412</v>
+        <v>70.30592729967964</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>159</v>
+        <v>174</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>b'3FHL J1107.8+1501 '</t>
+          <t>b'3FHL J1145.0+1935 '</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>166.9655914306641</v>
+        <v>176.2684783935547</v>
       </c>
       <c r="D45" t="n">
-        <v>15.02733516693115</v>
+        <v>19.5903205871582</v>
       </c>
       <c r="E45" t="n">
-        <v>2240.185974418625</v>
+        <v>93.48446529540507</v>
       </c>
       <c r="F45" t="n">
-        <v>234.34727958246</v>
+        <v>235.771105621029</v>
       </c>
       <c r="G45" t="n">
-        <v>63.06038848548737</v>
+        <v>73.02859819966865</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>160</v>
+        <v>175</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>b'3FHL J1109.7+3735 '</t>
+          <t>b'3FHL J1150.3+2418 '</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>167.4311370849609</v>
+        <v>177.5877227783203</v>
       </c>
       <c r="D46" t="n">
-        <v>37.58807754516602</v>
+        <v>24.30084228515625</v>
       </c>
       <c r="E46" t="n">
-        <v>1563.657198577747</v>
+        <v>826.3707136061979</v>
       </c>
       <c r="F46" t="n">
-        <v>180.457347654663</v>
+        <v>221.1457388558182</v>
       </c>
       <c r="G46" t="n">
-        <v>66.2143548292574</v>
+        <v>75.96302613210874</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>161</v>
+        <v>176</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>b'3FHL J1117.0+2014 '</t>
+          <t>b'3FHL J1153.2+4929 '</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>169.2679595947266</v>
+        <v>178.3224639892578</v>
       </c>
       <c r="D47" t="n">
-        <v>20.23810386657715</v>
+        <v>49.49262237548828</v>
       </c>
       <c r="E47" t="n">
-        <v>578.6172947152628</v>
+        <v>1335.3602067056</v>
       </c>
       <c r="F47" t="n">
-        <v>225.5716267064807</v>
+        <v>145.6204816776282</v>
       </c>
       <c r="G47" t="n">
-        <v>67.36670331755562</v>
+        <v>64.99564919843898</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>163</v>
+        <v>179</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>b'3FHL J1120.8+4212 '</t>
+          <t>b'3FHL J1203.1+6030 '</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>170.2008819580078</v>
+        <v>180.7808227539062</v>
       </c>
       <c r="D48" t="n">
-        <v>42.20166015625</v>
+        <v>60.51219177246094</v>
       </c>
       <c r="E48" t="n">
-        <v>521.6104982541038</v>
+        <v>277.125303444809</v>
       </c>
       <c r="F48" t="n">
-        <v>167.856902782118</v>
+        <v>133.4418834029724</v>
       </c>
       <c r="G48" t="n">
-        <v>66.16418823817627</v>
+        <v>55.61926798865239</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>166</v>
+        <v>182</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>b'3FHL J1131.6+5809 '</t>
+          <t>b'3FHL J1208.1+6120 '</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>172.9062042236328</v>
+        <v>182.0427551269531</v>
       </c>
       <c r="D49" t="n">
-        <v>58.16561508178711</v>
+        <v>61.34061431884766</v>
       </c>
       <c r="E49" t="n">
-        <v>1429.924347323077</v>
+        <v>1115.723809237682</v>
       </c>
       <c r="F49" t="n">
-        <v>141.6893921444634</v>
+        <v>131.9651880062851</v>
       </c>
       <c r="G49" t="n">
-        <v>55.9604528362288</v>
+        <v>55.02232038849426</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>b'3FHL J1136.8+2549 '</t>
+          <t>b'3FHL J1217.9+3006 '</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>174.2185363769531</v>
+        <v>184.4772338867188</v>
       </c>
       <c r="D50" t="n">
-        <v>25.8327808380127</v>
+        <v>30.11482238769531</v>
       </c>
       <c r="E50" t="n">
-        <v>651.3386580792431</v>
+        <v>546.0896141426656</v>
       </c>
       <c r="F50" t="n">
-        <v>213.1465867327724</v>
+        <v>188.8666537572836</v>
       </c>
       <c r="G50" t="n">
-        <v>73.27986298713279</v>
+        <v>82.06187773446577</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>171</v>
+        <v>189</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>b'3FHL J1140.5+1528 '</t>
+          <t>b'3FHL J1221.3+3010 '</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>175.1320648193359</v>
+        <v>185.3371734619141</v>
       </c>
       <c r="D51" t="n">
-        <v>15.48001480102539</v>
+        <v>30.16693115234375</v>
       </c>
       <c r="E51" t="n">
-        <v>997.5030593997925</v>
+        <v>763.1726232934241</v>
       </c>
       <c r="F51" t="n">
-        <v>244.6038972738466</v>
+        <v>186.4431504600458</v>
       </c>
       <c r="G51" t="n">
-        <v>69.83077528557813</v>
+        <v>82.7350715996196</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>172</v>
+        <v>190</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>b'3FHL J1142.0+1546 '</t>
+          <t>b'3FHL J1221.5+2813 '</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>175.5173187255859</v>
+        <v>185.3848114013672</v>
       </c>
       <c r="D52" t="n">
-        <v>15.77690410614014</v>
+        <v>28.23212242126465</v>
       </c>
       <c r="E52" t="n">
-        <v>1205.915061750614</v>
+        <v>431.2447065513599</v>
       </c>
       <c r="F52" t="n">
-        <v>244.5908969669972</v>
+        <v>201.7391806851846</v>
       </c>
       <c r="G52" t="n">
-        <v>70.30592729967964</v>
+        <v>83.29053790221776</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>173</v>
+        <v>191</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>b'3FHL J1143.1+6121 '</t>
+          <t>b'3FHL J1224.4+2436 '</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>175.7978515625</v>
+        <v>186.1085205078125</v>
       </c>
       <c r="D53" t="n">
-        <v>61.35290145874023</v>
+        <v>24.6070442199707</v>
       </c>
       <c r="E53" t="n">
-        <v>209.6566093130006</v>
+        <v>900.7483492023172</v>
       </c>
       <c r="F53" t="n">
-        <v>136.7459514614812</v>
+        <v>233.9729892145359</v>
       </c>
       <c r="G53" t="n">
-        <v>53.90689117248857</v>
+        <v>83.42441521408441</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>b'3FHL J1145.0+1935 '</t>
+          <t>b'3FHL J1224.9+2122 '</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>176.2684783935547</v>
+        <v>186.2270355224609</v>
       </c>
       <c r="D54" t="n">
-        <v>19.5903205871582</v>
+        <v>21.38190269470215</v>
       </c>
       <c r="E54" t="n">
-        <v>93.48446529540507</v>
+        <v>1691.687106632469</v>
       </c>
       <c r="F54" t="n">
-        <v>235.771105621029</v>
+        <v>255.0624608818417</v>
       </c>
       <c r="G54" t="n">
-        <v>73.02859819966865</v>
+        <v>81.66152573596764</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>175</v>
+        <v>195</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>b'3FHL J1150.3+2418 '</t>
+          <t>b'3FHL J1229.2+0201 '</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>177.5877227783203</v>
+        <v>187.3038330078125</v>
       </c>
       <c r="D55" t="n">
-        <v>24.30084228515625</v>
+        <v>2.024992942810059</v>
       </c>
       <c r="E55" t="n">
-        <v>826.3707136061979</v>
+        <v>659.3789000935117</v>
       </c>
       <c r="F55" t="n">
-        <v>221.1457388558182</v>
+        <v>290.0221226405291</v>
       </c>
       <c r="G55" t="n">
-        <v>75.96302613210874</v>
+        <v>64.33829691205085</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>176</v>
+        <v>196</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>b'3FHL J1153.2+4929 '</t>
+          <t>b'3FHL J1230.2+2517 '</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>178.3224639892578</v>
+        <v>187.5732727050781</v>
       </c>
       <c r="D56" t="n">
-        <v>49.49262237548828</v>
+        <v>25.29787635803223</v>
       </c>
       <c r="E56" t="n">
-        <v>1335.3602067056</v>
+        <v>566.434356575713</v>
       </c>
       <c r="F56" t="n">
-        <v>145.6204816776282</v>
+        <v>232.8530732554522</v>
       </c>
       <c r="G56" t="n">
-        <v>64.99564919843898</v>
+        <v>84.91711617677194</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>179</v>
+        <v>197</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>b'3FHL J1203.1+6030 '</t>
+          <t>b'3FHL J1230.8+1223 '</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>180.7808227539062</v>
+        <v>187.7033386230469</v>
       </c>
       <c r="D57" t="n">
-        <v>60.51219177246094</v>
+        <v>12.38887977600098</v>
       </c>
       <c r="E57" t="n">
-        <v>277.125303444809</v>
+        <v>18.50588103089174</v>
       </c>
       <c r="F57" t="n">
-        <v>133.4418834029724</v>
+        <v>283.7712082555389</v>
       </c>
       <c r="G57" t="n">
-        <v>55.61926798865239</v>
+        <v>74.48825666506053</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>182</v>
+        <v>198</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>b'3FHL J1208.1+6120 '</t>
+          <t>b'3FHL J1231.4+1422 '</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>182.0427551269531</v>
+        <v>187.8662414550781</v>
       </c>
       <c r="D58" t="n">
-        <v>61.34061431884766</v>
+        <v>14.3680305480957</v>
       </c>
       <c r="E58" t="n">
-        <v>1115.723809237682</v>
+        <v>1043.496525858729</v>
       </c>
       <c r="F58" t="n">
-        <v>131.9651880062851</v>
+        <v>281.8921172763349</v>
       </c>
       <c r="G58" t="n">
-        <v>55.02232038849426</v>
+        <v>76.41707829778731</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>184</v>
+        <v>200</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>b'3FHL J1216.0-0242 '</t>
+          <t>b'3FHL J1231.7+2847 '</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>184.0193023681641</v>
+        <v>187.9381866455078</v>
       </c>
       <c r="D59" t="n">
-        <v>-2.713768005371094</v>
+        <v>28.79290008544922</v>
       </c>
       <c r="E59" t="n">
-        <v>1426.312274688342</v>
+        <v>968.4201348245213</v>
       </c>
       <c r="F59" t="n">
-        <v>285.6103354390478</v>
+        <v>190.8352813272477</v>
       </c>
       <c r="G59" t="n">
-        <v>58.96364214349016</v>
+        <v>85.34586086634012</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>185</v>
+        <v>204</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>b'3FHL J1217.9+3006 '</t>
+          <t>b'3FHL J1247.0+4421 '</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>184.4772338867188</v>
+        <v>191.7523803710938</v>
       </c>
       <c r="D60" t="n">
-        <v>30.11482238769531</v>
+        <v>44.35237503051758</v>
       </c>
       <c r="E60" t="n">
-        <v>546.0896141426656</v>
+        <v>2240.185974418625</v>
       </c>
       <c r="F60" t="n">
-        <v>188.8666537572836</v>
+        <v>125.6027117904971</v>
       </c>
       <c r="G60" t="n">
-        <v>82.06187773446577</v>
+        <v>72.75290303465637</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>186</v>
+        <v>206</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>b'3FHL J1218.0-0028 '</t>
+          <t>b'3FHL J1253.7+0328 '</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>184.51953125</v>
+        <v>193.4472503662109</v>
       </c>
       <c r="D61" t="n">
-        <v>-0.4782386422157288</v>
+        <v>3.473009824752808</v>
       </c>
       <c r="E61" t="n">
-        <v>1639.503972536957</v>
+        <v>281.3257125002922</v>
       </c>
       <c r="F61" t="n">
-        <v>285.3804349262129</v>
+        <v>304.3938914960014</v>
       </c>
       <c r="G61" t="n">
-        <v>61.25154181229235</v>
+        <v>66.33808457924333</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>187</v>
+        <v>207</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>b'3FHL J1219.7-0312 '</t>
+          <t>b'3FHL J1254.4+2210 '</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>184.9271392822266</v>
+        <v>193.6058959960938</v>
       </c>
       <c r="D62" t="n">
-        <v>-3.212921857833862</v>
+        <v>22.18258476257324</v>
       </c>
       <c r="E62" t="n">
-        <v>1205.915061750614</v>
+        <v>1946.014319805091</v>
       </c>
       <c r="F62" t="n">
-        <v>287.5483319154165</v>
+        <v>310.9003864000454</v>
       </c>
       <c r="G62" t="n">
-        <v>58.70790553974744</v>
+        <v>85.00807392479871</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>189</v>
+        <v>210</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>b'3FHL J1221.3+3010 '</t>
+          <t>b'3FHL J1258.3+6121 '</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>185.3371734619141</v>
+        <v>194.5815887451172</v>
       </c>
       <c r="D63" t="n">
-        <v>30.16693115234375</v>
+        <v>61.36655807495117</v>
       </c>
       <c r="E63" t="n">
-        <v>763.1726232934241</v>
+        <v>920.2003591656152</v>
       </c>
       <c r="F63" t="n">
-        <v>186.4431504600458</v>
+        <v>121.4659798152458</v>
       </c>
       <c r="G63" t="n">
-        <v>82.7350715996196</v>
+        <v>55.7420815224022</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>190</v>
+        <v>213</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>b'3FHL J1221.5+2813 '</t>
+          <t>b'3FHL J1312.6+4828 '</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>185.3848114013672</v>
+        <v>198.1574249267578</v>
       </c>
       <c r="D64" t="n">
-        <v>28.23212242126465</v>
+        <v>48.47776031494141</v>
       </c>
       <c r="E64" t="n">
-        <v>431.2447065513599</v>
+        <v>1919.40425528274</v>
       </c>
       <c r="F64" t="n">
-        <v>201.7391806851846</v>
+        <v>113.4210086615013</v>
       </c>
       <c r="G64" t="n">
-        <v>83.29053790221776</v>
+        <v>68.25727662537837</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>191</v>
+        <v>216</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>b'3FHL J1224.4+2436 '</t>
+          <t>b'3FHL J1319.5+1404 '</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>186.1085205078125</v>
+        <v>199.8961791992188</v>
       </c>
       <c r="D65" t="n">
-        <v>24.6070442199707</v>
+        <v>14.07064819335938</v>
       </c>
       <c r="E65" t="n">
-        <v>900.7483492023172</v>
+        <v>2154.520586195584</v>
       </c>
       <c r="F65" t="n">
-        <v>233.9729892145359</v>
+        <v>331.0264520499293</v>
       </c>
       <c r="G65" t="n">
-        <v>83.42441521408441</v>
+        <v>75.38452389248357</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>192</v>
+        <v>220</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>b'3FHL J1224.9+2122 '</t>
+          <t>b'3FHL J1340.5+4410 '</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>186.2270355224609</v>
+        <v>205.1303100585938</v>
       </c>
       <c r="D66" t="n">
-        <v>21.38190269470215</v>
+        <v>44.18074798583984</v>
       </c>
       <c r="E66" t="n">
-        <v>1691.687106632469</v>
+        <v>2067.499118066273</v>
       </c>
       <c r="F66" t="n">
-        <v>255.0624608818417</v>
+        <v>96.05410900986132</v>
       </c>
       <c r="G66" t="n">
-        <v>81.66152573596764</v>
+        <v>70.29735077732514</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>195</v>
+        <v>221</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>b'3FHL J1229.2+0201 '</t>
+          <t>b'3FHL J1341.2+3959 '</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>187.3038330078125</v>
+        <v>205.3132781982422</v>
       </c>
       <c r="D67" t="n">
-        <v>2.024992942810059</v>
+        <v>39.98970031738281</v>
       </c>
       <c r="E67" t="n">
-        <v>659.3789000935117</v>
+        <v>715.4362988699944</v>
       </c>
       <c r="F67" t="n">
-        <v>290.0221226405291</v>
+        <v>87.33566812682206</v>
       </c>
       <c r="G67" t="n">
-        <v>64.33829691205085</v>
+        <v>73.50951317099407</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>b'3FHL J1230.2+2517 '</t>
+          <t>b'3FHL J1402.6+1559 '</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>187.5732727050781</v>
+        <v>210.6538238525391</v>
       </c>
       <c r="D68" t="n">
-        <v>25.29787635803223</v>
+        <v>15.98397254943848</v>
       </c>
       <c r="E68" t="n">
-        <v>566.434356575713</v>
+        <v>997.5030593997925</v>
       </c>
       <c r="F68" t="n">
-        <v>232.8530732554522</v>
+        <v>2.539795875341265</v>
       </c>
       <c r="G68" t="n">
-        <v>84.91711617677194</v>
+        <v>70.08723433248876</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>197</v>
+        <v>225</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>b'3FHL J1230.8+1223 '</t>
+          <t>b'3FHL J1404.9+0401 '</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>187.7033386230469</v>
+        <v>211.2331237792969</v>
       </c>
       <c r="D69" t="n">
-        <v>12.38887977600098</v>
+        <v>4.028957843780518</v>
       </c>
       <c r="E69" t="n">
-        <v>18.50588103089174</v>
+        <v>1371.891644524125</v>
       </c>
       <c r="F69" t="n">
-        <v>283.7712082555389</v>
+        <v>343.356454326494</v>
       </c>
       <c r="G69" t="n">
-        <v>74.48825666506053</v>
+        <v>60.99387507635056</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>198</v>
+        <v>226</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>b'3FHL J1231.4+1422 '</t>
+          <t>b'3FHL J1411.8+5249 '</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>187.8662414550781</v>
+        <v>212.9649963378906</v>
       </c>
       <c r="D70" t="n">
-        <v>14.3680305480957</v>
+        <v>52.82292938232422</v>
       </c>
       <c r="E70" t="n">
-        <v>1043.496525858729</v>
+        <v>325.2711537377689</v>
       </c>
       <c r="F70" t="n">
-        <v>281.8921172763349</v>
+        <v>98.17146981808737</v>
       </c>
       <c r="G70" t="n">
-        <v>76.41707829778731</v>
+        <v>60.26679845594848</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>199</v>
+        <v>227</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>b'3FHL J1231.6+6415 '</t>
+          <t>b'3FHL J1415.6+4830 '</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>187.9054565429688</v>
+        <v>213.9147796630859</v>
       </c>
       <c r="D71" t="n">
-        <v>64.26630401611328</v>
+        <v>48.51522445678711</v>
       </c>
       <c r="E71" t="n">
-        <v>679.4444413307867</v>
+        <v>1902.710656439457</v>
       </c>
       <c r="F71" t="n">
-        <v>126.4813572877882</v>
+        <v>91.19850370499088</v>
       </c>
       <c r="G71" t="n">
-        <v>52.72516890602747</v>
+        <v>63.09742003770977</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>200</v>
+        <v>229</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>b'3FHL J1231.7+2847 '</t>
+          <t>b'3FHL J1418.0+2543 '</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>187.9381866455078</v>
+        <v>214.5009460449219</v>
       </c>
       <c r="D72" t="n">
-        <v>28.79290008544922</v>
+        <v>25.7291259765625</v>
       </c>
       <c r="E72" t="n">
-        <v>968.4201348245213</v>
+        <v>970.5390841006508</v>
       </c>
       <c r="F72" t="n">
-        <v>190.8352813272477</v>
+        <v>33.71460610300097</v>
       </c>
       <c r="G72" t="n">
-        <v>85.34586086634012</v>
+        <v>70.59372559903728</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>204</v>
+        <v>230</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>b'3FHL J1247.0+4421 '</t>
+          <t>b'3FHL J1419.4+0444 '</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>191.7523803710938</v>
+        <v>214.8675231933594</v>
       </c>
       <c r="D73" t="n">
-        <v>44.35237503051758</v>
+        <v>4.745282173156738</v>
       </c>
       <c r="E73" t="n">
-        <v>2240.185974418625</v>
+        <v>598.8824976040644</v>
       </c>
       <c r="F73" t="n">
-        <v>125.6027117904971</v>
+        <v>349.978509379617</v>
       </c>
       <c r="G73" t="n">
-        <v>72.75290303465637</v>
+        <v>59.3198698029064</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>206</v>
+        <v>231</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>b'3FHL J1253.7+0328 '</t>
+          <t>b'3FHL J1419.7+5423 '</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>193.4472503662109</v>
+        <v>214.9465789794922</v>
       </c>
       <c r="D74" t="n">
-        <v>3.473009824752808</v>
+        <v>54.39066696166992</v>
       </c>
       <c r="E74" t="n">
-        <v>281.3257125002922</v>
+        <v>639.2633050973789</v>
       </c>
       <c r="F74" t="n">
-        <v>304.3938914960014</v>
+        <v>98.30243691724219</v>
       </c>
       <c r="G74" t="n">
-        <v>66.33808457924333</v>
+        <v>58.30848489225325</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>207</v>
+        <v>233</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>b'3FHL J1254.4+2210 '</t>
+          <t>b'3FHL J1428.5+4240 '</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>193.6058959960938</v>
+        <v>217.1364593505859</v>
       </c>
       <c r="D75" t="n">
-        <v>22.18258476257324</v>
+        <v>42.67203521728516</v>
       </c>
       <c r="E75" t="n">
-        <v>1946.014319805091</v>
+        <v>542.0147093189177</v>
       </c>
       <c r="F75" t="n">
-        <v>310.9003864000454</v>
+        <v>77.48566790521888</v>
       </c>
       <c r="G75" t="n">
-        <v>85.00807392479871</v>
+        <v>64.8988126310412</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>208</v>
+        <v>235</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>b'3FHL J1256.1-0547 '</t>
+          <t>b'3FHL J1439.3+3931 '</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>194.0442810058594</v>
+        <v>219.8288269042969</v>
       </c>
       <c r="D76" t="n">
-        <v>-5.79459285736084</v>
+        <v>39.52298355102539</v>
       </c>
       <c r="E76" t="n">
-        <v>2034.921432753547</v>
+        <v>1371.891644524125</v>
       </c>
       <c r="F76" t="n">
-        <v>305.0998846118308</v>
+        <v>68.79583747417368</v>
       </c>
       <c r="G76" t="n">
-        <v>57.05720524664127</v>
+        <v>64.42668452711504</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>210</v>
+        <v>236</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>b'3FHL J1258.3+6121 '</t>
+          <t>b'3FHL J1440.9+0610 '</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>194.5815887451172</v>
+        <v>220.2337188720703</v>
       </c>
       <c r="D77" t="n">
-        <v>61.36655807495117</v>
+        <v>6.175134658813477</v>
       </c>
       <c r="E77" t="n">
-        <v>920.2003591656152</v>
+        <v>1558.62649529763</v>
       </c>
       <c r="F77" t="n">
-        <v>121.4659798152458</v>
+        <v>359.0613035363558</v>
       </c>
       <c r="G77" t="n">
-        <v>55.7420815224022</v>
+        <v>56.59426497141165</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>b'3FHL J1312.6+4828 '</t>
+          <t>b'3FHL J1442.8+1200 '</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>198.1574249267578</v>
+        <v>220.7103729248047</v>
       </c>
       <c r="D78" t="n">
-        <v>48.47776031494141</v>
+        <v>12.00308227539062</v>
       </c>
       <c r="E78" t="n">
-        <v>1919.40425528274</v>
+        <v>679.4444413307867</v>
       </c>
       <c r="F78" t="n">
-        <v>113.4210086615013</v>
+        <v>8.326391244799357</v>
       </c>
       <c r="G78" t="n">
-        <v>68.25727662537837</v>
+        <v>59.82810578059493</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>216</v>
+        <v>238</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>b'3FHL J1319.5+1404 '</t>
+          <t>b'3FHL J1443.5+2515 '</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>199.8961791992188</v>
+        <v>220.8969116210938</v>
       </c>
       <c r="D79" t="n">
-        <v>14.07064819335938</v>
+        <v>25.26393508911133</v>
       </c>
       <c r="E79" t="n">
-        <v>2154.520586195584</v>
+        <v>2012.076573556624</v>
       </c>
       <c r="F79" t="n">
-        <v>331.0264520499293</v>
+        <v>35.06898725925156</v>
       </c>
       <c r="G79" t="n">
-        <v>75.38452389248357</v>
+        <v>64.8249872712824</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>220</v>
+        <v>240</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>b'3FHL J1340.5+4410 '</t>
+          <t>b'3FHL J1449.5+2745 '</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>205.1303100585938</v>
+        <v>222.3851776123047</v>
       </c>
       <c r="D80" t="n">
-        <v>44.18074798583984</v>
+        <v>27.75633811950684</v>
       </c>
       <c r="E80" t="n">
-        <v>2067.499118066273</v>
+        <v>931.8472681578297</v>
       </c>
       <c r="F80" t="n">
-        <v>96.05410900986132</v>
+        <v>41.19890036398075</v>
       </c>
       <c r="G80" t="n">
-        <v>70.29735077732514</v>
+        <v>63.8522071735304</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>221</v>
+        <v>242</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>b'3FHL J1341.2+3959 '</t>
+          <t>b'3FHL J1458.7+3722 '</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>205.3132781982422</v>
+        <v>224.6948089599609</v>
       </c>
       <c r="D81" t="n">
-        <v>39.98970031738281</v>
+        <v>37.36803436279297</v>
       </c>
       <c r="E81" t="n">
-        <v>715.4362988699944</v>
+        <v>1331.696061964219</v>
       </c>
       <c r="F81" t="n">
-        <v>87.33566812682206</v>
+        <v>61.92235747685517</v>
       </c>
       <c r="G81" t="n">
-        <v>73.50951317099407</v>
+        <v>61.36237350674613</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>223</v>
+        <v>243</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>b'3FHL J1402.6+1559 '</t>
+          <t>b'3FHL J1500.9+2238 '</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>210.6538238525391</v>
+        <v>225.2482757568359</v>
       </c>
       <c r="D82" t="n">
-        <v>15.98397254943848</v>
+        <v>22.64022445678711</v>
       </c>
       <c r="E82" t="n">
-        <v>997.5030593997925</v>
+        <v>962.8168789726126</v>
       </c>
       <c r="F82" t="n">
-        <v>2.539795875341265</v>
+        <v>31.45102290888001</v>
       </c>
       <c r="G82" t="n">
-        <v>70.08723433248876</v>
+        <v>60.35999634319712</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>225</v>
+        <v>244</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>b'3FHL J1404.9+0401 '</t>
+          <t>b'3FHL J1503.3+4758 '</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>211.2331237792969</v>
+        <v>225.8384399414062</v>
       </c>
       <c r="D83" t="n">
-        <v>4.028957843780518</v>
+        <v>47.97346878051758</v>
       </c>
       <c r="E83" t="n">
         <v>1371.891644524125</v>
       </c>
       <c r="F83" t="n">
-        <v>343.356454326494</v>
+        <v>80.9535755751856</v>
       </c>
       <c r="G83" t="n">
-        <v>60.99387507635056</v>
+        <v>56.98629153475792</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>226</v>
+        <v>245</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>b'3FHL J1411.8+5249 '</t>
+          <t>b'3FHL J1506.0+3732 '</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>212.9649963378906</v>
+        <v>226.5228424072266</v>
       </c>
       <c r="D84" t="n">
-        <v>52.82292938232422</v>
+        <v>37.54251480102539</v>
       </c>
       <c r="E84" t="n">
-        <v>325.2711537377689</v>
+        <v>2465.150914639177</v>
       </c>
       <c r="F84" t="n">
-        <v>98.17146981808737</v>
+        <v>61.70862488595789</v>
       </c>
       <c r="G84" t="n">
-        <v>60.26679845594848</v>
+        <v>59.90456332383156</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>227</v>
+        <v>246</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>b'3FHL J1415.6+4830 '</t>
+          <t>b'3FHL J1506.7+0813 '</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>213.9147796630859</v>
+        <v>226.6905822753906</v>
       </c>
       <c r="D85" t="n">
-        <v>48.51522445678711</v>
+        <v>8.218801498413086</v>
       </c>
       <c r="E85" t="n">
-        <v>1902.710656439457</v>
+        <v>1487.444413390686</v>
       </c>
       <c r="F85" t="n">
-        <v>91.19850370499088</v>
+        <v>8.730330769087979</v>
       </c>
       <c r="G85" t="n">
-        <v>63.09742003770977</v>
+        <v>52.83404159105811</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>229</v>
+        <v>247</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>b'3FHL J1418.0+2543 '</t>
+          <t>b'3FHL J1507.2+1722 '</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>214.5009460449219</v>
+        <v>226.8249816894531</v>
       </c>
       <c r="D86" t="n">
-        <v>25.7291259765625</v>
+        <v>17.36773490905762</v>
       </c>
       <c r="E86" t="n">
-        <v>970.5390841006508</v>
+        <v>2129.778114886851</v>
       </c>
       <c r="F86" t="n">
-        <v>33.71460610300097</v>
+        <v>22.80134452177674</v>
       </c>
       <c r="G86" t="n">
-        <v>70.59372559903728</v>
+        <v>57.20281900749549</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>230</v>
+        <v>248</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>b'3FHL J1419.4+0444 '</t>
+          <t>b'3FHL J1508.7+2708 '</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>214.8675231933594</v>
+        <v>227.1883544921875</v>
       </c>
       <c r="D87" t="n">
-        <v>4.745282173156738</v>
+        <v>27.14417457580566</v>
       </c>
       <c r="E87" t="n">
-        <v>598.8824976040644</v>
+        <v>1096.787424633644</v>
       </c>
       <c r="F87" t="n">
-        <v>349.978509379617</v>
+        <v>40.97986187978024</v>
       </c>
       <c r="G87" t="n">
-        <v>59.3198698029064</v>
+        <v>59.54763194954369</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>231</v>
+        <v>250</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>b'3FHL J1419.7+5423 '</t>
+          <t>b'3FHL J1512.2+0203 '</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>214.9465789794922</v>
+        <v>228.0720062255859</v>
       </c>
       <c r="D88" t="n">
-        <v>54.39066696166992</v>
+        <v>2.060366868972778</v>
       </c>
       <c r="E88" t="n">
-        <v>639.2633050973789</v>
+        <v>904.6427903224928</v>
       </c>
       <c r="F88" t="n">
-        <v>98.30243691724219</v>
+        <v>2.367075362555521</v>
       </c>
       <c r="G88" t="n">
-        <v>58.30848489225325</v>
+        <v>47.99279308444518</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>232</v>
+        <v>253</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>b'3FHL J1422.6+5801 '</t>
+          <t>b'3FHL J1518.5+4044 '</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>215.6541900634766</v>
+        <v>229.6453247070312</v>
       </c>
       <c r="D89" t="n">
-        <v>58.01887893676758</v>
+        <v>40.73994827270508</v>
       </c>
       <c r="E89" t="n">
-        <v>2349.244257634401</v>
+        <v>277.125303444809</v>
       </c>
       <c r="F89" t="n">
-        <v>101.8492086867801</v>
+        <v>66.76651396705567</v>
       </c>
       <c r="G89" t="n">
-        <v>55.21857129706387</v>
+        <v>56.89182212745664</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>233</v>
+        <v>254</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>b'3FHL J1428.5+4240 '</t>
+          <t>b'3FHL J1531.9+3016 '</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>217.1364593505859</v>
+        <v>232.9860992431641</v>
       </c>
       <c r="D90" t="n">
-        <v>42.67203521728516</v>
+        <v>30.27317047119141</v>
       </c>
       <c r="E90" t="n">
-        <v>542.0147093189177</v>
+        <v>277.125303444809</v>
       </c>
       <c r="F90" t="n">
-        <v>77.48566790521888</v>
+        <v>47.77962265205297</v>
       </c>
       <c r="G90" t="n">
-        <v>64.8988126310412</v>
+        <v>54.84301768980958</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>234</v>
+        <v>255</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>b'3FHL J1436.9+5639 '</t>
+          <t>b'3FHL J1533.2+1855 '</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>219.2470092773438</v>
+        <v>233.3144226074219</v>
       </c>
       <c r="D91" t="n">
-        <v>56.66003799438477</v>
+        <v>18.93068313598633</v>
       </c>
       <c r="E91" t="n">
-        <v>627.1700359849448</v>
+        <v>1235.720342438146</v>
       </c>
       <c r="F91" t="n">
-        <v>97.72870692965985</v>
+        <v>29.25278554792897</v>
       </c>
       <c r="G91" t="n">
-        <v>54.99658828453175</v>
+        <v>52.0464613686915</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>235</v>
+        <v>256</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>b'3FHL J1439.3+3931 '</t>
+          <t>b'3FHL J1540.7+1448 '</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>219.8288269042969</v>
+        <v>235.1949615478516</v>
       </c>
       <c r="D92" t="n">
-        <v>39.52298355102539</v>
+        <v>14.81568145751953</v>
       </c>
       <c r="E92" t="n">
-        <v>1371.891644524125</v>
+        <v>2255.902501594245</v>
       </c>
       <c r="F92" t="n">
-        <v>68.79583747417368</v>
+        <v>24.34762000956751</v>
       </c>
       <c r="G92" t="n">
-        <v>64.42668452711504</v>
+        <v>48.81774577195303</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>236</v>
+        <v>258</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>b'3FHL J1440.9+0610 '</t>
+          <t>b'3FHL J1543.6+0452 '</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>220.2337188720703</v>
+        <v>235.9000091552734</v>
       </c>
       <c r="D93" t="n">
-        <v>6.175134658813477</v>
+        <v>4.879972457885742</v>
       </c>
       <c r="E93" t="n">
-        <v>1558.62649529763</v>
+        <v>171.3237639398314</v>
       </c>
       <c r="F93" t="n">
-        <v>359.0613035363558</v>
+        <v>12.27756886738662</v>
       </c>
       <c r="G93" t="n">
-        <v>56.59426497141165</v>
+        <v>43.38510723073886</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>237</v>
+        <v>260</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>b'3FHL J1442.8+1200 '</t>
+          <t>b'3FHL J1554.2+2010 '</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>220.7103729248047</v>
+        <v>238.5714263916016</v>
       </c>
       <c r="D94" t="n">
-        <v>12.00308227539062</v>
+        <v>20.17705154418945</v>
       </c>
       <c r="E94" t="n">
-        <v>679.4444413307867</v>
+        <v>912.4256141983458</v>
       </c>
       <c r="F94" t="n">
-        <v>8.326391244799357</v>
+        <v>33.62416920162958</v>
       </c>
       <c r="G94" t="n">
-        <v>59.82810578059493</v>
+        <v>47.78168755695976</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>238</v>
+        <v>263</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>b'3FHL J1443.5+2515 '</t>
+          <t>b'3FHL J1603.8+1103 '</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>220.8969116210938</v>
+        <v>240.9507446289062</v>
       </c>
       <c r="D95" t="n">
-        <v>25.26393508911133</v>
+        <v>11.0573263168335</v>
       </c>
       <c r="E95" t="n">
-        <v>2012.076573556624</v>
+        <v>598.8824976040644</v>
       </c>
       <c r="F95" t="n">
-        <v>35.06898725925156</v>
+        <v>22.97464182629868</v>
       </c>
       <c r="G95" t="n">
-        <v>64.8249872712824</v>
+        <v>42.13516682302727</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>240</v>
+        <v>266</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>b'3FHL J1449.5+2745 '</t>
+          <t>b'3FHL J1607.0+1550 '</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>222.3851776123047</v>
+        <v>241.7560882568359</v>
       </c>
       <c r="D96" t="n">
-        <v>27.75633811950684</v>
+        <v>15.83572101593018</v>
       </c>
       <c r="E96" t="n">
-        <v>931.8472681578297</v>
+        <v>1902.710656439457</v>
       </c>
       <c r="F96" t="n">
-        <v>41.19890036398075</v>
+        <v>29.33763480478526</v>
       </c>
       <c r="G96" t="n">
-        <v>63.8522071735304</v>
+        <v>43.41828545322375</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>242</v>
+        <v>268</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>b'3FHL J1458.7+3722 '</t>
+          <t>b'3FHL J1626.2+3515 '</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>224.6948089599609</v>
+        <v>246.5747680664062</v>
       </c>
       <c r="D97" t="n">
-        <v>37.36803436279297</v>
+        <v>35.26229095458984</v>
       </c>
       <c r="E97" t="n">
-        <v>1331.696061964219</v>
+        <v>1907.322882417562</v>
       </c>
       <c r="F97" t="n">
-        <v>61.92235747685517</v>
+        <v>56.96303155478957</v>
       </c>
       <c r="G97" t="n">
-        <v>61.36237350674613</v>
+        <v>43.8921473549683</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>243</v>
+        <v>271</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>b'3FHL J1500.9+2238 '</t>
+          <t>b'3FHL J1642.9+3948 '</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>225.2482757568359</v>
+        <v>250.7349090576172</v>
       </c>
       <c r="D98" t="n">
-        <v>22.64022445678711</v>
+        <v>39.81490707397461</v>
       </c>
       <c r="E98" t="n">
-        <v>962.8168789726126</v>
+        <v>2218.105585899384</v>
       </c>
       <c r="F98" t="n">
-        <v>31.45102290888001</v>
+        <v>63.46049227208619</v>
       </c>
       <c r="G98" t="n">
-        <v>60.35999634319712</v>
+        <v>40.95690199972307</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>244</v>
+        <v>274</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>b'3FHL J1503.3+4758 '</t>
+          <t>b'3FHL J1652.7+4024 '</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>225.8384399414062</v>
+        <v>253.1941070556641</v>
       </c>
       <c r="D99" t="n">
-        <v>47.97346878051758</v>
+        <v>40.40338897705078</v>
       </c>
       <c r="E99" t="n">
-        <v>1371.891644524125</v>
+        <v>982.1071720326452</v>
       </c>
       <c r="F99" t="n">
-        <v>80.9535755751856</v>
+        <v>64.40155662759337</v>
       </c>
       <c r="G99" t="n">
-        <v>56.98629153475792</v>
+        <v>39.12261782369705</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>245</v>
+        <v>275</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>b'3FHL J1506.0+3732 '</t>
+          <t>b'3FHL J1653.8+3945 '</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>226.5228424072266</v>
+        <v>253.4710998535156</v>
       </c>
       <c r="D100" t="n">
-        <v>37.54251480102539</v>
+        <v>39.75818634033203</v>
       </c>
       <c r="E100" t="n">
-        <v>2465.150914639177</v>
+        <v>141.697084695296</v>
       </c>
       <c r="F100" t="n">
-        <v>61.70862488595789</v>
+        <v>63.59781706285712</v>
       </c>
       <c r="G100" t="n">
-        <v>59.90456332383156</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" s="1" t="n">
-        <v>246</v>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>b'3FHL J1506.7+0813 '</t>
-        </is>
-      </c>
-      <c r="C101" t="n">
-        <v>226.6905822753906</v>
-      </c>
-      <c r="D101" t="n">
-        <v>8.218801498413086</v>
-      </c>
-      <c r="E101" t="n">
-        <v>1487.444413390686</v>
-      </c>
-      <c r="F101" t="n">
-        <v>8.730330769087979</v>
-      </c>
-      <c r="G101" t="n">
-        <v>52.83404159105811</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" s="1" t="n">
-        <v>247</v>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>b'3FHL J1507.2+1722 '</t>
-        </is>
-      </c>
-      <c r="C102" t="n">
-        <v>226.8249816894531</v>
-      </c>
-      <c r="D102" t="n">
-        <v>17.36773490905762</v>
-      </c>
-      <c r="E102" t="n">
-        <v>2129.778114886851</v>
-      </c>
-      <c r="F102" t="n">
-        <v>22.80134452177674</v>
-      </c>
-      <c r="G102" t="n">
-        <v>57.20281900749549</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" s="1" t="n">
-        <v>248</v>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>b'3FHL J1508.7+2708 '</t>
-        </is>
-      </c>
-      <c r="C103" t="n">
-        <v>227.1883544921875</v>
-      </c>
-      <c r="D103" t="n">
-        <v>27.14417457580566</v>
-      </c>
-      <c r="E103" t="n">
-        <v>1096.787424633644</v>
-      </c>
-      <c r="F103" t="n">
-        <v>40.97986187978024</v>
-      </c>
-      <c r="G103" t="n">
-        <v>59.54763194954369</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" s="1" t="n">
-        <v>250</v>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>b'3FHL J1512.2+0203 '</t>
-        </is>
-      </c>
-      <c r="C104" t="n">
-        <v>228.0720062255859</v>
-      </c>
-      <c r="D104" t="n">
-        <v>2.060366868972778</v>
-      </c>
-      <c r="E104" t="n">
-        <v>904.6427903224928</v>
-      </c>
-      <c r="F104" t="n">
-        <v>2.367075362555521</v>
-      </c>
-      <c r="G104" t="n">
-        <v>47.99279308444518</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" s="1" t="n">
-        <v>253</v>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>b'3FHL J1518.5+4044 '</t>
-        </is>
-      </c>
-      <c r="C105" t="n">
-        <v>229.6453247070312</v>
-      </c>
-      <c r="D105" t="n">
-        <v>40.73994827270508</v>
-      </c>
-      <c r="E105" t="n">
-        <v>277.125303444809</v>
-      </c>
-      <c r="F105" t="n">
-        <v>66.76651396705567</v>
-      </c>
-      <c r="G105" t="n">
-        <v>56.89182212745664</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" s="1" t="n">
-        <v>254</v>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>b'3FHL J1531.9+3016 '</t>
-        </is>
-      </c>
-      <c r="C106" t="n">
-        <v>232.9860992431641</v>
-      </c>
-      <c r="D106" t="n">
-        <v>30.27317047119141</v>
-      </c>
-      <c r="E106" t="n">
-        <v>277.125303444809</v>
-      </c>
-      <c r="F106" t="n">
-        <v>47.77962265205297</v>
-      </c>
-      <c r="G106" t="n">
-        <v>54.84301768980958</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" s="1" t="n">
-        <v>255</v>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>b'3FHL J1533.2+1855 '</t>
-        </is>
-      </c>
-      <c r="C107" t="n">
-        <v>233.3144226074219</v>
-      </c>
-      <c r="D107" t="n">
-        <v>18.93068313598633</v>
-      </c>
-      <c r="E107" t="n">
-        <v>1235.720342438146</v>
-      </c>
-      <c r="F107" t="n">
-        <v>29.25278554792897</v>
-      </c>
-      <c r="G107" t="n">
-        <v>52.0464613686915</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" s="1" t="n">
-        <v>256</v>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>b'3FHL J1540.7+1448 '</t>
-        </is>
-      </c>
-      <c r="C108" t="n">
-        <v>235.1949615478516</v>
-      </c>
-      <c r="D108" t="n">
-        <v>14.81568145751953</v>
-      </c>
-      <c r="E108" t="n">
-        <v>2255.902501594245</v>
-      </c>
-      <c r="F108" t="n">
-        <v>24.34762000956751</v>
-      </c>
-      <c r="G108" t="n">
-        <v>48.81774577195303</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" s="1" t="n">
-        <v>258</v>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>b'3FHL J1543.6+0452 '</t>
-        </is>
-      </c>
-      <c r="C109" t="n">
-        <v>235.9000091552734</v>
-      </c>
-      <c r="D109" t="n">
-        <v>4.879972457885742</v>
-      </c>
-      <c r="E109" t="n">
-        <v>171.3237639398314</v>
-      </c>
-      <c r="F109" t="n">
-        <v>12.27756886738662</v>
-      </c>
-      <c r="G109" t="n">
-        <v>43.38510723073886</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" s="1" t="n">
-        <v>260</v>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>b'3FHL J1554.2+2010 '</t>
-        </is>
-      </c>
-      <c r="C110" t="n">
-        <v>238.5714263916016</v>
-      </c>
-      <c r="D110" t="n">
-        <v>20.17705154418945</v>
-      </c>
-      <c r="E110" t="n">
-        <v>912.4256141983458</v>
-      </c>
-      <c r="F110" t="n">
-        <v>33.62416920162958</v>
-      </c>
-      <c r="G110" t="n">
-        <v>47.78168755695976</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" s="1" t="n">
-        <v>261</v>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>b'3FHL J1558.8+5626 '</t>
-        </is>
-      </c>
-      <c r="C111" t="n">
-        <v>239.7223358154297</v>
-      </c>
-      <c r="D111" t="n">
-        <v>56.44340133666992</v>
-      </c>
-      <c r="E111" t="n">
-        <v>1209.647842624998</v>
-      </c>
-      <c r="F111" t="n">
-        <v>87.61477950088891</v>
-      </c>
-      <c r="G111" t="n">
-        <v>45.75468964677962</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" s="1" t="n">
-        <v>263</v>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>b'3FHL J1603.8+1103 '</t>
-        </is>
-      </c>
-      <c r="C112" t="n">
-        <v>240.9507446289062</v>
-      </c>
-      <c r="D112" t="n">
-        <v>11.0573263168335</v>
-      </c>
-      <c r="E112" t="n">
-        <v>598.8824976040644</v>
-      </c>
-      <c r="F112" t="n">
-        <v>22.97464182629868</v>
-      </c>
-      <c r="G112" t="n">
-        <v>42.13516682302727</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" s="1" t="n">
-        <v>264</v>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>b'3FHL J1603.8+5010 '</t>
-        </is>
-      </c>
-      <c r="C113" t="n">
-        <v>240.9585723876953</v>
-      </c>
-      <c r="D113" t="n">
-        <v>50.16685104370117</v>
-      </c>
-      <c r="E113" t="n">
-        <v>2305.888248308498</v>
-      </c>
-      <c r="F113" t="n">
-        <v>78.62070005851318</v>
-      </c>
-      <c r="G113" t="n">
-        <v>46.96057254045356</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" s="1" t="n">
-        <v>265</v>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>b'3FHL J1606.2+5629 '</t>
-        </is>
-      </c>
-      <c r="C114" t="n">
-        <v>241.56298828125</v>
-      </c>
-      <c r="D114" t="n">
-        <v>56.4957389831543</v>
-      </c>
-      <c r="E114" t="n">
-        <v>1746.861857496495</v>
-      </c>
-      <c r="F114" t="n">
-        <v>87.17804013571619</v>
-      </c>
-      <c r="G114" t="n">
-        <v>44.78413662138935</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" s="1" t="n">
-        <v>266</v>
-      </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>b'3FHL J1607.0+1550 '</t>
-        </is>
-      </c>
-      <c r="C115" t="n">
-        <v>241.7560882568359</v>
-      </c>
-      <c r="D115" t="n">
-        <v>15.83572101593018</v>
-      </c>
-      <c r="E115" t="n">
-        <v>1902.710656439457</v>
-      </c>
-      <c r="F115" t="n">
-        <v>29.33763480478526</v>
-      </c>
-      <c r="G115" t="n">
-        <v>43.41828545322375</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" s="1" t="n">
-        <v>267</v>
-      </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>b'3FHL J1615.4+4711 '</t>
-        </is>
-      </c>
-      <c r="C116" t="n">
-        <v>243.8666687011719</v>
-      </c>
-      <c r="D116" t="n">
-        <v>47.19518280029297</v>
-      </c>
-      <c r="E116" t="n">
-        <v>820.9795643094412</v>
-      </c>
-      <c r="F116" t="n">
-        <v>73.86428573709217</v>
-      </c>
-      <c r="G116" t="n">
-        <v>45.64854529020995</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" s="1" t="n">
-        <v>268</v>
-      </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>b'3FHL J1626.2+3515 '</t>
-        </is>
-      </c>
-      <c r="C117" t="n">
-        <v>246.5747680664062</v>
-      </c>
-      <c r="D117" t="n">
-        <v>35.26229095458984</v>
-      </c>
-      <c r="E117" t="n">
-        <v>1907.322882417562</v>
-      </c>
-      <c r="F117" t="n">
-        <v>56.96303155478957</v>
-      </c>
-      <c r="G117" t="n">
-        <v>43.8921473549683</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" s="1" t="n">
-        <v>271</v>
-      </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>b'3FHL J1642.9+3948 '</t>
-        </is>
-      </c>
-      <c r="C118" t="n">
-        <v>250.7349090576172</v>
-      </c>
-      <c r="D118" t="n">
-        <v>39.81490707397461</v>
-      </c>
-      <c r="E118" t="n">
-        <v>2218.105585899384</v>
-      </c>
-      <c r="F118" t="n">
-        <v>63.46049227208619</v>
-      </c>
-      <c r="G118" t="n">
-        <v>40.95690199972307</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" s="1" t="n">
-        <v>273</v>
-      </c>
-      <c r="B119" t="inlineStr">
-        <is>
-          <t>b'3FHL J1647.6+4950 '</t>
-        </is>
-      </c>
-      <c r="C119" t="n">
-        <v>251.9024505615234</v>
-      </c>
-      <c r="D119" t="n">
-        <v>49.84615325927734</v>
-      </c>
-      <c r="E119" t="n">
-        <v>201.1884205905175</v>
-      </c>
-      <c r="F119" t="n">
-        <v>76.66087340567729</v>
-      </c>
-      <c r="G119" t="n">
-        <v>40.07035923704507</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" s="1" t="n">
-        <v>274</v>
-      </c>
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>b'3FHL J1652.7+4024 '</t>
-        </is>
-      </c>
-      <c r="C120" t="n">
-        <v>253.1941070556641</v>
-      </c>
-      <c r="D120" t="n">
-        <v>40.40338897705078</v>
-      </c>
-      <c r="E120" t="n">
-        <v>982.1071720326452</v>
-      </c>
-      <c r="F120" t="n">
-        <v>64.40155662759337</v>
-      </c>
-      <c r="G120" t="n">
-        <v>39.12261782369705</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" s="1" t="n">
-        <v>275</v>
-      </c>
-      <c r="B121" t="inlineStr">
-        <is>
-          <t>b'3FHL J1653.8+3945 '</t>
-        </is>
-      </c>
-      <c r="C121" t="n">
-        <v>253.4710998535156</v>
-      </c>
-      <c r="D121" t="n">
-        <v>39.75818634033203</v>
-      </c>
-      <c r="E121" t="n">
-        <v>141.697084695296</v>
-      </c>
-      <c r="F121" t="n">
-        <v>63.59781706285712</v>
-      </c>
-      <c r="G121" t="n">
         <v>38.85626839795113</v>
       </c>
     </row>

</xml_diff>